<commit_message>
defined CCD_CRUISE_DVM_EVAL_V as a detailed report and CCD_CRUISE_DVM_EVAL_RPT_V as a subset of the CCD_CRUISE_DVM_EVAL_V view
</commit_message>
<xml_diff>
--- a/docs/DB_DDL_helper_template.xlsx
+++ b/docs/DB_DDL_helper_template.xlsx
@@ -737,7 +737,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3257" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3498" uniqueCount="567">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -2415,6 +2415,30 @@
   </si>
   <si>
     <t>CCD_CRUISE_DVM_RULE_EVAL_V</t>
+  </si>
+  <si>
+    <t>DATA_STREAM_DESC</t>
+  </si>
+  <si>
+    <t>DATA_STREAM_ID</t>
+  </si>
+  <si>
+    <t>EVAL_DATE</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_DVM_EVAL_V</t>
+  </si>
+  <si>
+    <t>The description for the given data stream</t>
+  </si>
+  <si>
+    <t>Primary Key for the SPT_DATA_STREAMS table</t>
+  </si>
+  <si>
+    <t>The date/time the given parent record was evaluated using the DVM for the associated data stream</t>
+  </si>
+  <si>
+    <t>This field contains the Standard Survey Name defined for the given cruise. 	If the STD_SVY_NAME_ID field is defined then the associated CCD_STD_SVY_NAMES.STD_SVY_NAME is used because the foreign key is given precedence, otherwise the STD_SVY_NAME_OTH field value is used</t>
   </si>
 </sst>
 </file>
@@ -8300,10 +8324,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2805"/>
+  <dimension ref="A1:D2804"/>
   <sheetViews>
-    <sheetView topLeftCell="A344" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D333" sqref="D333:D379"/>
+    <sheetView topLeftCell="A387" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D404" sqref="D404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13618,41 +13642,746 @@
         <v>COMMENT ON COLUMN CCD_CRUISE_DVM_RULE_EVAL_V.LEG_VESS_NAME_DATES_BR_LIST IS '&lt;BR&gt; tag (intended for web pages) delimited list of leg names, the associated leg dates and vessel name associated with the given cruise';</v>
       </c>
     </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A385" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B385" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="C385" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="D385" s="22" t="str">
+        <f t="shared" ref="D385:D433" si="9">CONCATENATE("COMMENT ON COLUMN ",A385, ".", B385, " IS '", SUBSTITUTE(C385, "'", "''"), "';")</f>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.CRUISE_ID IS 'Primary key for the CCD_CRUISES table';</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A386" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B386" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C386" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="D386" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.CRUISE_NAME IS 'The name of the given cruise designated by NOAA (e.g. SE-15-01)';</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A387" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B387" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C387" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="D387" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.CRUISE_NOTES IS 'Any notes for the given research cruise';</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A388" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B388" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="C388" s="19" t="s">
+        <v>445</v>
+      </c>
+      <c r="D388" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.CRUISE_DESC IS 'Description for the given research cruise';</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A389" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B389" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="C389" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="D389" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.OBJ_BASED_METRICS IS 'Objective Based Metrics for the given research cruise';</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A390" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B390" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C390" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="D390" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.SCI_CENTER_DIV_ID IS 'Primary key for the Science Center Division table';</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A391" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B391" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="C391" s="19" t="s">
+        <v>448</v>
+      </c>
+      <c r="D391" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.SCI_CENTER_DIV_CODE IS 'Abbreviated code for the given Science Center Division';</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A392" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B392" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="C392" s="19" t="s">
+        <v>449</v>
+      </c>
+      <c r="D392" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.SCI_CENTER_DIV_NAME IS 'Name of the given Science Center Division';</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A393" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B393" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="C393" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="D393" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.SCI_CENTER_DIV_DESC IS 'Description for the given Science Center Division';</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A394" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B394" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C394" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="D394" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.SCI_CENTER_ID IS 'Primary key for the Science Center table';</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A395" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B395" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="C395" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="D395" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.SCI_CENTER_NAME IS 'Name of the given Science Center';</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A396" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B396" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="C396" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="D396" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.SCI_CENTER_DESC IS 'Description for the given Science Center';</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A397" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B397" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="C397" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="D397" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.STD_SVY_NAME_ID IS 'Primary key for the Standard Survey Name table';</v>
+      </c>
+    </row>
     <row r="398" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A398" s="19"/>
-      <c r="B398" s="19"/>
-      <c r="C398" s="19"/>
-      <c r="D398" s="22"/>
+      <c r="A398" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B398" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="C398" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="D398" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.STD_SVY_NAME IS 'Name of the given Standard Survey Name';</v>
+      </c>
     </row>
     <row r="399" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A399" s="19"/>
-      <c r="B399" s="19"/>
-      <c r="C399" s="19"/>
-      <c r="D399" s="22"/>
+      <c r="A399" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B399" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="C399" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="D399" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.STD_SVY_DESC IS 'Description for the given Standard Survey Name';</v>
+      </c>
     </row>
     <row r="400" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A400" s="19"/>
-      <c r="B400" s="19"/>
-      <c r="C400" s="19"/>
-      <c r="D400" s="22"/>
+      <c r="A400" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B400" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="C400" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="D400" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.SVY_FREQ_ID IS 'Primary key for the Survey Frequency table';</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A401" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B401" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="C401" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="D401" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.SVY_FREQ_NAME IS 'Name of the given Survey Frequency';</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A402" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B402" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="C402" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="D402" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.SVY_FREQ_DESC IS 'Description for the given Survey Frequency';</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A403" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B403" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C403" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="D403" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.STD_SVY_NAME_OTH IS 'Field defines a Standard Survey Name that is not included in the Standard Survey Name table';</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A404" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B404" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="C404" s="19" t="s">
+        <v>566</v>
+      </c>
+      <c r="D404" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.STD_SVY_NAME_VAL IS 'This field contains the Standard Survey Name defined for the given cruise. 	If the STD_SVY_NAME_ID field is defined then the associated CCD_STD_SVY_NAMES.STD_SVY_NAME is used because the foreign key is given precedence, otherwise the STD_SVY_NAME_OTH field value is used';</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A405" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B405" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="C405" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="D405" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.SVY_TYPE_ID IS 'Primary key for the Survey Type table';</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A406" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B406" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="C406" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="D406" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.SVY_TYPE_NAME IS 'Name of the given Survey Type';</v>
+      </c>
     </row>
     <row r="407" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A407" s="19"/>
-      <c r="B407" s="19"/>
-      <c r="C407" s="19"/>
-      <c r="D407" s="22"/>
+      <c r="A407" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B407" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="C407" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="D407" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.SVY_TYPE_DESC IS 'Description for the given Survey Type';</v>
+      </c>
     </row>
     <row r="408" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A408" s="19"/>
-      <c r="B408" s="19"/>
-      <c r="C408" s="19"/>
-      <c r="D408" s="22"/>
+      <c r="A408" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B408" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="C408" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="D408" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.CRUISE_URL IS 'The Cruise URL (Referred to as "Survey URL" in FINSS System) for the given Cruise';</v>
+      </c>
     </row>
     <row r="409" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A409" s="19"/>
-      <c r="B409" s="19"/>
-      <c r="C409" s="19"/>
-      <c r="D409" s="22"/>
+      <c r="A409" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B409" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="C409" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="D409" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.CRUISE_CONT_EMAIL IS 'The Cruise Contact Email (Referred to as "Survey Contact Email" in FINSS System) for the given Cruise';</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A410" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B410" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="C410" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="D410" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.NUM_LEGS IS 'The number of cruise legs associated with the given cruise';</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A411" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B411" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="C411" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="D411" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.CRUISE_START_DATE IS 'The start date in the corresponding time zone for the given cruise (based on the earliest associated cruise leg''s start date)';</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A412" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B412" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C412" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="D412" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.FORMAT_CRUISE_START_DATE IS 'The formatted start date in the corresponding time zone for the given cruise (based on the earliest associated cruise leg''s start date) in MM/DD/YYYY HH24:MI:SS format';</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A413" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B413" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="C413" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="D413" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.CRUISE_END_DATE IS 'The end date in the corresponding time zone for the given cruise (based on the latest associated cruise leg''s end date)';</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A414" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B414" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="C414" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="D414" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.FORMAT_CRUISE_END_DATE IS 'The formatted end date in the corresponding time zone for the given cruise (based on the latest associated cruise leg''s end date) in MM/DD/YYYY HH24:MI:SS format';</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A415" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B415" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="C415" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="D415" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.CRUISE_DAS IS 'The total number of days at sea for each of the legs associated with the given cruise';</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A416" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B416" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="C416" s="19" t="s">
+        <v>452</v>
+      </c>
+      <c r="D416" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.CRUISE_LEN_DAYS IS 'The total number of days between the Cruise Start and End Dates for the given cruise';</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A417" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B417" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C417" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="D417" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.CRUISE_YEAR IS 'The calendar year for the given cruise (based on the earliest associated cruise leg''s start date)';</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A418" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B418" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="C418" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="D418" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.CRUISE_FISC_YEAR IS 'The calendar year for the given cruise (based on the earliest associated cruise leg''s start date)';</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A419" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B419" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C419" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="D419" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.LEG_NAME_CD_LIST IS 'Comma-delimited list of leg names associated with the given cruise';</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A420" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B420" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C420" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="D420" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.LEG_NAME_SCD_LIST IS 'Semicolon-delimited list of leg names associated with the given cruise';</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A421" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B421" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="C421" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="D421" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.LEG_NAME_RC_LIST IS 'Return carriage/new line delimited list of leg names associated with the given cruise';</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A422" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B422" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="C422" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="D422" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.LEG_NAME_BR_LIST IS '&lt;BR&gt; tag (intended for web pages) delimited list of leg names associated with the given cruise';</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A423" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B423" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="C423" s="19" t="s">
+        <v>554</v>
+      </c>
+      <c r="D423" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.LEG_NAME_DATES_CD_LIST IS 'Comma-delimited list of leg names, the associated leg dates for the given cruise';</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A424" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B424" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="C424" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="D424" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.LEG_NAME_DATES_SCD_LIST IS 'Semicolon-delimited list of leg names, the associated leg dates for the given cruise';</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A425" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B425" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="C425" s="19" t="s">
+        <v>556</v>
+      </c>
+      <c r="D425" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.LEG_NAME_DATES_RC_LIST IS 'Return carriage/new line delimited list of leg names, the associated leg dates for the given cruise';</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A426" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B426" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="C426" s="19" t="s">
+        <v>557</v>
+      </c>
+      <c r="D426" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.LEG_NAME_DATES_BR_LIST IS '&lt;BR&gt; tag (intended for web pages) delimited list of leg names, the associated leg dates for the given cruise';</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A427" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B427" s="18" t="s">
+        <v>495</v>
+      </c>
+      <c r="C427" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="D427" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.LEG_VESS_NAME_DATES_CD_LIST IS 'Comma-delimited list of leg names, the associated leg dates and vessel name associated with the given cruise';</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A428" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B428" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="C428" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="D428" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.LEG_VESS_NAME_DATES_SCD_LIST IS 'Semicolon-delimited list of leg names, the associated leg dates and vessel name associated with the given cruise';</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A429" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B429" s="18" t="s">
+        <v>497</v>
+      </c>
+      <c r="C429" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="D429" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.LEG_VESS_NAME_DATES_RC_LIST IS 'Return carriage/new line delimited list of leg names, the associated leg dates and vessel name associated with the given cruise';</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A430" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B430" s="18" t="s">
+        <v>498</v>
+      </c>
+      <c r="C430" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="D430" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.LEG_VESS_NAME_DATES_BR_LIST IS '&lt;BR&gt; tag (intended for web pages) delimited list of leg names, the associated leg dates and vessel name associated with the given cruise';</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A431" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B431" s="19" t="s">
+        <v>559</v>
+      </c>
+      <c r="C431" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="D431" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.DATA_STREAM_DESC IS 'The description for the given data stream';</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A432" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B432" s="19" t="s">
+        <v>560</v>
+      </c>
+      <c r="C432" s="19" t="s">
+        <v>564</v>
+      </c>
+      <c r="D432" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.DATA_STREAM_ID IS 'Primary Key for the SPT_DATA_STREAMS table';</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A433" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B433" s="19" t="s">
+        <v>561</v>
+      </c>
+      <c r="C433" s="19" t="s">
+        <v>565</v>
+      </c>
+      <c r="D433" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>COMMENT ON COLUMN CCD_CRUISE_DVM_EVAL_V.EVAL_DATE IS 'The date/time the given parent record was evaluated using the DVM for the associated data stream';</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A434" s="19"/>
+      <c r="B434" s="19"/>
+      <c r="C434" s="19"/>
+      <c r="D434" s="22"/>
     </row>
     <row r="435" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A435" s="19"/>
@@ -13666,17 +14395,17 @@
       <c r="C436" s="19"/>
       <c r="D436" s="22"/>
     </row>
-    <row r="437" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A437" s="19"/>
-      <c r="B437" s="19"/>
-      <c r="C437" s="19"/>
-      <c r="D437" s="22"/>
-    </row>
-    <row r="459" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A459" s="19"/>
-      <c r="B459" s="19"/>
-      <c r="C459" s="19"/>
-      <c r="D459" s="22"/>
+    <row r="458" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A458" s="19"/>
+      <c r="B458" s="19"/>
+      <c r="C458" s="19"/>
+      <c r="D458" s="22"/>
+    </row>
+    <row r="463" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A463" s="19"/>
+      <c r="B463" s="19"/>
+      <c r="C463" s="19"/>
+      <c r="D463" s="22"/>
     </row>
     <row r="464" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A464" s="19"/>
@@ -13690,11 +14419,11 @@
       <c r="C465" s="19"/>
       <c r="D465" s="22"/>
     </row>
-    <row r="466" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A466" s="19"/>
-      <c r="B466" s="19"/>
-      <c r="C466" s="19"/>
-      <c r="D466" s="22"/>
+    <row r="472" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A472" s="19"/>
+      <c r="B472" s="19"/>
+      <c r="C472" s="19"/>
+      <c r="D472" s="22"/>
     </row>
     <row r="473" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A473" s="19"/>
@@ -13702,17 +14431,17 @@
       <c r="C473" s="19"/>
       <c r="D473" s="22"/>
     </row>
-    <row r="474" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A474" s="19"/>
       <c r="B474" s="19"/>
       <c r="C474" s="19"/>
       <c r="D474" s="22"/>
     </row>
-    <row r="475" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A475" s="19"/>
-      <c r="B475" s="19"/>
-      <c r="C475" s="19"/>
-      <c r="D475" s="22"/>
+    <row r="509" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A509" s="19"/>
+      <c r="B509" s="19"/>
+      <c r="C509" s="19"/>
+      <c r="D509" s="22"/>
     </row>
     <row r="510" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A510" s="19"/>
@@ -13720,17 +14449,17 @@
       <c r="C510" s="19"/>
       <c r="D510" s="22"/>
     </row>
-    <row r="511" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A511" s="19"/>
       <c r="B511" s="19"/>
       <c r="C511" s="19"/>
       <c r="D511" s="22"/>
     </row>
-    <row r="512" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A512" s="19"/>
-      <c r="B512" s="19"/>
-      <c r="C512" s="19"/>
-      <c r="D512" s="22"/>
+    <row r="547" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A547" s="19"/>
+      <c r="B547" s="19"/>
+      <c r="C547" s="19"/>
+      <c r="D547" s="22"/>
     </row>
     <row r="548" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A548" s="19"/>
@@ -13774,11 +14503,11 @@
       <c r="C554" s="19"/>
       <c r="D554" s="22"/>
     </row>
-    <row r="555" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A555" s="19"/>
-      <c r="B555" s="19"/>
-      <c r="C555" s="19"/>
-      <c r="D555" s="22"/>
+    <row r="559" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A559" s="19"/>
+      <c r="B559" s="19"/>
+      <c r="C559" s="19"/>
+      <c r="D559" s="22"/>
     </row>
     <row r="560" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A560" s="19"/>
@@ -13798,17 +14527,17 @@
       <c r="C562" s="19"/>
       <c r="D562" s="22"/>
     </row>
-    <row r="563" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A563" s="19"/>
-      <c r="B563" s="19"/>
-      <c r="C563" s="19"/>
-      <c r="D563" s="22"/>
-    </row>
-    <row r="565" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A565" s="19"/>
-      <c r="B565" s="19"/>
-      <c r="C565" s="19"/>
-      <c r="D565" s="22"/>
+    <row r="564" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A564" s="19"/>
+      <c r="B564" s="19"/>
+      <c r="C564" s="19"/>
+      <c r="D564" s="22"/>
+    </row>
+    <row r="567" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A567" s="19"/>
+      <c r="B567" s="19"/>
+      <c r="C567" s="19"/>
+      <c r="D567" s="22"/>
     </row>
     <row r="568" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A568" s="19"/>
@@ -13816,13 +14545,13 @@
       <c r="C568" s="19"/>
       <c r="D568" s="22"/>
     </row>
-    <row r="569" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A569" s="19"/>
-      <c r="B569" s="19"/>
-      <c r="C569" s="19"/>
-      <c r="D569" s="22"/>
-    </row>
-    <row r="595" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A594" s="19"/>
+      <c r="B594" s="19"/>
+      <c r="C594" s="19"/>
+      <c r="D594" s="22"/>
+    </row>
+    <row r="595" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A595" s="19"/>
       <c r="B595" s="19"/>
       <c r="C595" s="19"/>
@@ -13834,19 +14563,19 @@
       <c r="C596" s="19"/>
       <c r="D596" s="22"/>
     </row>
-    <row r="597" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A597" s="19"/>
       <c r="B597" s="19"/>
       <c r="C597" s="19"/>
       <c r="D597" s="22"/>
     </row>
-    <row r="598" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A598" s="19"/>
       <c r="B598" s="19"/>
       <c r="C598" s="19"/>
       <c r="D598" s="22"/>
     </row>
-    <row r="599" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="599" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A599" s="19"/>
       <c r="B599" s="19"/>
       <c r="C599" s="19"/>
@@ -13864,7 +14593,7 @@
       <c r="C601" s="19"/>
       <c r="D601" s="22"/>
     </row>
-    <row r="602" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A602" s="19"/>
       <c r="B602" s="19"/>
       <c r="C602" s="19"/>
@@ -13894,7 +14623,7 @@
       <c r="C606" s="19"/>
       <c r="D606" s="22"/>
     </row>
-    <row r="607" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A607" s="19"/>
       <c r="B607" s="19"/>
       <c r="C607" s="19"/>
@@ -13912,7 +14641,7 @@
       <c r="C609" s="19"/>
       <c r="D609" s="22"/>
     </row>
-    <row r="610" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A610" s="19"/>
       <c r="B610" s="19"/>
       <c r="C610" s="19"/>
@@ -14164,41 +14893,41 @@
       <c r="C651" s="19"/>
       <c r="D651" s="22"/>
     </row>
-    <row r="652" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A652" s="19"/>
       <c r="B652" s="19"/>
       <c r="C652" s="19"/>
       <c r="D652" s="22"/>
     </row>
-    <row r="653" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A653" s="19"/>
-      <c r="B653" s="19"/>
-      <c r="C653" s="19"/>
-      <c r="D653" s="22"/>
-    </row>
-    <row r="660" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A660" s="19"/>
-      <c r="B660" s="19"/>
-      <c r="C660" s="19"/>
-      <c r="D660" s="22"/>
-    </row>
-    <row r="672" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A672" s="19"/>
-      <c r="B672" s="19"/>
-      <c r="C672" s="19"/>
-      <c r="D672" s="22"/>
-    </row>
-    <row r="674" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A674" s="19"/>
-      <c r="B674" s="19"/>
-      <c r="C674" s="19"/>
-      <c r="D674" s="22"/>
-    </row>
-    <row r="689" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A689" s="19"/>
-      <c r="B689" s="19"/>
-      <c r="C689" s="19"/>
-      <c r="D689" s="22"/>
+    <row r="659" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A659" s="19"/>
+      <c r="B659" s="19"/>
+      <c r="C659" s="19"/>
+      <c r="D659" s="22"/>
+    </row>
+    <row r="671" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A671" s="19"/>
+      <c r="B671" s="19"/>
+      <c r="C671" s="19"/>
+      <c r="D671" s="22"/>
+    </row>
+    <row r="673" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A673" s="19"/>
+      <c r="B673" s="19"/>
+      <c r="C673" s="19"/>
+      <c r="D673" s="22"/>
+    </row>
+    <row r="688" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A688" s="19"/>
+      <c r="B688" s="19"/>
+      <c r="C688" s="19"/>
+      <c r="D688" s="22"/>
+    </row>
+    <row r="726" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A726" s="19"/>
+      <c r="B726" s="19"/>
+      <c r="C726" s="19"/>
+      <c r="D726" s="22"/>
     </row>
     <row r="727" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A727" s="19"/>
@@ -14218,11 +14947,11 @@
       <c r="C729" s="19"/>
       <c r="D729" s="22"/>
     </row>
-    <row r="730" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A730" s="19"/>
-      <c r="B730" s="19"/>
-      <c r="C730" s="19"/>
-      <c r="D730" s="22"/>
+    <row r="775" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A775" s="19"/>
+      <c r="B775" s="19"/>
+      <c r="C775" s="19"/>
+      <c r="D775" s="22"/>
     </row>
     <row r="776" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A776" s="19"/>
@@ -14236,23 +14965,23 @@
       <c r="C777" s="19"/>
       <c r="D777" s="22"/>
     </row>
-    <row r="778" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A778" s="19"/>
-      <c r="B778" s="19"/>
-      <c r="C778" s="19"/>
-      <c r="D778" s="22"/>
-    </row>
-    <row r="781" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A781" s="19"/>
-      <c r="B781" s="19"/>
-      <c r="C781" s="19"/>
-      <c r="D781" s="22"/>
-    </row>
-    <row r="783" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A783" s="19"/>
-      <c r="B783" s="19"/>
-      <c r="C783" s="19"/>
-      <c r="D783" s="22"/>
+    <row r="780" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A780" s="19"/>
+      <c r="B780" s="19"/>
+      <c r="C780" s="19"/>
+      <c r="D780" s="22"/>
+    </row>
+    <row r="782" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A782" s="19"/>
+      <c r="B782" s="19"/>
+      <c r="C782" s="19"/>
+      <c r="D782" s="22"/>
+    </row>
+    <row r="784" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A784" s="19"/>
+      <c r="B784" s="19"/>
+      <c r="C784" s="19"/>
+      <c r="D784" s="22"/>
     </row>
     <row r="785" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A785" s="19"/>
@@ -14266,23 +14995,23 @@
       <c r="C786" s="19"/>
       <c r="D786" s="22"/>
     </row>
-    <row r="787" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A787" s="19"/>
-      <c r="B787" s="19"/>
-      <c r="C787" s="19"/>
-      <c r="D787" s="22"/>
-    </row>
-    <row r="792" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A792" s="19"/>
-      <c r="B792" s="19"/>
-      <c r="C792" s="19"/>
-      <c r="D792" s="22"/>
-    </row>
-    <row r="794" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A794" s="19"/>
-      <c r="B794" s="19"/>
-      <c r="C794" s="19"/>
-      <c r="D794" s="22"/>
+    <row r="791" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A791" s="19"/>
+      <c r="B791" s="19"/>
+      <c r="C791" s="19"/>
+      <c r="D791" s="22"/>
+    </row>
+    <row r="793" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A793" s="19"/>
+      <c r="B793" s="19"/>
+      <c r="C793" s="19"/>
+      <c r="D793" s="22"/>
+    </row>
+    <row r="795" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A795" s="19"/>
+      <c r="B795" s="19"/>
+      <c r="C795" s="19"/>
+      <c r="D795" s="22"/>
     </row>
     <row r="796" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A796" s="19"/>
@@ -14290,71 +15019,71 @@
       <c r="C796" s="19"/>
       <c r="D796" s="22"/>
     </row>
-    <row r="797" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="797" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A797" s="19"/>
       <c r="B797" s="19"/>
       <c r="C797" s="19"/>
       <c r="D797" s="22"/>
     </row>
-    <row r="798" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A798" s="19"/>
-      <c r="B798" s="19"/>
-      <c r="C798" s="19"/>
-      <c r="D798" s="22"/>
-    </row>
-    <row r="803" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A803" s="19"/>
-      <c r="B803" s="19"/>
-      <c r="C803" s="19"/>
-      <c r="D803" s="22"/>
-    </row>
-    <row r="805" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A805" s="19"/>
-      <c r="B805" s="19"/>
-      <c r="C805" s="19"/>
-      <c r="D805" s="22"/>
-    </row>
-    <row r="807" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="802" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A802" s="19"/>
+      <c r="B802" s="19"/>
+      <c r="C802" s="19"/>
+      <c r="D802" s="22"/>
+    </row>
+    <row r="804" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A804" s="19"/>
+      <c r="B804" s="19"/>
+      <c r="C804" s="19"/>
+      <c r="D804" s="22"/>
+    </row>
+    <row r="806" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A806" s="19"/>
+      <c r="B806" s="19"/>
+      <c r="C806" s="19"/>
+      <c r="D806" s="22"/>
+    </row>
+    <row r="807" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A807" s="19"/>
       <c r="B807" s="19"/>
       <c r="C807" s="19"/>
       <c r="D807" s="22"/>
     </row>
-    <row r="808" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="808" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A808" s="19"/>
       <c r="B808" s="19"/>
       <c r="C808" s="19"/>
       <c r="D808" s="22"/>
     </row>
-    <row r="809" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A809" s="19"/>
-      <c r="B809" s="19"/>
-      <c r="C809" s="19"/>
-      <c r="D809" s="22"/>
-    </row>
-    <row r="815" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A815" s="19"/>
-      <c r="B815" s="19"/>
-      <c r="C815" s="19"/>
-      <c r="D815" s="22"/>
-    </row>
-    <row r="821" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A821" s="19"/>
-      <c r="B821" s="19"/>
-      <c r="C821" s="19"/>
-      <c r="D821" s="22"/>
-    </row>
-    <row r="828" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A828" s="19"/>
-      <c r="B828" s="19"/>
-      <c r="C828" s="19"/>
-      <c r="D828" s="22"/>
-    </row>
-    <row r="830" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A830" s="19"/>
-      <c r="B830" s="19"/>
-      <c r="C830" s="19"/>
-      <c r="D830" s="22"/>
+    <row r="814" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A814" s="19"/>
+      <c r="B814" s="19"/>
+      <c r="C814" s="19"/>
+      <c r="D814" s="22"/>
+    </row>
+    <row r="820" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A820" s="19"/>
+      <c r="B820" s="19"/>
+      <c r="C820" s="19"/>
+      <c r="D820" s="22"/>
+    </row>
+    <row r="827" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A827" s="19"/>
+      <c r="B827" s="19"/>
+      <c r="C827" s="19"/>
+      <c r="D827" s="22"/>
+    </row>
+    <row r="829" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A829" s="19"/>
+      <c r="B829" s="19"/>
+      <c r="C829" s="19"/>
+      <c r="D829" s="22"/>
+    </row>
+    <row r="832" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A832" s="19"/>
+      <c r="B832" s="19"/>
+      <c r="C832" s="19"/>
+      <c r="D832" s="22"/>
     </row>
     <row r="833" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A833" s="19"/>
@@ -14368,7 +15097,7 @@
       <c r="C834" s="19"/>
       <c r="D834" s="22"/>
     </row>
-    <row r="835" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="835" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A835" s="19"/>
       <c r="B835" s="19"/>
       <c r="C835" s="19"/>
@@ -14380,77 +15109,77 @@
       <c r="C836" s="19"/>
       <c r="D836" s="22"/>
     </row>
-    <row r="837" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A837" s="19"/>
-      <c r="B837" s="19"/>
-      <c r="C837" s="19"/>
-      <c r="D837" s="22"/>
-    </row>
-    <row r="840" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A840" s="19"/>
-      <c r="B840" s="19"/>
-      <c r="C840" s="19"/>
-      <c r="D840" s="22"/>
-    </row>
-    <row r="845" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A845" s="19"/>
-      <c r="B845" s="19"/>
-      <c r="C845" s="19"/>
-      <c r="D845" s="22"/>
-    </row>
-    <row r="853" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A853" s="19"/>
-      <c r="B853" s="19"/>
-      <c r="C853" s="19"/>
-      <c r="D853" s="22"/>
-    </row>
-    <row r="856" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A856" s="19"/>
-      <c r="B856" s="19"/>
-      <c r="C856" s="19"/>
-      <c r="D856" s="22"/>
-    </row>
-    <row r="861" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A861" s="19"/>
-      <c r="B861" s="19"/>
-      <c r="C861" s="19"/>
-      <c r="D861" s="22"/>
-    </row>
-    <row r="864" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A864" s="19"/>
-      <c r="B864" s="19"/>
-      <c r="C864" s="19"/>
-      <c r="D864" s="22"/>
-    </row>
-    <row r="870" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A870" s="19"/>
-      <c r="B870" s="19"/>
-      <c r="C870" s="19"/>
-      <c r="D870" s="22"/>
-    </row>
-    <row r="874" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A874" s="19"/>
-      <c r="B874" s="19"/>
-      <c r="C874" s="19"/>
-      <c r="D874" s="22"/>
-    </row>
-    <row r="881" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A881" s="19"/>
-      <c r="B881" s="19"/>
-      <c r="C881" s="19"/>
-      <c r="D881" s="22"/>
-    </row>
-    <row r="883" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A883" s="19"/>
-      <c r="B883" s="19"/>
-      <c r="C883" s="19"/>
-      <c r="D883" s="22"/>
-    </row>
-    <row r="892" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A892" s="19"/>
-      <c r="B892" s="19"/>
-      <c r="C892" s="19"/>
-      <c r="D892" s="22"/>
+    <row r="839" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A839" s="19"/>
+      <c r="B839" s="19"/>
+      <c r="C839" s="19"/>
+      <c r="D839" s="22"/>
+    </row>
+    <row r="844" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A844" s="19"/>
+      <c r="B844" s="19"/>
+      <c r="C844" s="19"/>
+      <c r="D844" s="22"/>
+    </row>
+    <row r="852" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A852" s="19"/>
+      <c r="B852" s="19"/>
+      <c r="C852" s="19"/>
+      <c r="D852" s="22"/>
+    </row>
+    <row r="855" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A855" s="19"/>
+      <c r="B855" s="19"/>
+      <c r="C855" s="19"/>
+      <c r="D855" s="22"/>
+    </row>
+    <row r="860" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A860" s="19"/>
+      <c r="B860" s="19"/>
+      <c r="C860" s="19"/>
+      <c r="D860" s="22"/>
+    </row>
+    <row r="863" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A863" s="19"/>
+      <c r="B863" s="19"/>
+      <c r="C863" s="19"/>
+      <c r="D863" s="22"/>
+    </row>
+    <row r="869" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A869" s="19"/>
+      <c r="B869" s="19"/>
+      <c r="C869" s="19"/>
+      <c r="D869" s="22"/>
+    </row>
+    <row r="873" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A873" s="19"/>
+      <c r="B873" s="19"/>
+      <c r="C873" s="19"/>
+      <c r="D873" s="22"/>
+    </row>
+    <row r="880" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A880" s="19"/>
+      <c r="B880" s="19"/>
+      <c r="C880" s="19"/>
+      <c r="D880" s="22"/>
+    </row>
+    <row r="882" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A882" s="19"/>
+      <c r="B882" s="19"/>
+      <c r="C882" s="19"/>
+      <c r="D882" s="22"/>
+    </row>
+    <row r="891" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A891" s="19"/>
+      <c r="B891" s="19"/>
+      <c r="C891" s="19"/>
+      <c r="D891" s="22"/>
+    </row>
+    <row r="896" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A896" s="19"/>
+      <c r="B896" s="19"/>
+      <c r="C896" s="19"/>
+      <c r="D896" s="22"/>
     </row>
     <row r="897" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A897" s="19"/>
@@ -14458,17 +15187,17 @@
       <c r="C897" s="19"/>
       <c r="D897" s="22"/>
     </row>
-    <row r="898" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A898" s="19"/>
-      <c r="B898" s="19"/>
-      <c r="C898" s="19"/>
-      <c r="D898" s="22"/>
-    </row>
-    <row r="907" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A907" s="19"/>
-      <c r="B907" s="19"/>
-      <c r="C907" s="19"/>
-      <c r="D907" s="22"/>
+    <row r="906" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A906" s="19"/>
+      <c r="B906" s="19"/>
+      <c r="C906" s="19"/>
+      <c r="D906" s="22"/>
+    </row>
+    <row r="908" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A908" s="19"/>
+      <c r="B908" s="19"/>
+      <c r="C908" s="19"/>
+      <c r="D908" s="22"/>
     </row>
     <row r="909" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A909" s="19"/>
@@ -14476,11 +15205,11 @@
       <c r="C909" s="19"/>
       <c r="D909" s="22"/>
     </row>
-    <row r="910" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A910" s="19"/>
-      <c r="B910" s="19"/>
-      <c r="C910" s="19"/>
-      <c r="D910" s="22"/>
+    <row r="911" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A911" s="19"/>
+      <c r="B911" s="19"/>
+      <c r="C911" s="19"/>
+      <c r="D911" s="22"/>
     </row>
     <row r="912" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A912" s="19"/>
@@ -14494,11 +15223,11 @@
       <c r="C913" s="19"/>
       <c r="D913" s="22"/>
     </row>
-    <row r="914" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A914" s="19"/>
-      <c r="B914" s="19"/>
-      <c r="C914" s="19"/>
-      <c r="D914" s="22"/>
+    <row r="918" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A918" s="19"/>
+      <c r="B918" s="19"/>
+      <c r="C918" s="19"/>
+      <c r="D918" s="22"/>
     </row>
     <row r="919" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A919" s="19"/>
@@ -14512,13 +15241,13 @@
       <c r="C920" s="19"/>
       <c r="D920" s="22"/>
     </row>
-    <row r="921" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A921" s="19"/>
-      <c r="B921" s="19"/>
-      <c r="C921" s="19"/>
-      <c r="D921" s="22"/>
-    </row>
-    <row r="924" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="923" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A923" s="19"/>
+      <c r="B923" s="19"/>
+      <c r="C923" s="19"/>
+      <c r="D923" s="22"/>
+    </row>
+    <row r="924" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A924" s="19"/>
       <c r="B924" s="19"/>
       <c r="C924" s="19"/>
@@ -14548,7 +15277,7 @@
       <c r="C928" s="19"/>
       <c r="D928" s="22"/>
     </row>
-    <row r="929" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="929" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A929" s="19"/>
       <c r="B929" s="19"/>
       <c r="C929" s="19"/>
@@ -14566,23 +15295,23 @@
       <c r="C931" s="19"/>
       <c r="D931" s="22"/>
     </row>
-    <row r="932" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="932" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A932" s="19"/>
       <c r="B932" s="19"/>
       <c r="C932" s="19"/>
       <c r="D932" s="22"/>
     </row>
-    <row r="933" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A933" s="19"/>
-      <c r="B933" s="19"/>
-      <c r="C933" s="19"/>
-      <c r="D933" s="22"/>
-    </row>
-    <row r="947" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A947" s="19"/>
-      <c r="B947" s="19"/>
-      <c r="C947" s="19"/>
-      <c r="D947" s="22"/>
+    <row r="946" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A946" s="19"/>
+      <c r="B946" s="19"/>
+      <c r="C946" s="19"/>
+      <c r="D946" s="22"/>
+    </row>
+    <row r="953" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A953" s="19"/>
+      <c r="B953" s="19"/>
+      <c r="C953" s="19"/>
+      <c r="D953" s="22"/>
     </row>
     <row r="954" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A954" s="19"/>
@@ -14590,17 +15319,17 @@
       <c r="C954" s="19"/>
       <c r="D954" s="22"/>
     </row>
-    <row r="955" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A955" s="19"/>
-      <c r="B955" s="19"/>
-      <c r="C955" s="19"/>
-      <c r="D955" s="22"/>
-    </row>
-    <row r="957" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A957" s="19"/>
-      <c r="B957" s="19"/>
-      <c r="C957" s="19"/>
-      <c r="D957" s="22"/>
+    <row r="956" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A956" s="19"/>
+      <c r="B956" s="19"/>
+      <c r="C956" s="19"/>
+      <c r="D956" s="22"/>
+    </row>
+    <row r="962" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A962" s="19"/>
+      <c r="B962" s="19"/>
+      <c r="C962" s="19"/>
+      <c r="D962" s="22"/>
     </row>
     <row r="963" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A963" s="19"/>
@@ -14608,11 +15337,11 @@
       <c r="C963" s="19"/>
       <c r="D963" s="22"/>
     </row>
-    <row r="964" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A964" s="19"/>
-      <c r="B964" s="19"/>
-      <c r="C964" s="19"/>
-      <c r="D964" s="22"/>
+    <row r="969" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A969" s="19"/>
+      <c r="B969" s="19"/>
+      <c r="C969" s="19"/>
+      <c r="D969" s="22"/>
     </row>
     <row r="970" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A970" s="19"/>
@@ -14620,11 +15349,11 @@
       <c r="C970" s="19"/>
       <c r="D970" s="22"/>
     </row>
-    <row r="971" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A971" s="19"/>
-      <c r="B971" s="19"/>
-      <c r="C971" s="19"/>
-      <c r="D971" s="22"/>
+    <row r="980" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A980" s="19"/>
+      <c r="B980" s="19"/>
+      <c r="C980" s="19"/>
+      <c r="D980" s="22"/>
     </row>
     <row r="981" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A981" s="19"/>
@@ -14632,23 +15361,23 @@
       <c r="C981" s="19"/>
       <c r="D981" s="22"/>
     </row>
-    <row r="982" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A982" s="19"/>
-      <c r="B982" s="19"/>
-      <c r="C982" s="19"/>
-      <c r="D982" s="22"/>
-    </row>
-    <row r="992" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A992" s="19"/>
-      <c r="B992" s="19"/>
-      <c r="C992" s="19"/>
-      <c r="D992" s="22"/>
-    </row>
-    <row r="999" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A999" s="19"/>
-      <c r="B999" s="19"/>
-      <c r="C999" s="19"/>
-      <c r="D999" s="22"/>
+    <row r="991" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A991" s="19"/>
+      <c r="B991" s="19"/>
+      <c r="C991" s="19"/>
+      <c r="D991" s="22"/>
+    </row>
+    <row r="998" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A998" s="19"/>
+      <c r="B998" s="19"/>
+      <c r="C998" s="19"/>
+      <c r="D998" s="22"/>
+    </row>
+    <row r="1017" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1017" s="19"/>
+      <c r="B1017" s="19"/>
+      <c r="C1017" s="19"/>
+      <c r="D1017" s="22"/>
     </row>
     <row r="1018" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1018" s="19"/>
@@ -14668,7 +15397,7 @@
       <c r="C1020" s="19"/>
       <c r="D1020" s="22"/>
     </row>
-    <row r="1021" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1021" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1021" s="19"/>
       <c r="B1021" s="19"/>
       <c r="C1021" s="19"/>
@@ -14686,23 +15415,23 @@
       <c r="C1023" s="19"/>
       <c r="D1023" s="22"/>
     </row>
-    <row r="1024" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1024" s="19"/>
-      <c r="B1024" s="19"/>
-      <c r="C1024" s="19"/>
-      <c r="D1024" s="22"/>
-    </row>
-    <row r="1026" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1026" s="19"/>
-      <c r="B1026" s="19"/>
-      <c r="C1026" s="19"/>
-      <c r="D1026" s="22"/>
-    </row>
-    <row r="1039" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1039" s="19"/>
-      <c r="B1039" s="19"/>
-      <c r="C1039" s="19"/>
-      <c r="D1039" s="22"/>
+    <row r="1025" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1025" s="19"/>
+      <c r="B1025" s="19"/>
+      <c r="C1025" s="19"/>
+      <c r="D1025" s="22"/>
+    </row>
+    <row r="1038" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1038" s="19"/>
+      <c r="B1038" s="19"/>
+      <c r="C1038" s="19"/>
+      <c r="D1038" s="22"/>
+    </row>
+    <row r="1045" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1045" s="19"/>
+      <c r="B1045" s="19"/>
+      <c r="C1045" s="19"/>
+      <c r="D1045" s="22"/>
     </row>
     <row r="1046" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1046" s="19"/>
@@ -14710,7 +15439,7 @@
       <c r="C1046" s="19"/>
       <c r="D1046" s="22"/>
     </row>
-    <row r="1047" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1047" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1047" s="19"/>
       <c r="B1047" s="19"/>
       <c r="C1047" s="19"/>
@@ -14728,35 +15457,35 @@
       <c r="C1049" s="19"/>
       <c r="D1049" s="22"/>
     </row>
-    <row r="1050" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1050" s="19"/>
-      <c r="B1050" s="19"/>
-      <c r="C1050" s="19"/>
-      <c r="D1050" s="22"/>
-    </row>
-    <row r="1052" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1052" s="19"/>
-      <c r="B1052" s="19"/>
-      <c r="C1052" s="19"/>
-      <c r="D1052" s="22"/>
-    </row>
-    <row r="1054" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1054" s="19"/>
-      <c r="B1054" s="19"/>
-      <c r="C1054" s="19"/>
-      <c r="D1054" s="22"/>
-    </row>
-    <row r="1061" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1061" s="19"/>
-      <c r="B1061" s="19"/>
-      <c r="C1061" s="19"/>
-      <c r="D1061" s="22"/>
-    </row>
-    <row r="1066" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1066" s="19"/>
-      <c r="B1066" s="19"/>
-      <c r="C1066" s="19"/>
-      <c r="D1066" s="22"/>
+    <row r="1051" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1051" s="19"/>
+      <c r="B1051" s="19"/>
+      <c r="C1051" s="19"/>
+      <c r="D1051" s="22"/>
+    </row>
+    <row r="1053" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1053" s="19"/>
+      <c r="B1053" s="19"/>
+      <c r="C1053" s="19"/>
+      <c r="D1053" s="22"/>
+    </row>
+    <row r="1060" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1060" s="19"/>
+      <c r="B1060" s="19"/>
+      <c r="C1060" s="19"/>
+      <c r="D1060" s="22"/>
+    </row>
+    <row r="1065" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1065" s="19"/>
+      <c r="B1065" s="19"/>
+      <c r="C1065" s="19"/>
+      <c r="D1065" s="22"/>
+    </row>
+    <row r="1067" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1067" s="19"/>
+      <c r="B1067" s="19"/>
+      <c r="C1067" s="19"/>
+      <c r="D1067" s="22"/>
     </row>
     <row r="1068" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1068" s="19"/>
@@ -14770,11 +15499,11 @@
       <c r="C1069" s="19"/>
       <c r="D1069" s="22"/>
     </row>
-    <row r="1070" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1070" s="19"/>
-      <c r="B1070" s="19"/>
-      <c r="C1070" s="19"/>
-      <c r="D1070" s="22"/>
+    <row r="1072" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1072" s="19"/>
+      <c r="B1072" s="19"/>
+      <c r="C1072" s="19"/>
+      <c r="D1072" s="22"/>
     </row>
     <row r="1073" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1073" s="19"/>
@@ -14782,7 +15511,7 @@
       <c r="C1073" s="19"/>
       <c r="D1073" s="22"/>
     </row>
-    <row r="1074" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1074" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1074" s="19"/>
       <c r="B1074" s="19"/>
       <c r="C1074" s="19"/>
@@ -14818,7 +15547,7 @@
       <c r="C1079" s="19"/>
       <c r="D1079" s="22"/>
     </row>
-    <row r="1080" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1080" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1080" s="19"/>
       <c r="B1080" s="19"/>
       <c r="C1080" s="19"/>
@@ -14986,13 +15715,13 @@
       <c r="C1107" s="19"/>
       <c r="D1107" s="22"/>
     </row>
-    <row r="1108" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1108" s="19"/>
-      <c r="B1108" s="19"/>
-      <c r="C1108" s="19"/>
-      <c r="D1108" s="22"/>
-    </row>
-    <row r="1126" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1125" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1125" s="19"/>
+      <c r="B1125" s="19"/>
+      <c r="C1125" s="19"/>
+      <c r="D1125" s="22"/>
+    </row>
+    <row r="1126" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1126" s="19"/>
       <c r="B1126" s="19"/>
       <c r="C1126" s="19"/>
@@ -15022,37 +15751,37 @@
       <c r="C1130" s="19"/>
       <c r="D1130" s="22"/>
     </row>
-    <row r="1131" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1131" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1131" s="19"/>
       <c r="B1131" s="19"/>
       <c r="C1131" s="19"/>
       <c r="D1131" s="22"/>
     </row>
-    <row r="1132" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1132" s="19"/>
-      <c r="B1132" s="19"/>
-      <c r="C1132" s="19"/>
-      <c r="D1132" s="22"/>
-    </row>
-    <row r="1150" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1150" s="19"/>
-      <c r="B1150" s="19"/>
-      <c r="C1150" s="19"/>
-      <c r="D1150" s="22"/>
-    </row>
-    <row r="1152" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1152" s="19"/>
-      <c r="B1152" s="19"/>
-      <c r="C1152" s="19"/>
-      <c r="D1152" s="22"/>
-    </row>
-    <row r="1156" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1149" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1149" s="19"/>
+      <c r="B1149" s="19"/>
+      <c r="C1149" s="19"/>
+      <c r="D1149" s="22"/>
+    </row>
+    <row r="1151" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1151" s="19"/>
+      <c r="B1151" s="19"/>
+      <c r="C1151" s="19"/>
+      <c r="D1151" s="22"/>
+    </row>
+    <row r="1155" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1155" s="19"/>
+      <c r="B1155" s="19"/>
+      <c r="C1155" s="19"/>
+      <c r="D1155" s="22"/>
+    </row>
+    <row r="1156" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1156" s="19"/>
       <c r="B1156" s="19"/>
       <c r="C1156" s="19"/>
       <c r="D1156" s="22"/>
     </row>
-    <row r="1157" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1157" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1157" s="19"/>
       <c r="B1157" s="19"/>
       <c r="C1157" s="19"/>
@@ -15064,7 +15793,7 @@
       <c r="C1158" s="19"/>
       <c r="D1158" s="22"/>
     </row>
-    <row r="1159" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1159" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1159" s="19"/>
       <c r="B1159" s="19"/>
       <c r="C1159" s="19"/>
@@ -15190,11 +15919,11 @@
       <c r="C1179" s="19"/>
       <c r="D1179" s="22"/>
     </row>
-    <row r="1180" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1180" s="19"/>
-      <c r="B1180" s="19"/>
-      <c r="C1180" s="19"/>
-      <c r="D1180" s="22"/>
+    <row r="1189" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1189" s="19"/>
+      <c r="B1189" s="19"/>
+      <c r="C1189" s="19"/>
+      <c r="D1189" s="22"/>
     </row>
     <row r="1190" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1190" s="19"/>
@@ -15220,29 +15949,29 @@
       <c r="C1193" s="19"/>
       <c r="D1193" s="22"/>
     </row>
-    <row r="1194" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1194" s="19"/>
-      <c r="B1194" s="19"/>
-      <c r="C1194" s="19"/>
-      <c r="D1194" s="22"/>
-    </row>
-    <row r="1230" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1230" s="19"/>
-      <c r="B1230" s="19"/>
-      <c r="C1230" s="19"/>
-      <c r="D1230" s="22"/>
-    </row>
-    <row r="1243" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1243" s="19"/>
-      <c r="B1243" s="19"/>
-      <c r="C1243" s="19"/>
-      <c r="D1243" s="22"/>
-    </row>
-    <row r="1246" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1246" s="19"/>
-      <c r="B1246" s="19"/>
-      <c r="C1246" s="19"/>
-      <c r="D1246" s="22"/>
+    <row r="1229" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1229" s="19"/>
+      <c r="B1229" s="19"/>
+      <c r="C1229" s="19"/>
+      <c r="D1229" s="22"/>
+    </row>
+    <row r="1242" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1242" s="19"/>
+      <c r="B1242" s="19"/>
+      <c r="C1242" s="19"/>
+      <c r="D1242" s="22"/>
+    </row>
+    <row r="1245" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1245" s="19"/>
+      <c r="B1245" s="19"/>
+      <c r="C1245" s="19"/>
+      <c r="D1245" s="22"/>
+    </row>
+    <row r="1266" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1266" s="19"/>
+      <c r="B1266" s="19"/>
+      <c r="C1266" s="19"/>
+      <c r="D1266" s="22"/>
     </row>
     <row r="1267" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1267" s="19"/>
@@ -15268,11 +15997,11 @@
       <c r="C1270" s="19"/>
       <c r="D1270" s="22"/>
     </row>
-    <row r="1271" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1271" s="19"/>
-      <c r="B1271" s="19"/>
-      <c r="C1271" s="19"/>
-      <c r="D1271" s="22"/>
+    <row r="1292" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1292" s="19"/>
+      <c r="B1292" s="19"/>
+      <c r="C1292" s="19"/>
+      <c r="D1292" s="22"/>
     </row>
     <row r="1293" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1293" s="19"/>
@@ -15418,11 +16147,11 @@
       <c r="C1316" s="19"/>
       <c r="D1316" s="22"/>
     </row>
-    <row r="1317" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1317" s="19"/>
-      <c r="B1317" s="19"/>
-      <c r="C1317" s="19"/>
-      <c r="D1317" s="22"/>
+    <row r="1322" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1322" s="19"/>
+      <c r="B1322" s="19"/>
+      <c r="C1322" s="19"/>
+      <c r="D1322" s="22"/>
     </row>
     <row r="1323" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1323" s="19"/>
@@ -15430,11 +16159,11 @@
       <c r="C1323" s="19"/>
       <c r="D1323" s="22"/>
     </row>
-    <row r="1324" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1324" s="19"/>
-      <c r="B1324" s="19"/>
-      <c r="C1324" s="19"/>
-      <c r="D1324" s="22"/>
+    <row r="1338" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1338" s="19"/>
+      <c r="B1338" s="19"/>
+      <c r="C1338" s="19"/>
+      <c r="D1338" s="22"/>
     </row>
     <row r="1339" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1339" s="19"/>
@@ -15442,11 +16171,11 @@
       <c r="C1339" s="19"/>
       <c r="D1339" s="22"/>
     </row>
-    <row r="1340" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1340" s="19"/>
-      <c r="B1340" s="19"/>
-      <c r="C1340" s="19"/>
-      <c r="D1340" s="22"/>
+    <row r="1345" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1345" s="19"/>
+      <c r="B1345" s="19"/>
+      <c r="C1345" s="19"/>
+      <c r="D1345" s="22"/>
     </row>
     <row r="1346" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1346" s="19"/>
@@ -15478,47 +16207,47 @@
       <c r="C1350" s="19"/>
       <c r="D1350" s="22"/>
     </row>
-    <row r="1351" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1351" s="19"/>
-      <c r="B1351" s="19"/>
-      <c r="C1351" s="19"/>
-      <c r="D1351" s="22"/>
-    </row>
-    <row r="1357" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1356" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1356" s="19"/>
+      <c r="B1356" s="19"/>
+      <c r="C1356" s="19"/>
+      <c r="D1356" s="22"/>
+    </row>
+    <row r="1357" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1357" s="19"/>
       <c r="B1357" s="19"/>
       <c r="C1357" s="19"/>
       <c r="D1357" s="22"/>
     </row>
-    <row r="1358" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1358" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1358" s="19"/>
       <c r="B1358" s="19"/>
       <c r="C1358" s="19"/>
       <c r="D1358" s="22"/>
     </row>
-    <row r="1359" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1359" s="19"/>
-      <c r="B1359" s="19"/>
-      <c r="C1359" s="19"/>
-      <c r="D1359" s="22"/>
-    </row>
-    <row r="1363" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1362" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1362" s="19"/>
+      <c r="B1362" s="19"/>
+      <c r="C1362" s="19"/>
+      <c r="D1362" s="22"/>
+    </row>
+    <row r="1363" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1363" s="19"/>
       <c r="B1363" s="19"/>
       <c r="C1363" s="19"/>
       <c r="D1363" s="22"/>
     </row>
-    <row r="1364" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1364" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1364" s="19"/>
       <c r="B1364" s="19"/>
       <c r="C1364" s="19"/>
       <c r="D1364" s="22"/>
     </row>
-    <row r="1365" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1365" s="19"/>
-      <c r="B1365" s="19"/>
-      <c r="C1365" s="19"/>
-      <c r="D1365" s="22"/>
+    <row r="1370" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1370" s="19"/>
+      <c r="B1370" s="19"/>
+      <c r="C1370" s="19"/>
+      <c r="D1370" s="22"/>
     </row>
     <row r="1371" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1371" s="19"/>
@@ -15526,23 +16255,23 @@
       <c r="C1371" s="19"/>
       <c r="D1371" s="22"/>
     </row>
-    <row r="1372" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1372" s="19"/>
-      <c r="B1372" s="19"/>
-      <c r="C1372" s="19"/>
-      <c r="D1372" s="22"/>
-    </row>
-    <row r="1383" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1383" s="19"/>
-      <c r="B1383" s="19"/>
-      <c r="C1383" s="19"/>
-      <c r="D1383" s="22"/>
-    </row>
-    <row r="1450" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1450" s="19"/>
-      <c r="B1450" s="19"/>
-      <c r="C1450" s="19"/>
-      <c r="D1450" s="22"/>
+    <row r="1382" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1382" s="19"/>
+      <c r="B1382" s="19"/>
+      <c r="C1382" s="19"/>
+      <c r="D1382" s="22"/>
+    </row>
+    <row r="1449" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1449" s="19"/>
+      <c r="B1449" s="19"/>
+      <c r="C1449" s="19"/>
+      <c r="D1449" s="22"/>
+    </row>
+    <row r="1605" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1605" s="19"/>
+      <c r="B1605" s="19"/>
+      <c r="C1605" s="19"/>
+      <c r="D1605" s="22"/>
     </row>
     <row r="1606" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1606" s="19"/>
@@ -15550,37 +16279,37 @@
       <c r="C1606" s="19"/>
       <c r="D1606" s="22"/>
     </row>
-    <row r="1607" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1607" s="19"/>
-      <c r="B1607" s="19"/>
-      <c r="C1607" s="19"/>
-      <c r="D1607" s="22"/>
-    </row>
-    <row r="1653" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1653" s="19"/>
-      <c r="B1653" s="19"/>
-      <c r="C1653" s="19"/>
-      <c r="D1653" s="22"/>
-    </row>
-    <row r="1656" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1656" s="19"/>
-      <c r="B1656" s="19"/>
-      <c r="C1656" s="19"/>
-      <c r="D1656" s="22"/>
-    </row>
-    <row r="1662" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1662" s="19"/>
-      <c r="B1662" s="19"/>
-      <c r="C1662" s="19"/>
-      <c r="D1662" s="22"/>
-    </row>
-    <row r="1664" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1652" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1652" s="19"/>
+      <c r="B1652" s="19"/>
+      <c r="C1652" s="19"/>
+      <c r="D1652" s="22"/>
+    </row>
+    <row r="1655" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1655" s="19"/>
+      <c r="B1655" s="19"/>
+      <c r="C1655" s="19"/>
+      <c r="D1655" s="22"/>
+    </row>
+    <row r="1661" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1661" s="19"/>
+      <c r="B1661" s="19"/>
+      <c r="C1661" s="19"/>
+      <c r="D1661" s="22"/>
+    </row>
+    <row r="1663" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1663" s="19"/>
+      <c r="B1663" s="19"/>
+      <c r="C1663" s="19"/>
+      <c r="D1663" s="22"/>
+    </row>
+    <row r="1664" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1664" s="19"/>
       <c r="B1664" s="19"/>
       <c r="C1664" s="19"/>
       <c r="D1664" s="22"/>
     </row>
-    <row r="1665" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1665" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1665" s="19"/>
       <c r="B1665" s="19"/>
       <c r="C1665" s="19"/>
@@ -15592,23 +16321,23 @@
       <c r="C1666" s="19"/>
       <c r="D1666" s="22"/>
     </row>
-    <row r="1667" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1667" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1667" s="19"/>
       <c r="B1667" s="19"/>
       <c r="C1667" s="19"/>
       <c r="D1667" s="22"/>
     </row>
-    <row r="1668" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1668" s="19"/>
-      <c r="B1668" s="19"/>
-      <c r="C1668" s="19"/>
-      <c r="D1668" s="22"/>
-    </row>
-    <row r="1679" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1679" s="19"/>
-      <c r="B1679" s="19"/>
-      <c r="C1679" s="19"/>
-      <c r="D1679" s="22"/>
+    <row r="1678" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1678" s="19"/>
+      <c r="B1678" s="19"/>
+      <c r="C1678" s="19"/>
+      <c r="D1678" s="22"/>
+    </row>
+    <row r="1680" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1680" s="19"/>
+      <c r="B1680" s="19"/>
+      <c r="C1680" s="19"/>
+      <c r="D1680" s="22"/>
     </row>
     <row r="1681" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1681" s="19"/>
@@ -15760,11 +16489,11 @@
       <c r="C1705" s="19"/>
       <c r="D1705" s="22"/>
     </row>
-    <row r="1706" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1706" s="19"/>
-      <c r="B1706" s="19"/>
-      <c r="C1706" s="19"/>
-      <c r="D1706" s="22"/>
+    <row r="1764" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1764" s="19"/>
+      <c r="B1764" s="19"/>
+      <c r="C1764" s="19"/>
+      <c r="D1764" s="22"/>
     </row>
     <row r="1765" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1765" s="19"/>
@@ -15772,17 +16501,17 @@
       <c r="C1765" s="19"/>
       <c r="D1765" s="22"/>
     </row>
-    <row r="1766" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1766" s="19"/>
-      <c r="B1766" s="19"/>
-      <c r="C1766" s="19"/>
-      <c r="D1766" s="22"/>
-    </row>
-    <row r="2094" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2094" s="19"/>
-      <c r="B2094" s="19"/>
-      <c r="C2094" s="19"/>
-      <c r="D2094" s="22"/>
+    <row r="2093" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2093" s="19"/>
+      <c r="B2093" s="19"/>
+      <c r="C2093" s="19"/>
+      <c r="D2093" s="22"/>
+    </row>
+    <row r="2237" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2237" s="19"/>
+      <c r="B2237" s="19"/>
+      <c r="C2237" s="19"/>
+      <c r="D2237" s="22"/>
     </row>
     <row r="2238" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2238" s="19"/>
@@ -15880,47 +16609,47 @@
       <c r="C2253" s="19"/>
       <c r="D2253" s="22"/>
     </row>
-    <row r="2254" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2254" s="19"/>
-      <c r="B2254" s="19"/>
-      <c r="C2254" s="19"/>
-      <c r="D2254" s="22"/>
-    </row>
-    <row r="2261" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2261" s="19"/>
-      <c r="B2261" s="19"/>
-      <c r="C2261" s="19"/>
-      <c r="D2261" s="22"/>
-    </row>
-    <row r="2422" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2260" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2260" s="19"/>
+      <c r="B2260" s="19"/>
+      <c r="C2260" s="19"/>
+      <c r="D2260" s="22"/>
+    </row>
+    <row r="2421" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2421" s="19"/>
+      <c r="B2421" s="19"/>
+      <c r="C2421" s="19"/>
+      <c r="D2421" s="22"/>
+    </row>
+    <row r="2422" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2422" s="19"/>
       <c r="B2422" s="19"/>
       <c r="C2422" s="19"/>
       <c r="D2422" s="22"/>
     </row>
-    <row r="2423" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2423" s="19"/>
-      <c r="B2423" s="19"/>
-      <c r="C2423" s="19"/>
-      <c r="D2423" s="22"/>
-    </row>
-    <row r="2428" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2428" s="19"/>
-      <c r="B2428" s="19"/>
-      <c r="C2428" s="19"/>
-      <c r="D2428" s="22"/>
-    </row>
-    <row r="2522" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2522" s="19"/>
-      <c r="B2522" s="19"/>
-      <c r="C2522" s="19"/>
-      <c r="D2522" s="22"/>
-    </row>
-    <row r="2547" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2547" s="19"/>
-      <c r="B2547" s="19"/>
-      <c r="C2547" s="19"/>
-      <c r="D2547" s="22"/>
+    <row r="2427" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2427" s="19"/>
+      <c r="B2427" s="19"/>
+      <c r="C2427" s="19"/>
+      <c r="D2427" s="22"/>
+    </row>
+    <row r="2521" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2521" s="19"/>
+      <c r="B2521" s="19"/>
+      <c r="C2521" s="19"/>
+      <c r="D2521" s="22"/>
+    </row>
+    <row r="2546" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2546" s="19"/>
+      <c r="B2546" s="19"/>
+      <c r="C2546" s="19"/>
+      <c r="D2546" s="22"/>
+    </row>
+    <row r="2548" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2548" s="19"/>
+      <c r="B2548" s="19"/>
+      <c r="C2548" s="19"/>
+      <c r="D2548" s="22"/>
     </row>
     <row r="2549" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2549" s="19"/>
@@ -15928,11 +16657,11 @@
       <c r="C2549" s="19"/>
       <c r="D2549" s="22"/>
     </row>
-    <row r="2550" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2550" s="19"/>
-      <c r="B2550" s="19"/>
-      <c r="C2550" s="19"/>
-      <c r="D2550" s="22"/>
+    <row r="2551" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2551" s="19"/>
+      <c r="B2551" s="19"/>
+      <c r="C2551" s="19"/>
+      <c r="D2551" s="22"/>
     </row>
     <row r="2552" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2552" s="19"/>
@@ -15940,11 +16669,11 @@
       <c r="C2552" s="19"/>
       <c r="D2552" s="22"/>
     </row>
-    <row r="2553" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2553" s="19"/>
-      <c r="B2553" s="19"/>
-      <c r="C2553" s="19"/>
-      <c r="D2553" s="22"/>
+    <row r="2558" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2558" s="19"/>
+      <c r="B2558" s="19"/>
+      <c r="C2558" s="19"/>
+      <c r="D2558" s="22"/>
     </row>
     <row r="2559" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2559" s="19"/>
@@ -15970,17 +16699,17 @@
       <c r="C2562" s="19"/>
       <c r="D2562" s="22"/>
     </row>
-    <row r="2563" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2563" s="19"/>
-      <c r="B2563" s="19"/>
-      <c r="C2563" s="19"/>
-      <c r="D2563" s="22"/>
-    </row>
-    <row r="2572" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2572" s="19"/>
-      <c r="B2572" s="19"/>
-      <c r="C2572" s="19"/>
-      <c r="D2572" s="22"/>
+    <row r="2571" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2571" s="19"/>
+      <c r="B2571" s="19"/>
+      <c r="C2571" s="19"/>
+      <c r="D2571" s="22"/>
+    </row>
+    <row r="2573" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2573" s="19"/>
+      <c r="B2573" s="19"/>
+      <c r="C2573" s="19"/>
+      <c r="D2573" s="22"/>
     </row>
     <row r="2574" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2574" s="19"/>
@@ -15988,11 +16717,11 @@
       <c r="C2574" s="19"/>
       <c r="D2574" s="22"/>
     </row>
-    <row r="2575" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2575" s="19"/>
-      <c r="B2575" s="19"/>
-      <c r="C2575" s="19"/>
-      <c r="D2575" s="22"/>
+    <row r="2576" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2576" s="19"/>
+      <c r="B2576" s="19"/>
+      <c r="C2576" s="19"/>
+      <c r="D2576" s="22"/>
     </row>
     <row r="2577" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2577" s="19"/>
@@ -16000,11 +16729,11 @@
       <c r="C2577" s="19"/>
       <c r="D2577" s="22"/>
     </row>
-    <row r="2578" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2578" s="19"/>
-      <c r="B2578" s="19"/>
-      <c r="C2578" s="19"/>
-      <c r="D2578" s="22"/>
+    <row r="2583" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2583" s="19"/>
+      <c r="B2583" s="19"/>
+      <c r="C2583" s="19"/>
+      <c r="D2583" s="22"/>
     </row>
     <row r="2584" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2584" s="19"/>
@@ -16030,11 +16759,11 @@
       <c r="C2587" s="19"/>
       <c r="D2587" s="22"/>
     </row>
-    <row r="2588" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2588" s="19"/>
-      <c r="B2588" s="19"/>
-      <c r="C2588" s="19"/>
-      <c r="D2588" s="22"/>
+    <row r="2589" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2589" s="19"/>
+      <c r="B2589" s="19"/>
+      <c r="C2589" s="19"/>
+      <c r="D2589" s="22"/>
     </row>
     <row r="2590" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2590" s="19"/>
@@ -16048,11 +16777,11 @@
       <c r="C2591" s="19"/>
       <c r="D2591" s="22"/>
     </row>
-    <row r="2592" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2592" s="19"/>
-      <c r="B2592" s="19"/>
-      <c r="C2592" s="19"/>
-      <c r="D2592" s="22"/>
+    <row r="2606" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2606" s="19"/>
+      <c r="B2606" s="19"/>
+      <c r="C2606" s="19"/>
+      <c r="D2606" s="22"/>
     </row>
     <row r="2607" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2607" s="19"/>
@@ -16324,17 +17053,17 @@
       <c r="C2651" s="19"/>
       <c r="D2651" s="22"/>
     </row>
-    <row r="2652" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2652" s="19"/>
-      <c r="B2652" s="19"/>
-      <c r="C2652" s="19"/>
-      <c r="D2652" s="22"/>
-    </row>
-    <row r="2675" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2675" s="19"/>
-      <c r="B2675" s="19"/>
-      <c r="C2675" s="19"/>
-      <c r="D2675" s="22"/>
+    <row r="2674" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2674" s="19"/>
+      <c r="B2674" s="19"/>
+      <c r="C2674" s="19"/>
+      <c r="D2674" s="22"/>
+    </row>
+    <row r="2684" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2684" s="19"/>
+      <c r="B2684" s="19"/>
+      <c r="C2684" s="19"/>
+      <c r="D2684" s="22"/>
     </row>
     <row r="2685" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2685" s="19"/>
@@ -16342,17 +17071,17 @@
       <c r="C2685" s="19"/>
       <c r="D2685" s="22"/>
     </row>
-    <row r="2686" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2686" s="19"/>
-      <c r="B2686" s="19"/>
-      <c r="C2686" s="19"/>
-      <c r="D2686" s="22"/>
-    </row>
-    <row r="2691" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2691" s="19"/>
-      <c r="B2691" s="19"/>
-      <c r="C2691" s="19"/>
-      <c r="D2691" s="22"/>
+    <row r="2690" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2690" s="19"/>
+      <c r="B2690" s="19"/>
+      <c r="C2690" s="19"/>
+      <c r="D2690" s="22"/>
+    </row>
+    <row r="2700" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2700" s="19"/>
+      <c r="B2700" s="19"/>
+      <c r="C2700" s="19"/>
+      <c r="D2700" s="22"/>
     </row>
     <row r="2701" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2701" s="19"/>
@@ -16360,17 +17089,17 @@
       <c r="C2701" s="19"/>
       <c r="D2701" s="22"/>
     </row>
-    <row r="2702" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2702" s="19"/>
-      <c r="B2702" s="19"/>
-      <c r="C2702" s="19"/>
-      <c r="D2702" s="22"/>
-    </row>
-    <row r="2707" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2707" s="19"/>
-      <c r="B2707" s="19"/>
-      <c r="C2707" s="19"/>
-      <c r="D2707" s="22"/>
+    <row r="2706" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2706" s="19"/>
+      <c r="B2706" s="19"/>
+      <c r="C2706" s="19"/>
+      <c r="D2706" s="22"/>
+    </row>
+    <row r="2716" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2716" s="19"/>
+      <c r="B2716" s="19"/>
+      <c r="C2716" s="19"/>
+      <c r="D2716" s="22"/>
     </row>
     <row r="2717" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2717" s="19"/>
@@ -16378,35 +17107,29 @@
       <c r="C2717" s="19"/>
       <c r="D2717" s="22"/>
     </row>
-    <row r="2718" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2718" s="19"/>
-      <c r="B2718" s="19"/>
-      <c r="C2718" s="19"/>
-      <c r="D2718" s="22"/>
-    </row>
-    <row r="2737" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2737" s="19"/>
-      <c r="B2737" s="19"/>
-      <c r="C2737" s="19"/>
-      <c r="D2737" s="22"/>
-    </row>
-    <row r="2754" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2754" s="19"/>
-      <c r="B2754" s="19"/>
-      <c r="C2754" s="19"/>
-      <c r="D2754" s="22"/>
-    </row>
-    <row r="2779" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2779" s="19"/>
-      <c r="B2779" s="19"/>
-      <c r="C2779" s="19"/>
-      <c r="D2779" s="22"/>
-    </row>
-    <row r="2805" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2805" s="19"/>
-      <c r="B2805" s="19"/>
-      <c r="C2805" s="19"/>
-      <c r="D2805" s="22"/>
+    <row r="2736" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2736" s="19"/>
+      <c r="B2736" s="19"/>
+      <c r="C2736" s="19"/>
+      <c r="D2736" s="22"/>
+    </row>
+    <row r="2753" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2753" s="19"/>
+      <c r="B2753" s="19"/>
+      <c r="C2753" s="19"/>
+      <c r="D2753" s="22"/>
+    </row>
+    <row r="2778" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2778" s="19"/>
+      <c r="B2778" s="19"/>
+      <c r="C2778" s="19"/>
+      <c r="D2778" s="22"/>
+    </row>
+    <row r="2804" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2804" s="19"/>
+      <c r="B2804" s="19"/>
+      <c r="C2804" s="19"/>
+      <c r="D2804" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16535,10 +17258,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1129"/>
+  <dimension ref="A1:C1183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1073" workbookViewId="0">
-      <selection activeCell="C1021" sqref="C1021:C1129"/>
+    <sheetView tabSelected="1" topLeftCell="A1131" workbookViewId="0">
+      <selection activeCell="B1183" sqref="A1137:B1183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29173,6 +29896,570 @@
       <c r="C1129" s="18" t="str">
         <f t="shared" si="22"/>
         <v xml:space="preserve">CCD_CRUISE_LEG_DATA_SETS_V.STATUS_COLOR, </v>
+      </c>
+    </row>
+    <row r="1137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1137" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1137" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1137" s="18" t="str">
+        <f t="shared" ref="C1137:C1183" si="23">CONCATENATE(A1137, ".", B1137, ", ")</f>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.CRUISE_ID, </v>
+      </c>
+    </row>
+    <row r="1138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1138" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1138" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1138" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.CRUISE_NAME, </v>
+      </c>
+    </row>
+    <row r="1139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1139" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1139" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1139" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.CRUISE_NOTES, </v>
+      </c>
+    </row>
+    <row r="1140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1140" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1140" t="s">
+        <v>408</v>
+      </c>
+      <c r="C1140" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.CRUISE_DESC, </v>
+      </c>
+    </row>
+    <row r="1141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1141" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1141" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1141" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.OBJ_BASED_METRICS, </v>
+      </c>
+    </row>
+    <row r="1142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1142" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1142" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1142" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.SCI_CENTER_DIV_ID, </v>
+      </c>
+    </row>
+    <row r="1143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1143" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1143" t="s">
+        <v>410</v>
+      </c>
+      <c r="C1143" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.SCI_CENTER_DIV_CODE, </v>
+      </c>
+    </row>
+    <row r="1144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1144" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1144" t="s">
+        <v>411</v>
+      </c>
+      <c r="C1144" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.SCI_CENTER_DIV_NAME, </v>
+      </c>
+    </row>
+    <row r="1145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1145" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1145" t="s">
+        <v>412</v>
+      </c>
+      <c r="C1145" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.SCI_CENTER_DIV_DESC, </v>
+      </c>
+    </row>
+    <row r="1146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1146" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1146" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1146" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.SCI_CENTER_ID, </v>
+      </c>
+    </row>
+    <row r="1147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1147" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1147" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1147" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.SCI_CENTER_NAME, </v>
+      </c>
+    </row>
+    <row r="1148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1148" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1148" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1148" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.SCI_CENTER_DESC, </v>
+      </c>
+    </row>
+    <row r="1149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1149" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1149" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1149" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.STD_SVY_NAME_ID, </v>
+      </c>
+    </row>
+    <row r="1150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1150" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1150" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1150" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.STD_SVY_NAME, </v>
+      </c>
+    </row>
+    <row r="1151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1151" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1151" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1151" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.STD_SVY_DESC, </v>
+      </c>
+    </row>
+    <row r="1152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1152" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1152" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1152" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.SVY_FREQ_ID, </v>
+      </c>
+    </row>
+    <row r="1153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1153" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1153" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1153" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.SVY_FREQ_NAME, </v>
+      </c>
+    </row>
+    <row r="1154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1154" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1154" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1154" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.SVY_FREQ_DESC, </v>
+      </c>
+    </row>
+    <row r="1155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1155" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1155" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1155" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.STD_SVY_NAME_OTH, </v>
+      </c>
+    </row>
+    <row r="1156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1156" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1156" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1156" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.STD_SVY_NAME_VAL, </v>
+      </c>
+    </row>
+    <row r="1157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1157" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1157" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1157" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.SVY_TYPE_ID, </v>
+      </c>
+    </row>
+    <row r="1158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1158" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1158" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1158" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.SVY_TYPE_NAME, </v>
+      </c>
+    </row>
+    <row r="1159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1159" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1159" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1159" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.SVY_TYPE_DESC, </v>
+      </c>
+    </row>
+    <row r="1160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1160" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1160" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1160" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.CRUISE_URL, </v>
+      </c>
+    </row>
+    <row r="1161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1161" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1161" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1161" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.CRUISE_CONT_EMAIL, </v>
+      </c>
+    </row>
+    <row r="1162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1162" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1162" t="s">
+        <v>413</v>
+      </c>
+      <c r="C1162" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.PTA_ISS_ID, </v>
+      </c>
+    </row>
+    <row r="1163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1163" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1163" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1163" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.NUM_LEGS, </v>
+      </c>
+    </row>
+    <row r="1164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1164" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1164" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1164" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.CRUISE_START_DATE, </v>
+      </c>
+    </row>
+    <row r="1165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1165" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1165" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1165" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.FORMAT_CRUISE_START_DATE, </v>
+      </c>
+    </row>
+    <row r="1166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1166" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1166" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1166" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.CRUISE_END_DATE, </v>
+      </c>
+    </row>
+    <row r="1167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1167" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1167" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1167" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.FORMAT_CRUISE_END_DATE, </v>
+      </c>
+    </row>
+    <row r="1168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1168" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1168" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1168" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.CRUISE_DAS, </v>
+      </c>
+    </row>
+    <row r="1169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1169" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1169" t="s">
+        <v>414</v>
+      </c>
+      <c r="C1169" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.CRUISE_LEN_DAYS, </v>
+      </c>
+    </row>
+    <row r="1170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1170" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1170" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1170" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.CRUISE_YEAR, </v>
+      </c>
+    </row>
+    <row r="1171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1171" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1171" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1171" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.CRUISE_FISC_YEAR, </v>
+      </c>
+    </row>
+    <row r="1172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1172" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1172" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1172" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.LEG_NAME_CD_LIST, </v>
+      </c>
+    </row>
+    <row r="1173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1173" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1173" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1173" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.LEG_NAME_SCD_LIST, </v>
+      </c>
+    </row>
+    <row r="1174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1174" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1174" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1174" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.LEG_NAME_RC_LIST, </v>
+      </c>
+    </row>
+    <row r="1175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1175" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1175" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1175" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.LEG_NAME_BR_LIST, </v>
+      </c>
+    </row>
+    <row r="1176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1176" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1176" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1176" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.LEG_NAME_DATES_CD_LIST, </v>
+      </c>
+    </row>
+    <row r="1177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1177" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1177" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1177" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.LEG_NAME_DATES_SCD_LIST, </v>
+      </c>
+    </row>
+    <row r="1178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1178" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1178" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1178" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.LEG_NAME_DATES_RC_LIST, </v>
+      </c>
+    </row>
+    <row r="1179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1179" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1179" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1179" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.LEG_NAME_DATES_BR_LIST, </v>
+      </c>
+    </row>
+    <row r="1180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1180" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1180" t="s">
+        <v>495</v>
+      </c>
+      <c r="C1180" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.LEG_VESS_NAME_DATES_CD_LIST, </v>
+      </c>
+    </row>
+    <row r="1181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1181" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1181" t="s">
+        <v>496</v>
+      </c>
+      <c r="C1181" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.LEG_VESS_NAME_DATES_SCD_LIST, </v>
+      </c>
+    </row>
+    <row r="1182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1182" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1182" t="s">
+        <v>497</v>
+      </c>
+      <c r="C1182" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.LEG_VESS_NAME_DATES_RC_LIST, </v>
+      </c>
+    </row>
+    <row r="1183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1183" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1183" t="s">
+        <v>498</v>
+      </c>
+      <c r="C1183" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v xml:space="preserve">CCD_CRUISE_AGG_V.LEG_VESS_NAME_DATES_BR_LIST, </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resolved DB deployment errors
</commit_message>
<xml_diff>
--- a/docs/DB_DDL_helper_template.xlsx
+++ b/docs/DB_DDL_helper_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19080" windowHeight="6855" tabRatio="759" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19080" windowHeight="6855" tabRatio="759" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CORE DDL" sheetId="1" r:id="rId1"/>
@@ -737,7 +737,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3498" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3710" uniqueCount="569">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -2439,6 +2439,12 @@
   </si>
   <si>
     <t>This field contains the Standard Survey Name defined for the given cruise. 	If the STD_SVY_NAME_ID field is defined then the associated CCD_STD_SVY_NAMES.STD_SVY_NAME is used because the foreign key is given precedence, otherwise the STD_SVY_NAME_OTH field value is used</t>
+  </si>
+  <si>
+    <t>ccd_cruise_leg_v</t>
+  </si>
+  <si>
+    <t>This field contains the Standard Survey Name defined for the given cruise.	If the STD_SVY_NAME_ID field is defined then the associated CCD_STD_SVY_NAMES.STD_SVY_NAME is used because the foreign key is given precedence, otherwise the STD_SVY_NAME_OTH field value is used</t>
   </si>
 </sst>
 </file>
@@ -8324,10 +8330,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2804"/>
+  <dimension ref="A1:D2803"/>
   <sheetViews>
-    <sheetView topLeftCell="A387" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D404" sqref="D404"/>
+    <sheetView tabSelected="1" topLeftCell="A446" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C487" sqref="C487"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14395,47 +14401,641 @@
       <c r="C436" s="19"/>
       <c r="D436" s="22"/>
     </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A446" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B446" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="C446" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="D446" s="22" t="str">
+        <f t="shared" ref="D446:D487" si="10">CONCATENATE("COMMENT ON COLUMN ",A446, ".", B446, " IS '", SUBSTITUTE(C446, "'", "''"), "';")</f>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.CRUISE_ID IS 'Primary key for the CCD_CRUISES table';</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A447" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B447" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C447" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="D447" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.CRUISE_NAME IS 'The name of the given cruise designated by NOAA (e.g. SE-15-01)';</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A448" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B448" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C448" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="D448" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.CRUISE_NOTES IS 'Any notes for the given research cruise';</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A449" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B449" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="C449" s="19" t="s">
+        <v>445</v>
+      </c>
+      <c r="D449" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.CRUISE_DESC IS 'Description for the given research cruise';</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A450" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B450" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="C450" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="D450" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.OBJ_BASED_METRICS IS 'Objective Based Metrics for the given research cruise';</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A451" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B451" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C451" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="D451" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.SCI_CENTER_DIV_ID IS 'Primary key for the Science Center Division table';</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A452" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B452" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="C452" s="19" t="s">
+        <v>448</v>
+      </c>
+      <c r="D452" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.SCI_CENTER_DIV_CODE IS 'Abbreviated code for the given Science Center Division';</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A453" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B453" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="C453" s="19" t="s">
+        <v>449</v>
+      </c>
+      <c r="D453" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.SCI_CENTER_DIV_NAME IS 'Name of the given Science Center Division';</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A454" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B454" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="C454" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="D454" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.SCI_CENTER_DIV_DESC IS 'Description for the given Science Center Division';</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A455" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B455" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C455" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="D455" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.SCI_CENTER_ID IS 'Primary key for the Science Center table';</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A456" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B456" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="C456" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="D456" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.SCI_CENTER_NAME IS 'Name of the given Science Center';</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A457" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B457" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="C457" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="D457" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.SCI_CENTER_DESC IS 'Description for the given Science Center';</v>
+      </c>
+    </row>
     <row r="458" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A458" s="19"/>
-      <c r="B458" s="19"/>
-      <c r="C458" s="19"/>
-      <c r="D458" s="22"/>
+      <c r="A458" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B458" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="C458" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="D458" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.STD_SVY_NAME_ID IS 'Primary key for the Standard Survey Name table';</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A459" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B459" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="C459" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="D459" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.STD_SVY_NAME IS 'Name of the given Standard Survey Name';</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A460" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B460" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="C460" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="D460" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.STD_SVY_DESC IS 'Description for the given Standard Survey Name';</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A461" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B461" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="C461" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="D461" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.SVY_FREQ_ID IS 'Primary key for the Survey Frequency table';</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A462" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B462" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="C462" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="D462" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.SVY_FREQ_NAME IS 'Name of the given Survey Frequency';</v>
+      </c>
     </row>
     <row r="463" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A463" s="19"/>
-      <c r="B463" s="19"/>
-      <c r="C463" s="19"/>
-      <c r="D463" s="22"/>
+      <c r="A463" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B463" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="C463" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="D463" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.SVY_FREQ_DESC IS 'Description for the given Survey Frequency';</v>
+      </c>
     </row>
     <row r="464" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A464" s="19"/>
-      <c r="B464" s="19"/>
-      <c r="C464" s="19"/>
-      <c r="D464" s="22"/>
+      <c r="A464" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B464" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C464" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="D464" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.STD_SVY_NAME_OTH IS 'Field defines a Standard Survey Name that is not included in the Standard Survey Name table';</v>
+      </c>
     </row>
     <row r="465" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A465" s="19"/>
-      <c r="B465" s="19"/>
-      <c r="C465" s="19"/>
-      <c r="D465" s="22"/>
+      <c r="A465" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B465" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="C465" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="D465" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.STD_SVY_NAME_VAL IS 'This field contains the Standard Survey Name defined for the given cruise.	If the STD_SVY_NAME_ID field is defined then the associated CCD_STD_SVY_NAMES.STD_SVY_NAME is used because the foreign key is given precedence, otherwise the STD_SVY_NAME_OTH field value is used';</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A466" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B466" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="C466" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="D466" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.SVY_TYPE_ID IS 'Primary key for the Survey Type table';</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A467" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B467" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="C467" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="D467" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.SVY_TYPE_NAME IS 'Name of the given Survey Type';</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A468" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B468" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="C468" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="D468" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.SVY_TYPE_DESC IS 'Description for the given Survey Type';</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A469" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B469" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="C469" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="D469" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.CRUISE_URL IS 'The Cruise URL (Referred to as "Survey URL" in FINSS System) for the given Cruise';</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A470" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B470" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="C470" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="D470" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.CRUISE_CONT_EMAIL IS 'The Cruise Contact Email (Referred to as "Survey Contact Email" in FINSS System) for the given Cruise';</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A471" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B471" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="C471" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="D471" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.PTA_ISS_ID IS 'Foreign key reference to the Issues (PTA) intersection table';</v>
+      </c>
     </row>
     <row r="472" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A472" s="19"/>
-      <c r="B472" s="19"/>
-      <c r="C472" s="19"/>
-      <c r="D472" s="22"/>
-    </row>
-    <row r="473" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A473" s="19"/>
-      <c r="B473" s="19"/>
-      <c r="C473" s="19"/>
-      <c r="D473" s="22"/>
-    </row>
-    <row r="474" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A474" s="19"/>
-      <c r="B474" s="19"/>
-      <c r="C474" s="19"/>
-      <c r="D474" s="22"/>
+      <c r="A472" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B472" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C472" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="D472" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.LEG_NAME IS 'The name of the given cruise leg';</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A473" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B473" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="C473" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="D473" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.LEG_START_DATE IS 'The start date in the corresponding time zone for the given research cruise leg';</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A474" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B474" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C474" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="D474" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.FORMAT_LEG_START_DATE IS 'The start date in the corresponding time zone for the given research cruise leg in MM/DD/YYYY format';</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A475" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B475" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="C475" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="D475" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.LEG_END_DATE IS 'The end date in the corresponding time zone for the given research cruise leg';</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A476" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B476" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="C476" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="D476" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.FORMAT_LEG_END_DATE IS 'The end date in the corresponding time zone for the given research cruise leg in MM/DD/YYYY format';</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A477" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B477" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="C477" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="D477" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.LEG_DAS IS 'The number of days at sea for the given research cruise leg';</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A478" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B478" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="C478" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="D478" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.LEG_YEAR IS 'The calendar year for the start date of the given research cruise leg';</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A479" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B479" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="C479" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="D479" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.TZ_NAME IS 'The numeric offset for UTC or Time Zone Name (V$TIMEZONE_NAMES.TZNAME) for the local timezone where the cruise leg occurred (e.g. US/Hawaii, US/Samoa, Etc/GMT+9)';</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A480" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B480" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="C480" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="D480" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.LEG_FISC_YEAR IS 'The NOAA fiscal year for the start date of the given research cruise leg';</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A481" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B481" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="C481" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="D481" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.LEG_DESC IS 'The description for the given research cruise leg';</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A482" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B482" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="C482" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="D482" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.VESSEL_ID IS 'Foreign key reference to the CCD_VESSELS table for the cruise leg''s vessel';</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A483" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B483" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="C483" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="D483" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.VESSEL_NAME IS 'Name of the given research vessel';</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A484" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B484" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="C484" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="D484" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.VESSEL_DESC IS 'Description for the given research vessel';</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A485" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B485" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C485" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="D485" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.PLAT_TYPE_ID IS 'Platform Type for the given research cruise leg';</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A486" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B486" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="C486" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="D486" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.PLAT_TYPE_NAME IS 'Name of the given Platform Type';</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A487" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B487" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="C487" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="D487" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.PLAT_TYPE_DESC IS 'Description for the given Platform Type';</v>
+      </c>
+    </row>
+    <row r="508" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A508" s="19"/>
+      <c r="B508" s="19"/>
+      <c r="C508" s="19"/>
+      <c r="D508" s="22"/>
     </row>
     <row r="509" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A509" s="19"/>
@@ -14443,17 +15043,17 @@
       <c r="C509" s="19"/>
       <c r="D509" s="22"/>
     </row>
-    <row r="510" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A510" s="19"/>
       <c r="B510" s="19"/>
       <c r="C510" s="19"/>
       <c r="D510" s="22"/>
     </row>
-    <row r="511" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A511" s="19"/>
-      <c r="B511" s="19"/>
-      <c r="C511" s="19"/>
-      <c r="D511" s="22"/>
+    <row r="546" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A546" s="19"/>
+      <c r="B546" s="19"/>
+      <c r="C546" s="19"/>
+      <c r="D546" s="22"/>
     </row>
     <row r="547" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A547" s="19"/>
@@ -14497,11 +15097,11 @@
       <c r="C553" s="19"/>
       <c r="D553" s="22"/>
     </row>
-    <row r="554" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A554" s="19"/>
-      <c r="B554" s="19"/>
-      <c r="C554" s="19"/>
-      <c r="D554" s="22"/>
+    <row r="558" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A558" s="19"/>
+      <c r="B558" s="19"/>
+      <c r="C558" s="19"/>
+      <c r="D558" s="22"/>
     </row>
     <row r="559" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A559" s="19"/>
@@ -14521,17 +15121,17 @@
       <c r="C561" s="19"/>
       <c r="D561" s="22"/>
     </row>
-    <row r="562" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A562" s="19"/>
-      <c r="B562" s="19"/>
-      <c r="C562" s="19"/>
-      <c r="D562" s="22"/>
-    </row>
-    <row r="564" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A564" s="19"/>
-      <c r="B564" s="19"/>
-      <c r="C564" s="19"/>
-      <c r="D564" s="22"/>
+    <row r="563" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A563" s="19"/>
+      <c r="B563" s="19"/>
+      <c r="C563" s="19"/>
+      <c r="D563" s="22"/>
+    </row>
+    <row r="566" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A566" s="19"/>
+      <c r="B566" s="19"/>
+      <c r="C566" s="19"/>
+      <c r="D566" s="22"/>
     </row>
     <row r="567" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A567" s="19"/>
@@ -14539,13 +15139,13 @@
       <c r="C567" s="19"/>
       <c r="D567" s="22"/>
     </row>
-    <row r="568" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A568" s="19"/>
-      <c r="B568" s="19"/>
-      <c r="C568" s="19"/>
-      <c r="D568" s="22"/>
-    </row>
-    <row r="594" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A593" s="19"/>
+      <c r="B593" s="19"/>
+      <c r="C593" s="19"/>
+      <c r="D593" s="22"/>
+    </row>
+    <row r="594" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A594" s="19"/>
       <c r="B594" s="19"/>
       <c r="C594" s="19"/>
@@ -14557,19 +15157,19 @@
       <c r="C595" s="19"/>
       <c r="D595" s="22"/>
     </row>
-    <row r="596" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A596" s="19"/>
       <c r="B596" s="19"/>
       <c r="C596" s="19"/>
       <c r="D596" s="22"/>
     </row>
-    <row r="597" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A597" s="19"/>
       <c r="B597" s="19"/>
       <c r="C597" s="19"/>
       <c r="D597" s="22"/>
     </row>
-    <row r="598" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A598" s="19"/>
       <c r="B598" s="19"/>
       <c r="C598" s="19"/>
@@ -14587,7 +15187,7 @@
       <c r="C600" s="19"/>
       <c r="D600" s="22"/>
     </row>
-    <row r="601" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="601" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A601" s="19"/>
       <c r="B601" s="19"/>
       <c r="C601" s="19"/>
@@ -14617,7 +15217,7 @@
       <c r="C605" s="19"/>
       <c r="D605" s="22"/>
     </row>
-    <row r="606" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A606" s="19"/>
       <c r="B606" s="19"/>
       <c r="C606" s="19"/>
@@ -14635,7 +15235,7 @@
       <c r="C608" s="19"/>
       <c r="D608" s="22"/>
     </row>
-    <row r="609" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A609" s="19"/>
       <c r="B609" s="19"/>
       <c r="C609" s="19"/>
@@ -14887,41 +15487,41 @@
       <c r="C650" s="19"/>
       <c r="D650" s="22"/>
     </row>
-    <row r="651" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="651" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A651" s="19"/>
       <c r="B651" s="19"/>
       <c r="C651" s="19"/>
       <c r="D651" s="22"/>
     </row>
-    <row r="652" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A652" s="19"/>
-      <c r="B652" s="19"/>
-      <c r="C652" s="19"/>
-      <c r="D652" s="22"/>
-    </row>
-    <row r="659" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A659" s="19"/>
-      <c r="B659" s="19"/>
-      <c r="C659" s="19"/>
-      <c r="D659" s="22"/>
-    </row>
-    <row r="671" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A671" s="19"/>
-      <c r="B671" s="19"/>
-      <c r="C671" s="19"/>
-      <c r="D671" s="22"/>
-    </row>
-    <row r="673" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A673" s="19"/>
-      <c r="B673" s="19"/>
-      <c r="C673" s="19"/>
-      <c r="D673" s="22"/>
-    </row>
-    <row r="688" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A688" s="19"/>
-      <c r="B688" s="19"/>
-      <c r="C688" s="19"/>
-      <c r="D688" s="22"/>
+    <row r="658" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A658" s="19"/>
+      <c r="B658" s="19"/>
+      <c r="C658" s="19"/>
+      <c r="D658" s="22"/>
+    </row>
+    <row r="670" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A670" s="19"/>
+      <c r="B670" s="19"/>
+      <c r="C670" s="19"/>
+      <c r="D670" s="22"/>
+    </row>
+    <row r="672" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A672" s="19"/>
+      <c r="B672" s="19"/>
+      <c r="C672" s="19"/>
+      <c r="D672" s="22"/>
+    </row>
+    <row r="687" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A687" s="19"/>
+      <c r="B687" s="19"/>
+      <c r="C687" s="19"/>
+      <c r="D687" s="22"/>
+    </row>
+    <row r="725" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A725" s="19"/>
+      <c r="B725" s="19"/>
+      <c r="C725" s="19"/>
+      <c r="D725" s="22"/>
     </row>
     <row r="726" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A726" s="19"/>
@@ -14941,11 +15541,11 @@
       <c r="C728" s="19"/>
       <c r="D728" s="22"/>
     </row>
-    <row r="729" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A729" s="19"/>
-      <c r="B729" s="19"/>
-      <c r="C729" s="19"/>
-      <c r="D729" s="22"/>
+    <row r="774" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A774" s="19"/>
+      <c r="B774" s="19"/>
+      <c r="C774" s="19"/>
+      <c r="D774" s="22"/>
     </row>
     <row r="775" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A775" s="19"/>
@@ -14959,23 +15559,23 @@
       <c r="C776" s="19"/>
       <c r="D776" s="22"/>
     </row>
-    <row r="777" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A777" s="19"/>
-      <c r="B777" s="19"/>
-      <c r="C777" s="19"/>
-      <c r="D777" s="22"/>
-    </row>
-    <row r="780" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A780" s="19"/>
-      <c r="B780" s="19"/>
-      <c r="C780" s="19"/>
-      <c r="D780" s="22"/>
-    </row>
-    <row r="782" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A782" s="19"/>
-      <c r="B782" s="19"/>
-      <c r="C782" s="19"/>
-      <c r="D782" s="22"/>
+    <row r="779" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A779" s="19"/>
+      <c r="B779" s="19"/>
+      <c r="C779" s="19"/>
+      <c r="D779" s="22"/>
+    </row>
+    <row r="781" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A781" s="19"/>
+      <c r="B781" s="19"/>
+      <c r="C781" s="19"/>
+      <c r="D781" s="22"/>
+    </row>
+    <row r="783" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A783" s="19"/>
+      <c r="B783" s="19"/>
+      <c r="C783" s="19"/>
+      <c r="D783" s="22"/>
     </row>
     <row r="784" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A784" s="19"/>
@@ -14989,23 +15589,23 @@
       <c r="C785" s="19"/>
       <c r="D785" s="22"/>
     </row>
-    <row r="786" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A786" s="19"/>
-      <c r="B786" s="19"/>
-      <c r="C786" s="19"/>
-      <c r="D786" s="22"/>
-    </row>
-    <row r="791" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A791" s="19"/>
-      <c r="B791" s="19"/>
-      <c r="C791" s="19"/>
-      <c r="D791" s="22"/>
-    </row>
-    <row r="793" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A793" s="19"/>
-      <c r="B793" s="19"/>
-      <c r="C793" s="19"/>
-      <c r="D793" s="22"/>
+    <row r="790" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A790" s="19"/>
+      <c r="B790" s="19"/>
+      <c r="C790" s="19"/>
+      <c r="D790" s="22"/>
+    </row>
+    <row r="792" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A792" s="19"/>
+      <c r="B792" s="19"/>
+      <c r="C792" s="19"/>
+      <c r="D792" s="22"/>
+    </row>
+    <row r="794" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A794" s="19"/>
+      <c r="B794" s="19"/>
+      <c r="C794" s="19"/>
+      <c r="D794" s="22"/>
     </row>
     <row r="795" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A795" s="19"/>
@@ -15013,71 +15613,71 @@
       <c r="C795" s="19"/>
       <c r="D795" s="22"/>
     </row>
-    <row r="796" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="796" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A796" s="19"/>
       <c r="B796" s="19"/>
       <c r="C796" s="19"/>
       <c r="D796" s="22"/>
     </row>
-    <row r="797" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A797" s="19"/>
-      <c r="B797" s="19"/>
-      <c r="C797" s="19"/>
-      <c r="D797" s="22"/>
-    </row>
-    <row r="802" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A802" s="19"/>
-      <c r="B802" s="19"/>
-      <c r="C802" s="19"/>
-      <c r="D802" s="22"/>
-    </row>
-    <row r="804" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A804" s="19"/>
-      <c r="B804" s="19"/>
-      <c r="C804" s="19"/>
-      <c r="D804" s="22"/>
-    </row>
-    <row r="806" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="801" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A801" s="19"/>
+      <c r="B801" s="19"/>
+      <c r="C801" s="19"/>
+      <c r="D801" s="22"/>
+    </row>
+    <row r="803" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A803" s="19"/>
+      <c r="B803" s="19"/>
+      <c r="C803" s="19"/>
+      <c r="D803" s="22"/>
+    </row>
+    <row r="805" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A805" s="19"/>
+      <c r="B805" s="19"/>
+      <c r="C805" s="19"/>
+      <c r="D805" s="22"/>
+    </row>
+    <row r="806" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A806" s="19"/>
       <c r="B806" s="19"/>
       <c r="C806" s="19"/>
       <c r="D806" s="22"/>
     </row>
-    <row r="807" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="807" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A807" s="19"/>
       <c r="B807" s="19"/>
       <c r="C807" s="19"/>
       <c r="D807" s="22"/>
     </row>
-    <row r="808" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A808" s="19"/>
-      <c r="B808" s="19"/>
-      <c r="C808" s="19"/>
-      <c r="D808" s="22"/>
-    </row>
-    <row r="814" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A814" s="19"/>
-      <c r="B814" s="19"/>
-      <c r="C814" s="19"/>
-      <c r="D814" s="22"/>
-    </row>
-    <row r="820" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A820" s="19"/>
-      <c r="B820" s="19"/>
-      <c r="C820" s="19"/>
-      <c r="D820" s="22"/>
-    </row>
-    <row r="827" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A827" s="19"/>
-      <c r="B827" s="19"/>
-      <c r="C827" s="19"/>
-      <c r="D827" s="22"/>
-    </row>
-    <row r="829" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A829" s="19"/>
-      <c r="B829" s="19"/>
-      <c r="C829" s="19"/>
-      <c r="D829" s="22"/>
+    <row r="813" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A813" s="19"/>
+      <c r="B813" s="19"/>
+      <c r="C813" s="19"/>
+      <c r="D813" s="22"/>
+    </row>
+    <row r="819" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A819" s="19"/>
+      <c r="B819" s="19"/>
+      <c r="C819" s="19"/>
+      <c r="D819" s="22"/>
+    </row>
+    <row r="826" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A826" s="19"/>
+      <c r="B826" s="19"/>
+      <c r="C826" s="19"/>
+      <c r="D826" s="22"/>
+    </row>
+    <row r="828" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A828" s="19"/>
+      <c r="B828" s="19"/>
+      <c r="C828" s="19"/>
+      <c r="D828" s="22"/>
+    </row>
+    <row r="831" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A831" s="19"/>
+      <c r="B831" s="19"/>
+      <c r="C831" s="19"/>
+      <c r="D831" s="22"/>
     </row>
     <row r="832" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A832" s="19"/>
@@ -15091,7 +15691,7 @@
       <c r="C833" s="19"/>
       <c r="D833" s="22"/>
     </row>
-    <row r="834" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="834" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A834" s="19"/>
       <c r="B834" s="19"/>
       <c r="C834" s="19"/>
@@ -15103,77 +15703,77 @@
       <c r="C835" s="19"/>
       <c r="D835" s="22"/>
     </row>
-    <row r="836" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A836" s="19"/>
-      <c r="B836" s="19"/>
-      <c r="C836" s="19"/>
-      <c r="D836" s="22"/>
-    </row>
-    <row r="839" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A839" s="19"/>
-      <c r="B839" s="19"/>
-      <c r="C839" s="19"/>
-      <c r="D839" s="22"/>
-    </row>
-    <row r="844" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A844" s="19"/>
-      <c r="B844" s="19"/>
-      <c r="C844" s="19"/>
-      <c r="D844" s="22"/>
-    </row>
-    <row r="852" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A852" s="19"/>
-      <c r="B852" s="19"/>
-      <c r="C852" s="19"/>
-      <c r="D852" s="22"/>
-    </row>
-    <row r="855" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A855" s="19"/>
-      <c r="B855" s="19"/>
-      <c r="C855" s="19"/>
-      <c r="D855" s="22"/>
-    </row>
-    <row r="860" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A860" s="19"/>
-      <c r="B860" s="19"/>
-      <c r="C860" s="19"/>
-      <c r="D860" s="22"/>
-    </row>
-    <row r="863" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A863" s="19"/>
-      <c r="B863" s="19"/>
-      <c r="C863" s="19"/>
-      <c r="D863" s="22"/>
-    </row>
-    <row r="869" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A869" s="19"/>
-      <c r="B869" s="19"/>
-      <c r="C869" s="19"/>
-      <c r="D869" s="22"/>
-    </row>
-    <row r="873" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A873" s="19"/>
-      <c r="B873" s="19"/>
-      <c r="C873" s="19"/>
-      <c r="D873" s="22"/>
-    </row>
-    <row r="880" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A880" s="19"/>
-      <c r="B880" s="19"/>
-      <c r="C880" s="19"/>
-      <c r="D880" s="22"/>
-    </row>
-    <row r="882" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A882" s="19"/>
-      <c r="B882" s="19"/>
-      <c r="C882" s="19"/>
-      <c r="D882" s="22"/>
-    </row>
-    <row r="891" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A891" s="19"/>
-      <c r="B891" s="19"/>
-      <c r="C891" s="19"/>
-      <c r="D891" s="22"/>
+    <row r="838" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A838" s="19"/>
+      <c r="B838" s="19"/>
+      <c r="C838" s="19"/>
+      <c r="D838" s="22"/>
+    </row>
+    <row r="843" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A843" s="19"/>
+      <c r="B843" s="19"/>
+      <c r="C843" s="19"/>
+      <c r="D843" s="22"/>
+    </row>
+    <row r="851" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A851" s="19"/>
+      <c r="B851" s="19"/>
+      <c r="C851" s="19"/>
+      <c r="D851" s="22"/>
+    </row>
+    <row r="854" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A854" s="19"/>
+      <c r="B854" s="19"/>
+      <c r="C854" s="19"/>
+      <c r="D854" s="22"/>
+    </row>
+    <row r="859" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A859" s="19"/>
+      <c r="B859" s="19"/>
+      <c r="C859" s="19"/>
+      <c r="D859" s="22"/>
+    </row>
+    <row r="862" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A862" s="19"/>
+      <c r="B862" s="19"/>
+      <c r="C862" s="19"/>
+      <c r="D862" s="22"/>
+    </row>
+    <row r="868" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A868" s="19"/>
+      <c r="B868" s="19"/>
+      <c r="C868" s="19"/>
+      <c r="D868" s="22"/>
+    </row>
+    <row r="872" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A872" s="19"/>
+      <c r="B872" s="19"/>
+      <c r="C872" s="19"/>
+      <c r="D872" s="22"/>
+    </row>
+    <row r="879" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A879" s="19"/>
+      <c r="B879" s="19"/>
+      <c r="C879" s="19"/>
+      <c r="D879" s="22"/>
+    </row>
+    <row r="881" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A881" s="19"/>
+      <c r="B881" s="19"/>
+      <c r="C881" s="19"/>
+      <c r="D881" s="22"/>
+    </row>
+    <row r="890" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A890" s="19"/>
+      <c r="B890" s="19"/>
+      <c r="C890" s="19"/>
+      <c r="D890" s="22"/>
+    </row>
+    <row r="895" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A895" s="19"/>
+      <c r="B895" s="19"/>
+      <c r="C895" s="19"/>
+      <c r="D895" s="22"/>
     </row>
     <row r="896" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A896" s="19"/>
@@ -15181,17 +15781,17 @@
       <c r="C896" s="19"/>
       <c r="D896" s="22"/>
     </row>
-    <row r="897" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A897" s="19"/>
-      <c r="B897" s="19"/>
-      <c r="C897" s="19"/>
-      <c r="D897" s="22"/>
-    </row>
-    <row r="906" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A906" s="19"/>
-      <c r="B906" s="19"/>
-      <c r="C906" s="19"/>
-      <c r="D906" s="22"/>
+    <row r="905" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A905" s="19"/>
+      <c r="B905" s="19"/>
+      <c r="C905" s="19"/>
+      <c r="D905" s="22"/>
+    </row>
+    <row r="907" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A907" s="19"/>
+      <c r="B907" s="19"/>
+      <c r="C907" s="19"/>
+      <c r="D907" s="22"/>
     </row>
     <row r="908" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A908" s="19"/>
@@ -15199,11 +15799,11 @@
       <c r="C908" s="19"/>
       <c r="D908" s="22"/>
     </row>
-    <row r="909" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A909" s="19"/>
-      <c r="B909" s="19"/>
-      <c r="C909" s="19"/>
-      <c r="D909" s="22"/>
+    <row r="910" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A910" s="19"/>
+      <c r="B910" s="19"/>
+      <c r="C910" s="19"/>
+      <c r="D910" s="22"/>
     </row>
     <row r="911" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A911" s="19"/>
@@ -15217,11 +15817,11 @@
       <c r="C912" s="19"/>
       <c r="D912" s="22"/>
     </row>
-    <row r="913" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A913" s="19"/>
-      <c r="B913" s="19"/>
-      <c r="C913" s="19"/>
-      <c r="D913" s="22"/>
+    <row r="917" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A917" s="19"/>
+      <c r="B917" s="19"/>
+      <c r="C917" s="19"/>
+      <c r="D917" s="22"/>
     </row>
     <row r="918" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A918" s="19"/>
@@ -15235,13 +15835,13 @@
       <c r="C919" s="19"/>
       <c r="D919" s="22"/>
     </row>
-    <row r="920" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A920" s="19"/>
-      <c r="B920" s="19"/>
-      <c r="C920" s="19"/>
-      <c r="D920" s="22"/>
-    </row>
-    <row r="923" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="922" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A922" s="19"/>
+      <c r="B922" s="19"/>
+      <c r="C922" s="19"/>
+      <c r="D922" s="22"/>
+    </row>
+    <row r="923" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A923" s="19"/>
       <c r="B923" s="19"/>
       <c r="C923" s="19"/>
@@ -15271,7 +15871,7 @@
       <c r="C927" s="19"/>
       <c r="D927" s="22"/>
     </row>
-    <row r="928" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="928" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A928" s="19"/>
       <c r="B928" s="19"/>
       <c r="C928" s="19"/>
@@ -15289,23 +15889,23 @@
       <c r="C930" s="19"/>
       <c r="D930" s="22"/>
     </row>
-    <row r="931" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="931" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A931" s="19"/>
       <c r="B931" s="19"/>
       <c r="C931" s="19"/>
       <c r="D931" s="22"/>
     </row>
-    <row r="932" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A932" s="19"/>
-      <c r="B932" s="19"/>
-      <c r="C932" s="19"/>
-      <c r="D932" s="22"/>
-    </row>
-    <row r="946" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A946" s="19"/>
-      <c r="B946" s="19"/>
-      <c r="C946" s="19"/>
-      <c r="D946" s="22"/>
+    <row r="945" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A945" s="19"/>
+      <c r="B945" s="19"/>
+      <c r="C945" s="19"/>
+      <c r="D945" s="22"/>
+    </row>
+    <row r="952" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A952" s="19"/>
+      <c r="B952" s="19"/>
+      <c r="C952" s="19"/>
+      <c r="D952" s="22"/>
     </row>
     <row r="953" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A953" s="19"/>
@@ -15313,17 +15913,17 @@
       <c r="C953" s="19"/>
       <c r="D953" s="22"/>
     </row>
-    <row r="954" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A954" s="19"/>
-      <c r="B954" s="19"/>
-      <c r="C954" s="19"/>
-      <c r="D954" s="22"/>
-    </row>
-    <row r="956" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A956" s="19"/>
-      <c r="B956" s="19"/>
-      <c r="C956" s="19"/>
-      <c r="D956" s="22"/>
+    <row r="955" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A955" s="19"/>
+      <c r="B955" s="19"/>
+      <c r="C955" s="19"/>
+      <c r="D955" s="22"/>
+    </row>
+    <row r="961" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A961" s="19"/>
+      <c r="B961" s="19"/>
+      <c r="C961" s="19"/>
+      <c r="D961" s="22"/>
     </row>
     <row r="962" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A962" s="19"/>
@@ -15331,11 +15931,11 @@
       <c r="C962" s="19"/>
       <c r="D962" s="22"/>
     </row>
-    <row r="963" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A963" s="19"/>
-      <c r="B963" s="19"/>
-      <c r="C963" s="19"/>
-      <c r="D963" s="22"/>
+    <row r="968" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A968" s="19"/>
+      <c r="B968" s="19"/>
+      <c r="C968" s="19"/>
+      <c r="D968" s="22"/>
     </row>
     <row r="969" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A969" s="19"/>
@@ -15343,11 +15943,11 @@
       <c r="C969" s="19"/>
       <c r="D969" s="22"/>
     </row>
-    <row r="970" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A970" s="19"/>
-      <c r="B970" s="19"/>
-      <c r="C970" s="19"/>
-      <c r="D970" s="22"/>
+    <row r="979" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A979" s="19"/>
+      <c r="B979" s="19"/>
+      <c r="C979" s="19"/>
+      <c r="D979" s="22"/>
     </row>
     <row r="980" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A980" s="19"/>
@@ -15355,23 +15955,23 @@
       <c r="C980" s="19"/>
       <c r="D980" s="22"/>
     </row>
-    <row r="981" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A981" s="19"/>
-      <c r="B981" s="19"/>
-      <c r="C981" s="19"/>
-      <c r="D981" s="22"/>
-    </row>
-    <row r="991" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A991" s="19"/>
-      <c r="B991" s="19"/>
-      <c r="C991" s="19"/>
-      <c r="D991" s="22"/>
-    </row>
-    <row r="998" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A998" s="19"/>
-      <c r="B998" s="19"/>
-      <c r="C998" s="19"/>
-      <c r="D998" s="22"/>
+    <row r="990" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A990" s="19"/>
+      <c r="B990" s="19"/>
+      <c r="C990" s="19"/>
+      <c r="D990" s="22"/>
+    </row>
+    <row r="997" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A997" s="19"/>
+      <c r="B997" s="19"/>
+      <c r="C997" s="19"/>
+      <c r="D997" s="22"/>
+    </row>
+    <row r="1016" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1016" s="19"/>
+      <c r="B1016" s="19"/>
+      <c r="C1016" s="19"/>
+      <c r="D1016" s="22"/>
     </row>
     <row r="1017" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1017" s="19"/>
@@ -15391,7 +15991,7 @@
       <c r="C1019" s="19"/>
       <c r="D1019" s="22"/>
     </row>
-    <row r="1020" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1020" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1020" s="19"/>
       <c r="B1020" s="19"/>
       <c r="C1020" s="19"/>
@@ -15409,23 +16009,23 @@
       <c r="C1022" s="19"/>
       <c r="D1022" s="22"/>
     </row>
-    <row r="1023" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1023" s="19"/>
-      <c r="B1023" s="19"/>
-      <c r="C1023" s="19"/>
-      <c r="D1023" s="22"/>
-    </row>
-    <row r="1025" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1025" s="19"/>
-      <c r="B1025" s="19"/>
-      <c r="C1025" s="19"/>
-      <c r="D1025" s="22"/>
-    </row>
-    <row r="1038" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1038" s="19"/>
-      <c r="B1038" s="19"/>
-      <c r="C1038" s="19"/>
-      <c r="D1038" s="22"/>
+    <row r="1024" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1024" s="19"/>
+      <c r="B1024" s="19"/>
+      <c r="C1024" s="19"/>
+      <c r="D1024" s="22"/>
+    </row>
+    <row r="1037" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1037" s="19"/>
+      <c r="B1037" s="19"/>
+      <c r="C1037" s="19"/>
+      <c r="D1037" s="22"/>
+    </row>
+    <row r="1044" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1044" s="19"/>
+      <c r="B1044" s="19"/>
+      <c r="C1044" s="19"/>
+      <c r="D1044" s="22"/>
     </row>
     <row r="1045" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1045" s="19"/>
@@ -15433,7 +16033,7 @@
       <c r="C1045" s="19"/>
       <c r="D1045" s="22"/>
     </row>
-    <row r="1046" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1046" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1046" s="19"/>
       <c r="B1046" s="19"/>
       <c r="C1046" s="19"/>
@@ -15451,35 +16051,35 @@
       <c r="C1048" s="19"/>
       <c r="D1048" s="22"/>
     </row>
-    <row r="1049" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1049" s="19"/>
-      <c r="B1049" s="19"/>
-      <c r="C1049" s="19"/>
-      <c r="D1049" s="22"/>
-    </row>
-    <row r="1051" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1051" s="19"/>
-      <c r="B1051" s="19"/>
-      <c r="C1051" s="19"/>
-      <c r="D1051" s="22"/>
-    </row>
-    <row r="1053" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1053" s="19"/>
-      <c r="B1053" s="19"/>
-      <c r="C1053" s="19"/>
-      <c r="D1053" s="22"/>
-    </row>
-    <row r="1060" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1060" s="19"/>
-      <c r="B1060" s="19"/>
-      <c r="C1060" s="19"/>
-      <c r="D1060" s="22"/>
-    </row>
-    <row r="1065" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1065" s="19"/>
-      <c r="B1065" s="19"/>
-      <c r="C1065" s="19"/>
-      <c r="D1065" s="22"/>
+    <row r="1050" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1050" s="19"/>
+      <c r="B1050" s="19"/>
+      <c r="C1050" s="19"/>
+      <c r="D1050" s="22"/>
+    </row>
+    <row r="1052" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1052" s="19"/>
+      <c r="B1052" s="19"/>
+      <c r="C1052" s="19"/>
+      <c r="D1052" s="22"/>
+    </row>
+    <row r="1059" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1059" s="19"/>
+      <c r="B1059" s="19"/>
+      <c r="C1059" s="19"/>
+      <c r="D1059" s="22"/>
+    </row>
+    <row r="1064" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1064" s="19"/>
+      <c r="B1064" s="19"/>
+      <c r="C1064" s="19"/>
+      <c r="D1064" s="22"/>
+    </row>
+    <row r="1066" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1066" s="19"/>
+      <c r="B1066" s="19"/>
+      <c r="C1066" s="19"/>
+      <c r="D1066" s="22"/>
     </row>
     <row r="1067" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1067" s="19"/>
@@ -15493,11 +16093,11 @@
       <c r="C1068" s="19"/>
       <c r="D1068" s="22"/>
     </row>
-    <row r="1069" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1069" s="19"/>
-      <c r="B1069" s="19"/>
-      <c r="C1069" s="19"/>
-      <c r="D1069" s="22"/>
+    <row r="1071" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1071" s="19"/>
+      <c r="B1071" s="19"/>
+      <c r="C1071" s="19"/>
+      <c r="D1071" s="22"/>
     </row>
     <row r="1072" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1072" s="19"/>
@@ -15505,7 +16105,7 @@
       <c r="C1072" s="19"/>
       <c r="D1072" s="22"/>
     </row>
-    <row r="1073" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1073" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1073" s="19"/>
       <c r="B1073" s="19"/>
       <c r="C1073" s="19"/>
@@ -15541,7 +16141,7 @@
       <c r="C1078" s="19"/>
       <c r="D1078" s="22"/>
     </row>
-    <row r="1079" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1079" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1079" s="19"/>
       <c r="B1079" s="19"/>
       <c r="C1079" s="19"/>
@@ -15709,13 +16309,13 @@
       <c r="C1106" s="19"/>
       <c r="D1106" s="22"/>
     </row>
-    <row r="1107" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1107" s="19"/>
-      <c r="B1107" s="19"/>
-      <c r="C1107" s="19"/>
-      <c r="D1107" s="22"/>
-    </row>
-    <row r="1125" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1124" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1124" s="19"/>
+      <c r="B1124" s="19"/>
+      <c r="C1124" s="19"/>
+      <c r="D1124" s="22"/>
+    </row>
+    <row r="1125" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1125" s="19"/>
       <c r="B1125" s="19"/>
       <c r="C1125" s="19"/>
@@ -15745,37 +16345,37 @@
       <c r="C1129" s="19"/>
       <c r="D1129" s="22"/>
     </row>
-    <row r="1130" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1130" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1130" s="19"/>
       <c r="B1130" s="19"/>
       <c r="C1130" s="19"/>
       <c r="D1130" s="22"/>
     </row>
-    <row r="1131" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1131" s="19"/>
-      <c r="B1131" s="19"/>
-      <c r="C1131" s="19"/>
-      <c r="D1131" s="22"/>
-    </row>
-    <row r="1149" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1149" s="19"/>
-      <c r="B1149" s="19"/>
-      <c r="C1149" s="19"/>
-      <c r="D1149" s="22"/>
-    </row>
-    <row r="1151" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1151" s="19"/>
-      <c r="B1151" s="19"/>
-      <c r="C1151" s="19"/>
-      <c r="D1151" s="22"/>
-    </row>
-    <row r="1155" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1148" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1148" s="19"/>
+      <c r="B1148" s="19"/>
+      <c r="C1148" s="19"/>
+      <c r="D1148" s="22"/>
+    </row>
+    <row r="1150" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1150" s="19"/>
+      <c r="B1150" s="19"/>
+      <c r="C1150" s="19"/>
+      <c r="D1150" s="22"/>
+    </row>
+    <row r="1154" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1154" s="19"/>
+      <c r="B1154" s="19"/>
+      <c r="C1154" s="19"/>
+      <c r="D1154" s="22"/>
+    </row>
+    <row r="1155" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1155" s="19"/>
       <c r="B1155" s="19"/>
       <c r="C1155" s="19"/>
       <c r="D1155" s="22"/>
     </row>
-    <row r="1156" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1156" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1156" s="19"/>
       <c r="B1156" s="19"/>
       <c r="C1156" s="19"/>
@@ -15787,7 +16387,7 @@
       <c r="C1157" s="19"/>
       <c r="D1157" s="22"/>
     </row>
-    <row r="1158" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1158" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1158" s="19"/>
       <c r="B1158" s="19"/>
       <c r="C1158" s="19"/>
@@ -15913,11 +16513,11 @@
       <c r="C1178" s="19"/>
       <c r="D1178" s="22"/>
     </row>
-    <row r="1179" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1179" s="19"/>
-      <c r="B1179" s="19"/>
-      <c r="C1179" s="19"/>
-      <c r="D1179" s="22"/>
+    <row r="1188" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1188" s="19"/>
+      <c r="B1188" s="19"/>
+      <c r="C1188" s="19"/>
+      <c r="D1188" s="22"/>
     </row>
     <row r="1189" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1189" s="19"/>
@@ -15943,29 +16543,29 @@
       <c r="C1192" s="19"/>
       <c r="D1192" s="22"/>
     </row>
-    <row r="1193" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1193" s="19"/>
-      <c r="B1193" s="19"/>
-      <c r="C1193" s="19"/>
-      <c r="D1193" s="22"/>
-    </row>
-    <row r="1229" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1229" s="19"/>
-      <c r="B1229" s="19"/>
-      <c r="C1229" s="19"/>
-      <c r="D1229" s="22"/>
-    </row>
-    <row r="1242" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1242" s="19"/>
-      <c r="B1242" s="19"/>
-      <c r="C1242" s="19"/>
-      <c r="D1242" s="22"/>
-    </row>
-    <row r="1245" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1245" s="19"/>
-      <c r="B1245" s="19"/>
-      <c r="C1245" s="19"/>
-      <c r="D1245" s="22"/>
+    <row r="1228" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1228" s="19"/>
+      <c r="B1228" s="19"/>
+      <c r="C1228" s="19"/>
+      <c r="D1228" s="22"/>
+    </row>
+    <row r="1241" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1241" s="19"/>
+      <c r="B1241" s="19"/>
+      <c r="C1241" s="19"/>
+      <c r="D1241" s="22"/>
+    </row>
+    <row r="1244" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1244" s="19"/>
+      <c r="B1244" s="19"/>
+      <c r="C1244" s="19"/>
+      <c r="D1244" s="22"/>
+    </row>
+    <row r="1265" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1265" s="19"/>
+      <c r="B1265" s="19"/>
+      <c r="C1265" s="19"/>
+      <c r="D1265" s="22"/>
     </row>
     <row r="1266" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1266" s="19"/>
@@ -15991,11 +16591,11 @@
       <c r="C1269" s="19"/>
       <c r="D1269" s="22"/>
     </row>
-    <row r="1270" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1270" s="19"/>
-      <c r="B1270" s="19"/>
-      <c r="C1270" s="19"/>
-      <c r="D1270" s="22"/>
+    <row r="1291" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1291" s="19"/>
+      <c r="B1291" s="19"/>
+      <c r="C1291" s="19"/>
+      <c r="D1291" s="22"/>
     </row>
     <row r="1292" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1292" s="19"/>
@@ -16141,11 +16741,11 @@
       <c r="C1315" s="19"/>
       <c r="D1315" s="22"/>
     </row>
-    <row r="1316" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1316" s="19"/>
-      <c r="B1316" s="19"/>
-      <c r="C1316" s="19"/>
-      <c r="D1316" s="22"/>
+    <row r="1321" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1321" s="19"/>
+      <c r="B1321" s="19"/>
+      <c r="C1321" s="19"/>
+      <c r="D1321" s="22"/>
     </row>
     <row r="1322" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1322" s="19"/>
@@ -16153,11 +16753,11 @@
       <c r="C1322" s="19"/>
       <c r="D1322" s="22"/>
     </row>
-    <row r="1323" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1323" s="19"/>
-      <c r="B1323" s="19"/>
-      <c r="C1323" s="19"/>
-      <c r="D1323" s="22"/>
+    <row r="1337" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1337" s="19"/>
+      <c r="B1337" s="19"/>
+      <c r="C1337" s="19"/>
+      <c r="D1337" s="22"/>
     </row>
     <row r="1338" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1338" s="19"/>
@@ -16165,11 +16765,11 @@
       <c r="C1338" s="19"/>
       <c r="D1338" s="22"/>
     </row>
-    <row r="1339" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1339" s="19"/>
-      <c r="B1339" s="19"/>
-      <c r="C1339" s="19"/>
-      <c r="D1339" s="22"/>
+    <row r="1344" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1344" s="19"/>
+      <c r="B1344" s="19"/>
+      <c r="C1344" s="19"/>
+      <c r="D1344" s="22"/>
     </row>
     <row r="1345" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1345" s="19"/>
@@ -16201,47 +16801,47 @@
       <c r="C1349" s="19"/>
       <c r="D1349" s="22"/>
     </row>
-    <row r="1350" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1350" s="19"/>
-      <c r="B1350" s="19"/>
-      <c r="C1350" s="19"/>
-      <c r="D1350" s="22"/>
-    </row>
-    <row r="1356" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1355" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1355" s="19"/>
+      <c r="B1355" s="19"/>
+      <c r="C1355" s="19"/>
+      <c r="D1355" s="22"/>
+    </row>
+    <row r="1356" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1356" s="19"/>
       <c r="B1356" s="19"/>
       <c r="C1356" s="19"/>
       <c r="D1356" s="22"/>
     </row>
-    <row r="1357" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1357" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1357" s="19"/>
       <c r="B1357" s="19"/>
       <c r="C1357" s="19"/>
       <c r="D1357" s="22"/>
     </row>
-    <row r="1358" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1358" s="19"/>
-      <c r="B1358" s="19"/>
-      <c r="C1358" s="19"/>
-      <c r="D1358" s="22"/>
-    </row>
-    <row r="1362" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1361" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1361" s="19"/>
+      <c r="B1361" s="19"/>
+      <c r="C1361" s="19"/>
+      <c r="D1361" s="22"/>
+    </row>
+    <row r="1362" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1362" s="19"/>
       <c r="B1362" s="19"/>
       <c r="C1362" s="19"/>
       <c r="D1362" s="22"/>
     </row>
-    <row r="1363" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1363" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1363" s="19"/>
       <c r="B1363" s="19"/>
       <c r="C1363" s="19"/>
       <c r="D1363" s="22"/>
     </row>
-    <row r="1364" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1364" s="19"/>
-      <c r="B1364" s="19"/>
-      <c r="C1364" s="19"/>
-      <c r="D1364" s="22"/>
+    <row r="1369" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1369" s="19"/>
+      <c r="B1369" s="19"/>
+      <c r="C1369" s="19"/>
+      <c r="D1369" s="22"/>
     </row>
     <row r="1370" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1370" s="19"/>
@@ -16249,23 +16849,23 @@
       <c r="C1370" s="19"/>
       <c r="D1370" s="22"/>
     </row>
-    <row r="1371" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1371" s="19"/>
-      <c r="B1371" s="19"/>
-      <c r="C1371" s="19"/>
-      <c r="D1371" s="22"/>
-    </row>
-    <row r="1382" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1382" s="19"/>
-      <c r="B1382" s="19"/>
-      <c r="C1382" s="19"/>
-      <c r="D1382" s="22"/>
-    </row>
-    <row r="1449" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1449" s="19"/>
-      <c r="B1449" s="19"/>
-      <c r="C1449" s="19"/>
-      <c r="D1449" s="22"/>
+    <row r="1381" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1381" s="19"/>
+      <c r="B1381" s="19"/>
+      <c r="C1381" s="19"/>
+      <c r="D1381" s="22"/>
+    </row>
+    <row r="1448" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1448" s="19"/>
+      <c r="B1448" s="19"/>
+      <c r="C1448" s="19"/>
+      <c r="D1448" s="22"/>
+    </row>
+    <row r="1604" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1604" s="19"/>
+      <c r="B1604" s="19"/>
+      <c r="C1604" s="19"/>
+      <c r="D1604" s="22"/>
     </row>
     <row r="1605" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1605" s="19"/>
@@ -16273,37 +16873,37 @@
       <c r="C1605" s="19"/>
       <c r="D1605" s="22"/>
     </row>
-    <row r="1606" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1606" s="19"/>
-      <c r="B1606" s="19"/>
-      <c r="C1606" s="19"/>
-      <c r="D1606" s="22"/>
-    </row>
-    <row r="1652" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1652" s="19"/>
-      <c r="B1652" s="19"/>
-      <c r="C1652" s="19"/>
-      <c r="D1652" s="22"/>
-    </row>
-    <row r="1655" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1655" s="19"/>
-      <c r="B1655" s="19"/>
-      <c r="C1655" s="19"/>
-      <c r="D1655" s="22"/>
-    </row>
-    <row r="1661" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1661" s="19"/>
-      <c r="B1661" s="19"/>
-      <c r="C1661" s="19"/>
-      <c r="D1661" s="22"/>
-    </row>
-    <row r="1663" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1651" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1651" s="19"/>
+      <c r="B1651" s="19"/>
+      <c r="C1651" s="19"/>
+      <c r="D1651" s="22"/>
+    </row>
+    <row r="1654" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1654" s="19"/>
+      <c r="B1654" s="19"/>
+      <c r="C1654" s="19"/>
+      <c r="D1654" s="22"/>
+    </row>
+    <row r="1660" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1660" s="19"/>
+      <c r="B1660" s="19"/>
+      <c r="C1660" s="19"/>
+      <c r="D1660" s="22"/>
+    </row>
+    <row r="1662" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1662" s="19"/>
+      <c r="B1662" s="19"/>
+      <c r="C1662" s="19"/>
+      <c r="D1662" s="22"/>
+    </row>
+    <row r="1663" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1663" s="19"/>
       <c r="B1663" s="19"/>
       <c r="C1663" s="19"/>
       <c r="D1663" s="22"/>
     </row>
-    <row r="1664" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1664" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1664" s="19"/>
       <c r="B1664" s="19"/>
       <c r="C1664" s="19"/>
@@ -16315,23 +16915,23 @@
       <c r="C1665" s="19"/>
       <c r="D1665" s="22"/>
     </row>
-    <row r="1666" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1666" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1666" s="19"/>
       <c r="B1666" s="19"/>
       <c r="C1666" s="19"/>
       <c r="D1666" s="22"/>
     </row>
-    <row r="1667" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1667" s="19"/>
-      <c r="B1667" s="19"/>
-      <c r="C1667" s="19"/>
-      <c r="D1667" s="22"/>
-    </row>
-    <row r="1678" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1678" s="19"/>
-      <c r="B1678" s="19"/>
-      <c r="C1678" s="19"/>
-      <c r="D1678" s="22"/>
+    <row r="1677" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1677" s="19"/>
+      <c r="B1677" s="19"/>
+      <c r="C1677" s="19"/>
+      <c r="D1677" s="22"/>
+    </row>
+    <row r="1679" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1679" s="19"/>
+      <c r="B1679" s="19"/>
+      <c r="C1679" s="19"/>
+      <c r="D1679" s="22"/>
     </row>
     <row r="1680" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1680" s="19"/>
@@ -16483,11 +17083,11 @@
       <c r="C1704" s="19"/>
       <c r="D1704" s="22"/>
     </row>
-    <row r="1705" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1705" s="19"/>
-      <c r="B1705" s="19"/>
-      <c r="C1705" s="19"/>
-      <c r="D1705" s="22"/>
+    <row r="1763" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1763" s="19"/>
+      <c r="B1763" s="19"/>
+      <c r="C1763" s="19"/>
+      <c r="D1763" s="22"/>
     </row>
     <row r="1764" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1764" s="19"/>
@@ -16495,17 +17095,17 @@
       <c r="C1764" s="19"/>
       <c r="D1764" s="22"/>
     </row>
-    <row r="1765" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1765" s="19"/>
-      <c r="B1765" s="19"/>
-      <c r="C1765" s="19"/>
-      <c r="D1765" s="22"/>
-    </row>
-    <row r="2093" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2093" s="19"/>
-      <c r="B2093" s="19"/>
-      <c r="C2093" s="19"/>
-      <c r="D2093" s="22"/>
+    <row r="2092" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2092" s="19"/>
+      <c r="B2092" s="19"/>
+      <c r="C2092" s="19"/>
+      <c r="D2092" s="22"/>
+    </row>
+    <row r="2236" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2236" s="19"/>
+      <c r="B2236" s="19"/>
+      <c r="C2236" s="19"/>
+      <c r="D2236" s="22"/>
     </row>
     <row r="2237" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2237" s="19"/>
@@ -16603,47 +17203,47 @@
       <c r="C2252" s="19"/>
       <c r="D2252" s="22"/>
     </row>
-    <row r="2253" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2253" s="19"/>
-      <c r="B2253" s="19"/>
-      <c r="C2253" s="19"/>
-      <c r="D2253" s="22"/>
-    </row>
-    <row r="2260" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2260" s="19"/>
-      <c r="B2260" s="19"/>
-      <c r="C2260" s="19"/>
-      <c r="D2260" s="22"/>
-    </row>
-    <row r="2421" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2259" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2259" s="19"/>
+      <c r="B2259" s="19"/>
+      <c r="C2259" s="19"/>
+      <c r="D2259" s="22"/>
+    </row>
+    <row r="2420" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2420" s="19"/>
+      <c r="B2420" s="19"/>
+      <c r="C2420" s="19"/>
+      <c r="D2420" s="22"/>
+    </row>
+    <row r="2421" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2421" s="19"/>
       <c r="B2421" s="19"/>
       <c r="C2421" s="19"/>
       <c r="D2421" s="22"/>
     </row>
-    <row r="2422" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2422" s="19"/>
-      <c r="B2422" s="19"/>
-      <c r="C2422" s="19"/>
-      <c r="D2422" s="22"/>
-    </row>
-    <row r="2427" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2427" s="19"/>
-      <c r="B2427" s="19"/>
-      <c r="C2427" s="19"/>
-      <c r="D2427" s="22"/>
-    </row>
-    <row r="2521" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2521" s="19"/>
-      <c r="B2521" s="19"/>
-      <c r="C2521" s="19"/>
-      <c r="D2521" s="22"/>
-    </row>
-    <row r="2546" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2546" s="19"/>
-      <c r="B2546" s="19"/>
-      <c r="C2546" s="19"/>
-      <c r="D2546" s="22"/>
+    <row r="2426" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2426" s="19"/>
+      <c r="B2426" s="19"/>
+      <c r="C2426" s="19"/>
+      <c r="D2426" s="22"/>
+    </row>
+    <row r="2520" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2520" s="19"/>
+      <c r="B2520" s="19"/>
+      <c r="C2520" s="19"/>
+      <c r="D2520" s="22"/>
+    </row>
+    <row r="2545" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2545" s="19"/>
+      <c r="B2545" s="19"/>
+      <c r="C2545" s="19"/>
+      <c r="D2545" s="22"/>
+    </row>
+    <row r="2547" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2547" s="19"/>
+      <c r="B2547" s="19"/>
+      <c r="C2547" s="19"/>
+      <c r="D2547" s="22"/>
     </row>
     <row r="2548" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2548" s="19"/>
@@ -16651,11 +17251,11 @@
       <c r="C2548" s="19"/>
       <c r="D2548" s="22"/>
     </row>
-    <row r="2549" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2549" s="19"/>
-      <c r="B2549" s="19"/>
-      <c r="C2549" s="19"/>
-      <c r="D2549" s="22"/>
+    <row r="2550" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2550" s="19"/>
+      <c r="B2550" s="19"/>
+      <c r="C2550" s="19"/>
+      <c r="D2550" s="22"/>
     </row>
     <row r="2551" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2551" s="19"/>
@@ -16663,11 +17263,11 @@
       <c r="C2551" s="19"/>
       <c r="D2551" s="22"/>
     </row>
-    <row r="2552" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2552" s="19"/>
-      <c r="B2552" s="19"/>
-      <c r="C2552" s="19"/>
-      <c r="D2552" s="22"/>
+    <row r="2557" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2557" s="19"/>
+      <c r="B2557" s="19"/>
+      <c r="C2557" s="19"/>
+      <c r="D2557" s="22"/>
     </row>
     <row r="2558" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2558" s="19"/>
@@ -16693,17 +17293,17 @@
       <c r="C2561" s="19"/>
       <c r="D2561" s="22"/>
     </row>
-    <row r="2562" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2562" s="19"/>
-      <c r="B2562" s="19"/>
-      <c r="C2562" s="19"/>
-      <c r="D2562" s="22"/>
-    </row>
-    <row r="2571" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2571" s="19"/>
-      <c r="B2571" s="19"/>
-      <c r="C2571" s="19"/>
-      <c r="D2571" s="22"/>
+    <row r="2570" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2570" s="19"/>
+      <c r="B2570" s="19"/>
+      <c r="C2570" s="19"/>
+      <c r="D2570" s="22"/>
+    </row>
+    <row r="2572" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2572" s="19"/>
+      <c r="B2572" s="19"/>
+      <c r="C2572" s="19"/>
+      <c r="D2572" s="22"/>
     </row>
     <row r="2573" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2573" s="19"/>
@@ -16711,11 +17311,11 @@
       <c r="C2573" s="19"/>
       <c r="D2573" s="22"/>
     </row>
-    <row r="2574" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2574" s="19"/>
-      <c r="B2574" s="19"/>
-      <c r="C2574" s="19"/>
-      <c r="D2574" s="22"/>
+    <row r="2575" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2575" s="19"/>
+      <c r="B2575" s="19"/>
+      <c r="C2575" s="19"/>
+      <c r="D2575" s="22"/>
     </row>
     <row r="2576" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2576" s="19"/>
@@ -16723,11 +17323,11 @@
       <c r="C2576" s="19"/>
       <c r="D2576" s="22"/>
     </row>
-    <row r="2577" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2577" s="19"/>
-      <c r="B2577" s="19"/>
-      <c r="C2577" s="19"/>
-      <c r="D2577" s="22"/>
+    <row r="2582" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2582" s="19"/>
+      <c r="B2582" s="19"/>
+      <c r="C2582" s="19"/>
+      <c r="D2582" s="22"/>
     </row>
     <row r="2583" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2583" s="19"/>
@@ -16753,11 +17353,11 @@
       <c r="C2586" s="19"/>
       <c r="D2586" s="22"/>
     </row>
-    <row r="2587" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2587" s="19"/>
-      <c r="B2587" s="19"/>
-      <c r="C2587" s="19"/>
-      <c r="D2587" s="22"/>
+    <row r="2588" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2588" s="19"/>
+      <c r="B2588" s="19"/>
+      <c r="C2588" s="19"/>
+      <c r="D2588" s="22"/>
     </row>
     <row r="2589" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2589" s="19"/>
@@ -16771,11 +17371,11 @@
       <c r="C2590" s="19"/>
       <c r="D2590" s="22"/>
     </row>
-    <row r="2591" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2591" s="19"/>
-      <c r="B2591" s="19"/>
-      <c r="C2591" s="19"/>
-      <c r="D2591" s="22"/>
+    <row r="2605" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2605" s="19"/>
+      <c r="B2605" s="19"/>
+      <c r="C2605" s="19"/>
+      <c r="D2605" s="22"/>
     </row>
     <row r="2606" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2606" s="19"/>
@@ -17047,17 +17647,17 @@
       <c r="C2650" s="19"/>
       <c r="D2650" s="22"/>
     </row>
-    <row r="2651" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2651" s="19"/>
-      <c r="B2651" s="19"/>
-      <c r="C2651" s="19"/>
-      <c r="D2651" s="22"/>
-    </row>
-    <row r="2674" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2674" s="19"/>
-      <c r="B2674" s="19"/>
-      <c r="C2674" s="19"/>
-      <c r="D2674" s="22"/>
+    <row r="2673" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2673" s="19"/>
+      <c r="B2673" s="19"/>
+      <c r="C2673" s="19"/>
+      <c r="D2673" s="22"/>
+    </row>
+    <row r="2683" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2683" s="19"/>
+      <c r="B2683" s="19"/>
+      <c r="C2683" s="19"/>
+      <c r="D2683" s="22"/>
     </row>
     <row r="2684" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2684" s="19"/>
@@ -17065,17 +17665,17 @@
       <c r="C2684" s="19"/>
       <c r="D2684" s="22"/>
     </row>
-    <row r="2685" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2685" s="19"/>
-      <c r="B2685" s="19"/>
-      <c r="C2685" s="19"/>
-      <c r="D2685" s="22"/>
-    </row>
-    <row r="2690" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2690" s="19"/>
-      <c r="B2690" s="19"/>
-      <c r="C2690" s="19"/>
-      <c r="D2690" s="22"/>
+    <row r="2689" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2689" s="19"/>
+      <c r="B2689" s="19"/>
+      <c r="C2689" s="19"/>
+      <c r="D2689" s="22"/>
+    </row>
+    <row r="2699" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2699" s="19"/>
+      <c r="B2699" s="19"/>
+      <c r="C2699" s="19"/>
+      <c r="D2699" s="22"/>
     </row>
     <row r="2700" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2700" s="19"/>
@@ -17083,17 +17683,17 @@
       <c r="C2700" s="19"/>
       <c r="D2700" s="22"/>
     </row>
-    <row r="2701" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2701" s="19"/>
-      <c r="B2701" s="19"/>
-      <c r="C2701" s="19"/>
-      <c r="D2701" s="22"/>
-    </row>
-    <row r="2706" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2706" s="19"/>
-      <c r="B2706" s="19"/>
-      <c r="C2706" s="19"/>
-      <c r="D2706" s="22"/>
+    <row r="2705" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2705" s="19"/>
+      <c r="B2705" s="19"/>
+      <c r="C2705" s="19"/>
+      <c r="D2705" s="22"/>
+    </row>
+    <row r="2715" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2715" s="19"/>
+      <c r="B2715" s="19"/>
+      <c r="C2715" s="19"/>
+      <c r="D2715" s="22"/>
     </row>
     <row r="2716" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2716" s="19"/>
@@ -17101,35 +17701,29 @@
       <c r="C2716" s="19"/>
       <c r="D2716" s="22"/>
     </row>
-    <row r="2717" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2717" s="19"/>
-      <c r="B2717" s="19"/>
-      <c r="C2717" s="19"/>
-      <c r="D2717" s="22"/>
-    </row>
-    <row r="2736" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2736" s="19"/>
-      <c r="B2736" s="19"/>
-      <c r="C2736" s="19"/>
-      <c r="D2736" s="22"/>
-    </row>
-    <row r="2753" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2753" s="19"/>
-      <c r="B2753" s="19"/>
-      <c r="C2753" s="19"/>
-      <c r="D2753" s="22"/>
-    </row>
-    <row r="2778" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2778" s="19"/>
-      <c r="B2778" s="19"/>
-      <c r="C2778" s="19"/>
-      <c r="D2778" s="22"/>
-    </row>
-    <row r="2804" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2804" s="19"/>
-      <c r="B2804" s="19"/>
-      <c r="C2804" s="19"/>
-      <c r="D2804" s="22"/>
+    <row r="2735" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2735" s="19"/>
+      <c r="B2735" s="19"/>
+      <c r="C2735" s="19"/>
+      <c r="D2735" s="22"/>
+    </row>
+    <row r="2752" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2752" s="19"/>
+      <c r="B2752" s="19"/>
+      <c r="C2752" s="19"/>
+      <c r="D2752" s="22"/>
+    </row>
+    <row r="2777" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2777" s="19"/>
+      <c r="B2777" s="19"/>
+      <c r="C2777" s="19"/>
+      <c r="D2777" s="22"/>
+    </row>
+    <row r="2803" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2803" s="19"/>
+      <c r="B2803" s="19"/>
+      <c r="C2803" s="19"/>
+      <c r="D2803" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17258,10 +17852,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1183"/>
+  <dimension ref="A1:C1238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1131" workbookViewId="0">
-      <selection activeCell="B1183" sqref="A1137:B1183"/>
+    <sheetView topLeftCell="A1197" workbookViewId="0">
+      <selection activeCell="A1196" sqref="A1196:B1238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30460,6 +31054,522 @@
       <c r="C1183" s="18" t="str">
         <f t="shared" si="23"/>
         <v xml:space="preserve">CCD_CRUISE_AGG_V.LEG_VESS_NAME_DATES_BR_LIST, </v>
+      </c>
+    </row>
+    <row r="1196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1196" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1196" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1196" s="18" t="str">
+        <f t="shared" ref="C1196:C1238" si="24">CONCATENATE(A1196, ".", B1196, ", ")</f>
+        <v xml:space="preserve">ccd_cruise_leg_v.CRUISE_ID, </v>
+      </c>
+    </row>
+    <row r="1197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1197" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1197" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1197" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.CRUISE_NAME, </v>
+      </c>
+    </row>
+    <row r="1198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1198" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1198" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1198" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.CRUISE_NOTES, </v>
+      </c>
+    </row>
+    <row r="1199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1199" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1199" t="s">
+        <v>408</v>
+      </c>
+      <c r="C1199" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.CRUISE_DESC, </v>
+      </c>
+    </row>
+    <row r="1200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1200" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1200" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1200" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.OBJ_BASED_METRICS, </v>
+      </c>
+    </row>
+    <row r="1201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1201" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1201" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1201" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.SCI_CENTER_DIV_ID, </v>
+      </c>
+    </row>
+    <row r="1202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1202" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1202" t="s">
+        <v>410</v>
+      </c>
+      <c r="C1202" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.SCI_CENTER_DIV_CODE, </v>
+      </c>
+    </row>
+    <row r="1203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1203" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1203" t="s">
+        <v>411</v>
+      </c>
+      <c r="C1203" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.SCI_CENTER_DIV_NAME, </v>
+      </c>
+    </row>
+    <row r="1204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1204" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1204" t="s">
+        <v>412</v>
+      </c>
+      <c r="C1204" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.SCI_CENTER_DIV_DESC, </v>
+      </c>
+    </row>
+    <row r="1205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1205" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1205" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1205" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.SCI_CENTER_ID, </v>
+      </c>
+    </row>
+    <row r="1206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1206" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1206" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1206" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.SCI_CENTER_NAME, </v>
+      </c>
+    </row>
+    <row r="1207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1207" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1207" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1207" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.SCI_CENTER_DESC, </v>
+      </c>
+    </row>
+    <row r="1208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1208" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1208" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1208" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.STD_SVY_NAME_ID, </v>
+      </c>
+    </row>
+    <row r="1209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1209" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1209" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1209" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.STD_SVY_NAME, </v>
+      </c>
+    </row>
+    <row r="1210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1210" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1210" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1210" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.STD_SVY_DESC, </v>
+      </c>
+    </row>
+    <row r="1211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1211" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1211" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1211" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.SVY_FREQ_ID, </v>
+      </c>
+    </row>
+    <row r="1212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1212" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1212" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1212" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.SVY_FREQ_NAME, </v>
+      </c>
+    </row>
+    <row r="1213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1213" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1213" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1213" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.SVY_FREQ_DESC, </v>
+      </c>
+    </row>
+    <row r="1214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1214" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1214" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1214" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.STD_SVY_NAME_OTH, </v>
+      </c>
+    </row>
+    <row r="1215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1215" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1215" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1215" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.STD_SVY_NAME_VAL, </v>
+      </c>
+    </row>
+    <row r="1216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1216" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1216" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1216" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.SVY_TYPE_ID, </v>
+      </c>
+    </row>
+    <row r="1217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1217" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1217" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1217" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.SVY_TYPE_NAME, </v>
+      </c>
+    </row>
+    <row r="1218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1218" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1218" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1218" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.SVY_TYPE_DESC, </v>
+      </c>
+    </row>
+    <row r="1219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1219" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1219" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1219" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.CRUISE_URL, </v>
+      </c>
+    </row>
+    <row r="1220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1220" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1220" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1220" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.CRUISE_CONT_EMAIL, </v>
+      </c>
+    </row>
+    <row r="1221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1221" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1221" t="s">
+        <v>413</v>
+      </c>
+      <c r="C1221" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.PTA_ISS_ID, </v>
+      </c>
+    </row>
+    <row r="1222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1222" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1222" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.CRUISE_LEG_ID, </v>
+      </c>
+    </row>
+    <row r="1223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1223" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1223" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1223" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.LEG_NAME, </v>
+      </c>
+    </row>
+    <row r="1224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1224" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1224" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1224" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.LEG_START_DATE, </v>
+      </c>
+    </row>
+    <row r="1225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1225" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1225" t="s">
+        <v>239</v>
+      </c>
+      <c r="C1225" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.FORMAT_LEG_START_DATE, </v>
+      </c>
+    </row>
+    <row r="1226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1226" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1226" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1226" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.LEG_END_DATE, </v>
+      </c>
+    </row>
+    <row r="1227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1227" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1227" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1227" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.FORMAT_LEG_END_DATE, </v>
+      </c>
+    </row>
+    <row r="1228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1228" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1228" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1228" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.LEG_DAS, </v>
+      </c>
+    </row>
+    <row r="1229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1229" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1229" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1229" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.LEG_YEAR, </v>
+      </c>
+    </row>
+    <row r="1230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1230" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1230" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1230" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.TZ_NAME, </v>
+      </c>
+    </row>
+    <row r="1231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1231" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1231" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1231" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.LEG_FISC_YEAR, </v>
+      </c>
+    </row>
+    <row r="1232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1232" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1232" t="s">
+        <v>245</v>
+      </c>
+      <c r="C1232" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.LEG_DESC, </v>
+      </c>
+    </row>
+    <row r="1233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1233" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1233" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1233" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.VESSEL_ID, </v>
+      </c>
+    </row>
+    <row r="1234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1234" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1234" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1234" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.VESSEL_NAME, </v>
+      </c>
+    </row>
+    <row r="1235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1235" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1235" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1235" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.VESSEL_DESC, </v>
+      </c>
+    </row>
+    <row r="1236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1236" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1236" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1236" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.PLAT_TYPE_ID, </v>
+      </c>
+    </row>
+    <row r="1237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1237" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1237" t="s">
+        <v>250</v>
+      </c>
+      <c r="C1237" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.PLAT_TYPE_NAME, </v>
+      </c>
+    </row>
+    <row r="1238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1238" s="18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1238" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1238" s="18" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">ccd_cruise_leg_v.PLAT_TYPE_DESC, </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the data model to integrate the PICDM.DS_PIR_SCOR_V view
</commit_message>
<xml_diff>
--- a/docs/DB_DDL_helper_template.xlsx
+++ b/docs/DB_DDL_helper_template.xlsx
@@ -737,7 +737,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3710" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3987" uniqueCount="653">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -2445,6 +2445,258 @@
   </si>
   <si>
     <t>This field contains the Standard Survey Name defined for the given cruise.	If the STD_SVY_NAME_ID field is defined then the associated CCD_STD_SVY_NAMES.STD_SVY_NAME is used because the foreign key is given precedence, otherwise the STD_SVY_NAME_OTH field value is used</t>
+  </si>
+  <si>
+    <t>METADATA_FOLDER</t>
+  </si>
+  <si>
+    <t>ORG_ALIAS_ABBREV</t>
+  </si>
+  <si>
+    <t>LIBRARY_ORG</t>
+  </si>
+  <si>
+    <t>CAT_ID</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>PARR_KEYWORDS</t>
+  </si>
+  <si>
+    <t>COMPLETION_SCORE</t>
+  </si>
+  <si>
+    <t>COMPLETION_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>FORMAT_COMPLETION_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>IDENTIFICATION_SCORE</t>
+  </si>
+  <si>
+    <t>IDENTIFICATION_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>FORMAT_IDENTIFICATION_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>ACCESS_SCORE</t>
+  </si>
+  <si>
+    <t>ACCESS_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>FORMAT_ACCESS_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>COVERAGE_SCORE</t>
+  </si>
+  <si>
+    <t>COVERAGE_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>FORMAT_COVERAGE_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>CONTENT_SCORE</t>
+  </si>
+  <si>
+    <t>CONTENT_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>FORMAT_CONTENT_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>HISTORY_SCORE</t>
+  </si>
+  <si>
+    <t>HISTORY_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>FORMAT_HISTORY_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>QUALITY_SCORE</t>
+  </si>
+  <si>
+    <t>QUALITY_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>FORMAT_QUALITY_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>CONNECTION_SCORE</t>
+  </si>
+  <si>
+    <t>CONNECTION_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>FORMAT_CONNECTION_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>METADATA_SCORE</t>
+  </si>
+  <si>
+    <t>METADATA_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>FORMAT_METADATA_SCORE_PCT</t>
+  </si>
+  <si>
+    <t>METADATA_CONTACT</t>
+  </si>
+  <si>
+    <t>ACCESS_WAIVER_YN</t>
+  </si>
+  <si>
+    <t>GEO_DATA_PRES_FORM</t>
+  </si>
+  <si>
+    <t>PUBLISHED_STATUS</t>
+  </si>
+  <si>
+    <t>CREATE_DTM</t>
+  </si>
+  <si>
+    <t>LAST_MOD_DTM</t>
+  </si>
+  <si>
+    <t>INPORT_LINK_URL</t>
+  </si>
+  <si>
+    <t>REFRESH_DTM</t>
+  </si>
+  <si>
+    <t>FORMAT_REFRESH_DTM</t>
+  </si>
+  <si>
+    <t>DS_PIR_SCOR_V</t>
+  </si>
+  <si>
+    <t>The maximum parent InPort folder's Title (division/program level) for the given Pacific Island Region's data set</t>
+  </si>
+  <si>
+    <t>The organization division/program alias abbreviation defined for the given InPort Metadata Folder name</t>
+  </si>
+  <si>
+    <t>The InPort Library Organization</t>
+  </si>
+  <si>
+    <t>InPort Title (NMFS_INP_CATALOG_ITEMS.TITLE)</t>
+  </si>
+  <si>
+    <t>InPort  PARR Keywords (NMFS_INP_CC_KEYWORDS.KEYWORD)</t>
+  </si>
+  <si>
+    <t>InPort Completion Score (NMFS_INP_RBR_DS_SCORES.COMPLETION_SCORE)</t>
+  </si>
+  <si>
+    <t>InPort Completion Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>Formatted InPort Completion Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>InPort Identification Score (NMFS_INP_RBR_DS_SCORES.IDENTIFICATION_SCORE)</t>
+  </si>
+  <si>
+    <t>InPort Identification Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>Formatted InPort Identification Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>InPort Access Score (NMFS_INP_RBR_DS_SCORES.ACCESS_SCORE)</t>
+  </si>
+  <si>
+    <t>InPort Access Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>Formatted InPort Access Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>InPort Coverage Score (NMFS_INP_RBR_DS_SCORES.COVERAGE_SCORE)</t>
+  </si>
+  <si>
+    <t>InPort Coverage Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>Formatted InPort Coverage Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>InPort Content Score (NMFS_INP_RBR_DS_SCORES.CONTENT_SCORE)</t>
+  </si>
+  <si>
+    <t>InPort Content Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>Formatted InPort Content Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>InPort History Score (NMFS_INP_RBR_DS_SCORES.HISTORY_SCORE)</t>
+  </si>
+  <si>
+    <t>InPort History Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>Formatted InPort History Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>InPort Quality Score (NMFS_INP_RBR_DS_SCORES.QUALITY_SCORE)</t>
+  </si>
+  <si>
+    <t>InPort Quality Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>Formatted InPort Quality Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>InPort Connection Score (NMFS_INP_RBR_DS_SCORES.CONNECTION_SCORE)</t>
+  </si>
+  <si>
+    <t>InPort Connection Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>Formatted InPort Connection Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>InPort Metadata Score (NMFS_INP_RBR_DS_SCORES.METADATA_SCORE)</t>
+  </si>
+  <si>
+    <t>InPort Metadata Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>Formatted InPort Metadata Score Percentage (to 2 significant digits)</t>
+  </si>
+  <si>
+    <t>Comma-delimited list of metadata contacts for the corresponding data set</t>
+  </si>
+  <si>
+    <t>Access Waiver? (NMFS_INP_CC_DATA_MANAGEMENT.ACCESS_WAIVER_YN)</t>
+  </si>
+  <si>
+    <t>Geo Data Presentation Format (NMFS_INP_CATALOG_ITEMS.DS_GEO_DATA_PRES_FORM)</t>
+  </si>
+  <si>
+    <t>Published Status (NMFS_INP_CATALOG_ITEMS.PUBLISHED_STATUS)</t>
+  </si>
+  <si>
+    <t>Create Date/Time (NMFS_INP_CATALOG_ITEMS.CREATE_DTM)</t>
+  </si>
+  <si>
+    <t>Modified Date/Time (NMFS_INP_CATALOG_ITEMS.LAST_MOD_DTM)</t>
+  </si>
+  <si>
+    <t>Generated standard InPort data set URL based on the corresponding CAT_ID</t>
+  </si>
+  <si>
+    <t>The Date/Time the PIR data set record was refreshed from ODS</t>
+  </si>
+  <si>
+    <t>The Formatted Date/Time the PIR data set record was refreshed from ODS (in MM/DD/YYYY HH24:MI:SS format)</t>
   </si>
 </sst>
 </file>
@@ -8330,10 +8582,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2803"/>
+  <dimension ref="A1:D2802"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A446" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C487" sqref="C487"/>
+    <sheetView tabSelected="1" topLeftCell="A477" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D496" sqref="D496:D550"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15031,53 +15283,830 @@
         <v>COMMENT ON COLUMN CCD_LEG_DATA_SETS_V.PLAT_TYPE_DESC IS 'Description for the given Platform Type';</v>
       </c>
     </row>
+    <row r="496" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A496" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B496" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C496" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D496" s="22" t="str">
+        <f t="shared" ref="D496:D550" si="11">CONCATENATE("COMMENT ON COLUMN ",A496, ".", B496, " IS '", SUBSTITUTE(C496, "'", "''"), "';")</f>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_ID IS 'Primary key for the CCD_DATA_SETS table';</v>
+      </c>
+    </row>
+    <row r="497" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A497" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B497" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C497" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="D497" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_NAME IS 'The Name of the data set';</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A498" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B498" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C498" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="D498" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_DESC IS 'Description for the data set';</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A499" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B499" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C499" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D499" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_INPORT_CAT_ID IS 'InPort Catalog ID for the data set';</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A500" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B500" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C500" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="D500" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_INPORT_URL IS 'InPort metadata URL for the data set';</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A501" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B501" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C501" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D501" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_TYPE_ID IS 'Primary key for the CCD_DATA_SET_TYPES table';</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A502" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B502" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C502" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="D502" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_TYPE_NAME IS 'Name for the data set type';</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A503" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B503" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C503" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="D503" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_TYPE_DESC IS 'Description for the data set type';</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A504" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B504" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C504" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D504" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_TYPE_DOC_URL IS 'Documentation URL for the data type, this can be an InPort URL for the parent Project record of the individual data sets or a documentation package that provides information about this data set type';</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A505" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B505" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C505" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="D505" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_STATUS_ID IS 'Primary key for the CCD_DATA_SET_STATUS table';</v>
+      </c>
+    </row>
+    <row r="506" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A506" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B506" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C506" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="D506" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.STATUS_CODE IS 'The alpha-numeric code for the data status';</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A507" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B507" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C507" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="D507" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.STATUS_NAME IS 'The name of the data status';</v>
+      </c>
+    </row>
     <row r="508" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A508" s="19"/>
-      <c r="B508" s="19"/>
-      <c r="C508" s="19"/>
-      <c r="D508" s="22"/>
+      <c r="A508" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B508" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C508" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="D508" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.STATUS_DESC IS 'The description for the data status';</v>
+      </c>
     </row>
     <row r="509" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A509" s="19"/>
-      <c r="B509" s="19"/>
-      <c r="C509" s="19"/>
-      <c r="D509" s="22"/>
+      <c r="A509" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B509" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="C509" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D509" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.STATUS_COLOR IS 'The hex value for the color that the data set status has in the application interface';</v>
+      </c>
     </row>
     <row r="510" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A510" s="19"/>
-      <c r="B510" s="19"/>
-      <c r="C510" s="19"/>
-      <c r="D510" s="22"/>
+      <c r="A510" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B510" s="18" t="s">
+        <v>569</v>
+      </c>
+      <c r="C510" s="19" t="s">
+        <v>612</v>
+      </c>
+      <c r="D510" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.METADATA_FOLDER IS 'The maximum parent InPort folder''s Title (division/program level) for the given Pacific Island Region''s data set';</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A511" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B511" s="18" t="s">
+        <v>570</v>
+      </c>
+      <c r="C511" s="19" t="s">
+        <v>613</v>
+      </c>
+      <c r="D511" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.ORG_ALIAS_ABBREV IS 'The organization division/program alias abbreviation defined for the given InPort Metadata Folder name';</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A512" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B512" s="18" t="s">
+        <v>571</v>
+      </c>
+      <c r="C512" s="19" t="s">
+        <v>614</v>
+      </c>
+      <c r="D512" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.LIBRARY_ORG IS 'The InPort Library Organization';</v>
+      </c>
+    </row>
+    <row r="513" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A513" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B513" s="18" t="s">
+        <v>573</v>
+      </c>
+      <c r="C513" s="19" t="s">
+        <v>615</v>
+      </c>
+      <c r="D513" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.TITLE IS 'InPort Title (NMFS_INP_CATALOG_ITEMS.TITLE)';</v>
+      </c>
+    </row>
+    <row r="514" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A514" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B514" s="18" t="s">
+        <v>574</v>
+      </c>
+      <c r="C514" s="19" t="s">
+        <v>616</v>
+      </c>
+      <c r="D514" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.PARR_KEYWORDS IS 'InPort  PARR Keywords (NMFS_INP_CC_KEYWORDS.KEYWORD)';</v>
+      </c>
+    </row>
+    <row r="515" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A515" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B515" s="18" t="s">
+        <v>575</v>
+      </c>
+      <c r="C515" s="19" t="s">
+        <v>617</v>
+      </c>
+      <c r="D515" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.COMPLETION_SCORE IS 'InPort Completion Score (NMFS_INP_RBR_DS_SCORES.COMPLETION_SCORE)';</v>
+      </c>
+    </row>
+    <row r="516" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A516" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B516" s="18" t="s">
+        <v>576</v>
+      </c>
+      <c r="C516" s="19" t="s">
+        <v>618</v>
+      </c>
+      <c r="D516" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.COMPLETION_SCORE_PCT IS 'InPort Completion Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="517" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A517" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B517" s="18" t="s">
+        <v>577</v>
+      </c>
+      <c r="C517" s="19" t="s">
+        <v>619</v>
+      </c>
+      <c r="D517" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_COMPLETION_SCORE_PCT IS 'Formatted InPort Completion Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="518" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A518" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B518" s="18" t="s">
+        <v>578</v>
+      </c>
+      <c r="C518" s="19" t="s">
+        <v>620</v>
+      </c>
+      <c r="D518" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.IDENTIFICATION_SCORE IS 'InPort Identification Score (NMFS_INP_RBR_DS_SCORES.IDENTIFICATION_SCORE)';</v>
+      </c>
+    </row>
+    <row r="519" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A519" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B519" s="18" t="s">
+        <v>579</v>
+      </c>
+      <c r="C519" s="19" t="s">
+        <v>621</v>
+      </c>
+      <c r="D519" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.IDENTIFICATION_SCORE_PCT IS 'InPort Identification Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="520" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A520" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B520" s="18" t="s">
+        <v>580</v>
+      </c>
+      <c r="C520" s="19" t="s">
+        <v>622</v>
+      </c>
+      <c r="D520" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_IDENTIFICATION_SCORE_PCT IS 'Formatted InPort Identification Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="521" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A521" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B521" s="18" t="s">
+        <v>581</v>
+      </c>
+      <c r="C521" s="19" t="s">
+        <v>623</v>
+      </c>
+      <c r="D521" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.ACCESS_SCORE IS 'InPort Access Score (NMFS_INP_RBR_DS_SCORES.ACCESS_SCORE)';</v>
+      </c>
+    </row>
+    <row r="522" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A522" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B522" s="18" t="s">
+        <v>582</v>
+      </c>
+      <c r="C522" s="19" t="s">
+        <v>624</v>
+      </c>
+      <c r="D522" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.ACCESS_SCORE_PCT IS 'InPort Access Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="523" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A523" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B523" s="18" t="s">
+        <v>583</v>
+      </c>
+      <c r="C523" s="19" t="s">
+        <v>625</v>
+      </c>
+      <c r="D523" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_ACCESS_SCORE_PCT IS 'Formatted InPort Access Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="524" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A524" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B524" s="18" t="s">
+        <v>584</v>
+      </c>
+      <c r="C524" s="19" t="s">
+        <v>626</v>
+      </c>
+      <c r="D524" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.COVERAGE_SCORE IS 'InPort Coverage Score (NMFS_INP_RBR_DS_SCORES.COVERAGE_SCORE)';</v>
+      </c>
+    </row>
+    <row r="525" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A525" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B525" s="18" t="s">
+        <v>585</v>
+      </c>
+      <c r="C525" s="19" t="s">
+        <v>627</v>
+      </c>
+      <c r="D525" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.COVERAGE_SCORE_PCT IS 'InPort Coverage Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="526" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A526" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B526" s="18" t="s">
+        <v>586</v>
+      </c>
+      <c r="C526" s="19" t="s">
+        <v>628</v>
+      </c>
+      <c r="D526" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_COVERAGE_SCORE_PCT IS 'Formatted InPort Coverage Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="527" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A527" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B527" s="18" t="s">
+        <v>587</v>
+      </c>
+      <c r="C527" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="D527" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.CONTENT_SCORE IS 'InPort Content Score (NMFS_INP_RBR_DS_SCORES.CONTENT_SCORE)';</v>
+      </c>
+    </row>
+    <row r="528" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A528" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B528" s="18" t="s">
+        <v>588</v>
+      </c>
+      <c r="C528" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="D528" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.CONTENT_SCORE_PCT IS 'InPort Content Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="529" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A529" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B529" s="18" t="s">
+        <v>589</v>
+      </c>
+      <c r="C529" s="19" t="s">
+        <v>631</v>
+      </c>
+      <c r="D529" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_CONTENT_SCORE_PCT IS 'Formatted InPort Content Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="530" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A530" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B530" s="18" t="s">
+        <v>590</v>
+      </c>
+      <c r="C530" s="19" t="s">
+        <v>632</v>
+      </c>
+      <c r="D530" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.HISTORY_SCORE IS 'InPort History Score (NMFS_INP_RBR_DS_SCORES.HISTORY_SCORE)';</v>
+      </c>
+    </row>
+    <row r="531" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A531" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B531" s="18" t="s">
+        <v>591</v>
+      </c>
+      <c r="C531" s="19" t="s">
+        <v>633</v>
+      </c>
+      <c r="D531" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.HISTORY_SCORE_PCT IS 'InPort History Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="532" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A532" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B532" s="18" t="s">
+        <v>592</v>
+      </c>
+      <c r="C532" s="19" t="s">
+        <v>634</v>
+      </c>
+      <c r="D532" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_HISTORY_SCORE_PCT IS 'Formatted InPort History Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="533" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A533" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B533" s="18" t="s">
+        <v>593</v>
+      </c>
+      <c r="C533" s="19" t="s">
+        <v>635</v>
+      </c>
+      <c r="D533" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.QUALITY_SCORE IS 'InPort Quality Score (NMFS_INP_RBR_DS_SCORES.QUALITY_SCORE)';</v>
+      </c>
+    </row>
+    <row r="534" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A534" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B534" s="18" t="s">
+        <v>594</v>
+      </c>
+      <c r="C534" s="19" t="s">
+        <v>636</v>
+      </c>
+      <c r="D534" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.QUALITY_SCORE_PCT IS 'InPort Quality Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="535" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A535" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B535" s="18" t="s">
+        <v>595</v>
+      </c>
+      <c r="C535" s="19" t="s">
+        <v>637</v>
+      </c>
+      <c r="D535" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_QUALITY_SCORE_PCT IS 'Formatted InPort Quality Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="536" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A536" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B536" s="18" t="s">
+        <v>596</v>
+      </c>
+      <c r="C536" s="19" t="s">
+        <v>638</v>
+      </c>
+      <c r="D536" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.CONNECTION_SCORE IS 'InPort Connection Score (NMFS_INP_RBR_DS_SCORES.CONNECTION_SCORE)';</v>
+      </c>
+    </row>
+    <row r="537" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A537" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B537" s="18" t="s">
+        <v>597</v>
+      </c>
+      <c r="C537" s="19" t="s">
+        <v>639</v>
+      </c>
+      <c r="D537" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.CONNECTION_SCORE_PCT IS 'InPort Connection Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="538" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A538" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B538" s="18" t="s">
+        <v>598</v>
+      </c>
+      <c r="C538" s="19" t="s">
+        <v>640</v>
+      </c>
+      <c r="D538" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_CONNECTION_SCORE_PCT IS 'Formatted InPort Connection Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="539" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A539" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B539" s="18" t="s">
+        <v>599</v>
+      </c>
+      <c r="C539" s="19" t="s">
+        <v>641</v>
+      </c>
+      <c r="D539" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.METADATA_SCORE IS 'InPort Metadata Score (NMFS_INP_RBR_DS_SCORES.METADATA_SCORE)';</v>
+      </c>
+    </row>
+    <row r="540" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A540" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B540" s="18" t="s">
+        <v>600</v>
+      </c>
+      <c r="C540" s="19" t="s">
+        <v>642</v>
+      </c>
+      <c r="D540" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.METADATA_SCORE_PCT IS 'InPort Metadata Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="541" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A541" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B541" s="18" t="s">
+        <v>601</v>
+      </c>
+      <c r="C541" s="19" t="s">
+        <v>643</v>
+      </c>
+      <c r="D541" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_METADATA_SCORE_PCT IS 'Formatted InPort Metadata Score Percentage (to 2 significant digits)';</v>
+      </c>
+    </row>
+    <row r="542" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A542" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B542" s="18" t="s">
+        <v>602</v>
+      </c>
+      <c r="C542" s="19" t="s">
+        <v>644</v>
+      </c>
+      <c r="D542" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.METADATA_CONTACT IS 'Comma-delimited list of metadata contacts for the corresponding data set';</v>
+      </c>
+    </row>
+    <row r="543" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A543" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B543" s="18" t="s">
+        <v>603</v>
+      </c>
+      <c r="C543" s="19" t="s">
+        <v>645</v>
+      </c>
+      <c r="D543" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.ACCESS_WAIVER_YN IS 'Access Waiver? (NMFS_INP_CC_DATA_MANAGEMENT.ACCESS_WAIVER_YN)';</v>
+      </c>
+    </row>
+    <row r="544" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A544" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B544" s="18" t="s">
+        <v>604</v>
+      </c>
+      <c r="C544" s="19" t="s">
+        <v>646</v>
+      </c>
+      <c r="D544" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.GEO_DATA_PRES_FORM IS 'Geo Data Presentation Format (NMFS_INP_CATALOG_ITEMS.DS_GEO_DATA_PRES_FORM)';</v>
+      </c>
+    </row>
+    <row r="545" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A545" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B545" s="18" t="s">
+        <v>605</v>
+      </c>
+      <c r="C545" s="19" t="s">
+        <v>647</v>
+      </c>
+      <c r="D545" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.PUBLISHED_STATUS IS 'Published Status (NMFS_INP_CATALOG_ITEMS.PUBLISHED_STATUS)';</v>
+      </c>
     </row>
     <row r="546" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A546" s="19"/>
-      <c r="B546" s="19"/>
-      <c r="C546" s="19"/>
-      <c r="D546" s="22"/>
+      <c r="A546" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B546" s="18" t="s">
+        <v>606</v>
+      </c>
+      <c r="C546" s="19" t="s">
+        <v>648</v>
+      </c>
+      <c r="D546" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.CREATE_DTM IS 'Create Date/Time (NMFS_INP_CATALOG_ITEMS.CREATE_DTM)';</v>
+      </c>
     </row>
     <row r="547" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A547" s="19"/>
-      <c r="B547" s="19"/>
-      <c r="C547" s="19"/>
-      <c r="D547" s="22"/>
+      <c r="A547" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B547" s="18" t="s">
+        <v>607</v>
+      </c>
+      <c r="C547" s="19" t="s">
+        <v>649</v>
+      </c>
+      <c r="D547" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.LAST_MOD_DTM IS 'Modified Date/Time (NMFS_INP_CATALOG_ITEMS.LAST_MOD_DTM)';</v>
+      </c>
     </row>
     <row r="548" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A548" s="19"/>
-      <c r="B548" s="19"/>
-      <c r="C548" s="19"/>
-      <c r="D548" s="22"/>
+      <c r="A548" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B548" s="18" t="s">
+        <v>608</v>
+      </c>
+      <c r="C548" s="19" t="s">
+        <v>650</v>
+      </c>
+      <c r="D548" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.INPORT_LINK_URL IS 'Generated standard InPort data set URL based on the corresponding CAT_ID';</v>
+      </c>
     </row>
     <row r="549" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A549" s="19"/>
-      <c r="B549" s="19"/>
-      <c r="C549" s="19"/>
-      <c r="D549" s="22"/>
+      <c r="A549" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B549" s="18" t="s">
+        <v>609</v>
+      </c>
+      <c r="C549" s="19" t="s">
+        <v>651</v>
+      </c>
+      <c r="D549" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.REFRESH_DTM IS 'The Date/Time the PIR data set record was refreshed from ODS';</v>
+      </c>
     </row>
     <row r="550" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A550" s="19"/>
-      <c r="B550" s="19"/>
-      <c r="C550" s="19"/>
-      <c r="D550" s="22"/>
+      <c r="A550" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B550" s="18" t="s">
+        <v>610</v>
+      </c>
+      <c r="C550" s="19" t="s">
+        <v>652</v>
+      </c>
+      <c r="D550" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_REFRESH_DTM IS 'The Formatted Date/Time the PIR data set record was refreshed from ODS (in MM/DD/YYYY HH24:MI:SS format)';</v>
+      </c>
     </row>
     <row r="551" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A551" s="19"/>
@@ -15091,11 +16120,11 @@
       <c r="C552" s="19"/>
       <c r="D552" s="22"/>
     </row>
-    <row r="553" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A553" s="19"/>
-      <c r="B553" s="19"/>
-      <c r="C553" s="19"/>
-      <c r="D553" s="22"/>
+    <row r="557" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A557" s="19"/>
+      <c r="B557" s="19"/>
+      <c r="C557" s="19"/>
+      <c r="D557" s="22"/>
     </row>
     <row r="558" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A558" s="19"/>
@@ -15115,17 +16144,17 @@
       <c r="C560" s="19"/>
       <c r="D560" s="22"/>
     </row>
-    <row r="561" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A561" s="19"/>
-      <c r="B561" s="19"/>
-      <c r="C561" s="19"/>
-      <c r="D561" s="22"/>
-    </row>
-    <row r="563" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A563" s="19"/>
-      <c r="B563" s="19"/>
-      <c r="C563" s="19"/>
-      <c r="D563" s="22"/>
+    <row r="562" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A562" s="19"/>
+      <c r="B562" s="19"/>
+      <c r="C562" s="19"/>
+      <c r="D562" s="22"/>
+    </row>
+    <row r="565" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A565" s="19"/>
+      <c r="B565" s="19"/>
+      <c r="C565" s="19"/>
+      <c r="D565" s="22"/>
     </row>
     <row r="566" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A566" s="19"/>
@@ -15133,13 +16162,13 @@
       <c r="C566" s="19"/>
       <c r="D566" s="22"/>
     </row>
-    <row r="567" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A567" s="19"/>
-      <c r="B567" s="19"/>
-      <c r="C567" s="19"/>
-      <c r="D567" s="22"/>
-    </row>
-    <row r="593" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="592" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A592" s="19"/>
+      <c r="B592" s="19"/>
+      <c r="C592" s="19"/>
+      <c r="D592" s="22"/>
+    </row>
+    <row r="593" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A593" s="19"/>
       <c r="B593" s="19"/>
       <c r="C593" s="19"/>
@@ -15151,19 +16180,19 @@
       <c r="C594" s="19"/>
       <c r="D594" s="22"/>
     </row>
-    <row r="595" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A595" s="19"/>
       <c r="B595" s="19"/>
       <c r="C595" s="19"/>
       <c r="D595" s="22"/>
     </row>
-    <row r="596" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A596" s="19"/>
       <c r="B596" s="19"/>
       <c r="C596" s="19"/>
       <c r="D596" s="22"/>
     </row>
-    <row r="597" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A597" s="19"/>
       <c r="B597" s="19"/>
       <c r="C597" s="19"/>
@@ -15181,7 +16210,7 @@
       <c r="C599" s="19"/>
       <c r="D599" s="22"/>
     </row>
-    <row r="600" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A600" s="19"/>
       <c r="B600" s="19"/>
       <c r="C600" s="19"/>
@@ -15211,7 +16240,7 @@
       <c r="C604" s="19"/>
       <c r="D604" s="22"/>
     </row>
-    <row r="605" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="605" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A605" s="19"/>
       <c r="B605" s="19"/>
       <c r="C605" s="19"/>
@@ -15229,7 +16258,7 @@
       <c r="C607" s="19"/>
       <c r="D607" s="22"/>
     </row>
-    <row r="608" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A608" s="19"/>
       <c r="B608" s="19"/>
       <c r="C608" s="19"/>
@@ -15481,41 +16510,41 @@
       <c r="C649" s="19"/>
       <c r="D649" s="22"/>
     </row>
-    <row r="650" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="650" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A650" s="19"/>
       <c r="B650" s="19"/>
       <c r="C650" s="19"/>
       <c r="D650" s="22"/>
     </row>
-    <row r="651" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A651" s="19"/>
-      <c r="B651" s="19"/>
-      <c r="C651" s="19"/>
-      <c r="D651" s="22"/>
-    </row>
-    <row r="658" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A658" s="19"/>
-      <c r="B658" s="19"/>
-      <c r="C658" s="19"/>
-      <c r="D658" s="22"/>
-    </row>
-    <row r="670" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A670" s="19"/>
-      <c r="B670" s="19"/>
-      <c r="C670" s="19"/>
-      <c r="D670" s="22"/>
-    </row>
-    <row r="672" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A672" s="19"/>
-      <c r="B672" s="19"/>
-      <c r="C672" s="19"/>
-      <c r="D672" s="22"/>
-    </row>
-    <row r="687" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A687" s="19"/>
-      <c r="B687" s="19"/>
-      <c r="C687" s="19"/>
-      <c r="D687" s="22"/>
+    <row r="657" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A657" s="19"/>
+      <c r="B657" s="19"/>
+      <c r="C657" s="19"/>
+      <c r="D657" s="22"/>
+    </row>
+    <row r="669" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A669" s="19"/>
+      <c r="B669" s="19"/>
+      <c r="C669" s="19"/>
+      <c r="D669" s="22"/>
+    </row>
+    <row r="671" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A671" s="19"/>
+      <c r="B671" s="19"/>
+      <c r="C671" s="19"/>
+      <c r="D671" s="22"/>
+    </row>
+    <row r="686" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A686" s="19"/>
+      <c r="B686" s="19"/>
+      <c r="C686" s="19"/>
+      <c r="D686" s="22"/>
+    </row>
+    <row r="724" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A724" s="19"/>
+      <c r="B724" s="19"/>
+      <c r="C724" s="19"/>
+      <c r="D724" s="22"/>
     </row>
     <row r="725" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A725" s="19"/>
@@ -15535,11 +16564,11 @@
       <c r="C727" s="19"/>
       <c r="D727" s="22"/>
     </row>
-    <row r="728" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A728" s="19"/>
-      <c r="B728" s="19"/>
-      <c r="C728" s="19"/>
-      <c r="D728" s="22"/>
+    <row r="773" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A773" s="19"/>
+      <c r="B773" s="19"/>
+      <c r="C773" s="19"/>
+      <c r="D773" s="22"/>
     </row>
     <row r="774" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A774" s="19"/>
@@ -15553,23 +16582,23 @@
       <c r="C775" s="19"/>
       <c r="D775" s="22"/>
     </row>
-    <row r="776" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A776" s="19"/>
-      <c r="B776" s="19"/>
-      <c r="C776" s="19"/>
-      <c r="D776" s="22"/>
-    </row>
-    <row r="779" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A779" s="19"/>
-      <c r="B779" s="19"/>
-      <c r="C779" s="19"/>
-      <c r="D779" s="22"/>
-    </row>
-    <row r="781" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A781" s="19"/>
-      <c r="B781" s="19"/>
-      <c r="C781" s="19"/>
-      <c r="D781" s="22"/>
+    <row r="778" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A778" s="19"/>
+      <c r="B778" s="19"/>
+      <c r="C778" s="19"/>
+      <c r="D778" s="22"/>
+    </row>
+    <row r="780" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A780" s="19"/>
+      <c r="B780" s="19"/>
+      <c r="C780" s="19"/>
+      <c r="D780" s="22"/>
+    </row>
+    <row r="782" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A782" s="19"/>
+      <c r="B782" s="19"/>
+      <c r="C782" s="19"/>
+      <c r="D782" s="22"/>
     </row>
     <row r="783" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A783" s="19"/>
@@ -15583,23 +16612,23 @@
       <c r="C784" s="19"/>
       <c r="D784" s="22"/>
     </row>
-    <row r="785" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A785" s="19"/>
-      <c r="B785" s="19"/>
-      <c r="C785" s="19"/>
-      <c r="D785" s="22"/>
-    </row>
-    <row r="790" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A790" s="19"/>
-      <c r="B790" s="19"/>
-      <c r="C790" s="19"/>
-      <c r="D790" s="22"/>
-    </row>
-    <row r="792" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A792" s="19"/>
-      <c r="B792" s="19"/>
-      <c r="C792" s="19"/>
-      <c r="D792" s="22"/>
+    <row r="789" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A789" s="19"/>
+      <c r="B789" s="19"/>
+      <c r="C789" s="19"/>
+      <c r="D789" s="22"/>
+    </row>
+    <row r="791" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A791" s="19"/>
+      <c r="B791" s="19"/>
+      <c r="C791" s="19"/>
+      <c r="D791" s="22"/>
+    </row>
+    <row r="793" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A793" s="19"/>
+      <c r="B793" s="19"/>
+      <c r="C793" s="19"/>
+      <c r="D793" s="22"/>
     </row>
     <row r="794" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A794" s="19"/>
@@ -15607,71 +16636,71 @@
       <c r="C794" s="19"/>
       <c r="D794" s="22"/>
     </row>
-    <row r="795" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="795" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A795" s="19"/>
       <c r="B795" s="19"/>
       <c r="C795" s="19"/>
       <c r="D795" s="22"/>
     </row>
-    <row r="796" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A796" s="19"/>
-      <c r="B796" s="19"/>
-      <c r="C796" s="19"/>
-      <c r="D796" s="22"/>
-    </row>
-    <row r="801" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A801" s="19"/>
-      <c r="B801" s="19"/>
-      <c r="C801" s="19"/>
-      <c r="D801" s="22"/>
-    </row>
-    <row r="803" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A803" s="19"/>
-      <c r="B803" s="19"/>
-      <c r="C803" s="19"/>
-      <c r="D803" s="22"/>
-    </row>
-    <row r="805" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="800" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A800" s="19"/>
+      <c r="B800" s="19"/>
+      <c r="C800" s="19"/>
+      <c r="D800" s="22"/>
+    </row>
+    <row r="802" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A802" s="19"/>
+      <c r="B802" s="19"/>
+      <c r="C802" s="19"/>
+      <c r="D802" s="22"/>
+    </row>
+    <row r="804" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A804" s="19"/>
+      <c r="B804" s="19"/>
+      <c r="C804" s="19"/>
+      <c r="D804" s="22"/>
+    </row>
+    <row r="805" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A805" s="19"/>
       <c r="B805" s="19"/>
       <c r="C805" s="19"/>
       <c r="D805" s="22"/>
     </row>
-    <row r="806" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="806" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A806" s="19"/>
       <c r="B806" s="19"/>
       <c r="C806" s="19"/>
       <c r="D806" s="22"/>
     </row>
-    <row r="807" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A807" s="19"/>
-      <c r="B807" s="19"/>
-      <c r="C807" s="19"/>
-      <c r="D807" s="22"/>
-    </row>
-    <row r="813" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A813" s="19"/>
-      <c r="B813" s="19"/>
-      <c r="C813" s="19"/>
-      <c r="D813" s="22"/>
-    </row>
-    <row r="819" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A819" s="19"/>
-      <c r="B819" s="19"/>
-      <c r="C819" s="19"/>
-      <c r="D819" s="22"/>
-    </row>
-    <row r="826" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A826" s="19"/>
-      <c r="B826" s="19"/>
-      <c r="C826" s="19"/>
-      <c r="D826" s="22"/>
-    </row>
-    <row r="828" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A828" s="19"/>
-      <c r="B828" s="19"/>
-      <c r="C828" s="19"/>
-      <c r="D828" s="22"/>
+    <row r="812" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A812" s="19"/>
+      <c r="B812" s="19"/>
+      <c r="C812" s="19"/>
+      <c r="D812" s="22"/>
+    </row>
+    <row r="818" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A818" s="19"/>
+      <c r="B818" s="19"/>
+      <c r="C818" s="19"/>
+      <c r="D818" s="22"/>
+    </row>
+    <row r="825" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A825" s="19"/>
+      <c r="B825" s="19"/>
+      <c r="C825" s="19"/>
+      <c r="D825" s="22"/>
+    </row>
+    <row r="827" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A827" s="19"/>
+      <c r="B827" s="19"/>
+      <c r="C827" s="19"/>
+      <c r="D827" s="22"/>
+    </row>
+    <row r="830" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A830" s="19"/>
+      <c r="B830" s="19"/>
+      <c r="C830" s="19"/>
+      <c r="D830" s="22"/>
     </row>
     <row r="831" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A831" s="19"/>
@@ -15685,7 +16714,7 @@
       <c r="C832" s="19"/>
       <c r="D832" s="22"/>
     </row>
-    <row r="833" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="833" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A833" s="19"/>
       <c r="B833" s="19"/>
       <c r="C833" s="19"/>
@@ -15697,77 +16726,77 @@
       <c r="C834" s="19"/>
       <c r="D834" s="22"/>
     </row>
-    <row r="835" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A835" s="19"/>
-      <c r="B835" s="19"/>
-      <c r="C835" s="19"/>
-      <c r="D835" s="22"/>
-    </row>
-    <row r="838" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A838" s="19"/>
-      <c r="B838" s="19"/>
-      <c r="C838" s="19"/>
-      <c r="D838" s="22"/>
-    </row>
-    <row r="843" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A843" s="19"/>
-      <c r="B843" s="19"/>
-      <c r="C843" s="19"/>
-      <c r="D843" s="22"/>
-    </row>
-    <row r="851" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A851" s="19"/>
-      <c r="B851" s="19"/>
-      <c r="C851" s="19"/>
-      <c r="D851" s="22"/>
-    </row>
-    <row r="854" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A854" s="19"/>
-      <c r="B854" s="19"/>
-      <c r="C854" s="19"/>
-      <c r="D854" s="22"/>
-    </row>
-    <row r="859" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A859" s="19"/>
-      <c r="B859" s="19"/>
-      <c r="C859" s="19"/>
-      <c r="D859" s="22"/>
-    </row>
-    <row r="862" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A862" s="19"/>
-      <c r="B862" s="19"/>
-      <c r="C862" s="19"/>
-      <c r="D862" s="22"/>
-    </row>
-    <row r="868" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A868" s="19"/>
-      <c r="B868" s="19"/>
-      <c r="C868" s="19"/>
-      <c r="D868" s="22"/>
-    </row>
-    <row r="872" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A872" s="19"/>
-      <c r="B872" s="19"/>
-      <c r="C872" s="19"/>
-      <c r="D872" s="22"/>
-    </row>
-    <row r="879" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A879" s="19"/>
-      <c r="B879" s="19"/>
-      <c r="C879" s="19"/>
-      <c r="D879" s="22"/>
-    </row>
-    <row r="881" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A881" s="19"/>
-      <c r="B881" s="19"/>
-      <c r="C881" s="19"/>
-      <c r="D881" s="22"/>
-    </row>
-    <row r="890" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A890" s="19"/>
-      <c r="B890" s="19"/>
-      <c r="C890" s="19"/>
-      <c r="D890" s="22"/>
+    <row r="837" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A837" s="19"/>
+      <c r="B837" s="19"/>
+      <c r="C837" s="19"/>
+      <c r="D837" s="22"/>
+    </row>
+    <row r="842" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A842" s="19"/>
+      <c r="B842" s="19"/>
+      <c r="C842" s="19"/>
+      <c r="D842" s="22"/>
+    </row>
+    <row r="850" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A850" s="19"/>
+      <c r="B850" s="19"/>
+      <c r="C850" s="19"/>
+      <c r="D850" s="22"/>
+    </row>
+    <row r="853" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A853" s="19"/>
+      <c r="B853" s="19"/>
+      <c r="C853" s="19"/>
+      <c r="D853" s="22"/>
+    </row>
+    <row r="858" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A858" s="19"/>
+      <c r="B858" s="19"/>
+      <c r="C858" s="19"/>
+      <c r="D858" s="22"/>
+    </row>
+    <row r="861" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A861" s="19"/>
+      <c r="B861" s="19"/>
+      <c r="C861" s="19"/>
+      <c r="D861" s="22"/>
+    </row>
+    <row r="867" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A867" s="19"/>
+      <c r="B867" s="19"/>
+      <c r="C867" s="19"/>
+      <c r="D867" s="22"/>
+    </row>
+    <row r="871" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A871" s="19"/>
+      <c r="B871" s="19"/>
+      <c r="C871" s="19"/>
+      <c r="D871" s="22"/>
+    </row>
+    <row r="878" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A878" s="19"/>
+      <c r="B878" s="19"/>
+      <c r="C878" s="19"/>
+      <c r="D878" s="22"/>
+    </row>
+    <row r="880" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A880" s="19"/>
+      <c r="B880" s="19"/>
+      <c r="C880" s="19"/>
+      <c r="D880" s="22"/>
+    </row>
+    <row r="889" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A889" s="19"/>
+      <c r="B889" s="19"/>
+      <c r="C889" s="19"/>
+      <c r="D889" s="22"/>
+    </row>
+    <row r="894" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A894" s="19"/>
+      <c r="B894" s="19"/>
+      <c r="C894" s="19"/>
+      <c r="D894" s="22"/>
     </row>
     <row r="895" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A895" s="19"/>
@@ -15775,17 +16804,17 @@
       <c r="C895" s="19"/>
       <c r="D895" s="22"/>
     </row>
-    <row r="896" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A896" s="19"/>
-      <c r="B896" s="19"/>
-      <c r="C896" s="19"/>
-      <c r="D896" s="22"/>
-    </row>
-    <row r="905" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A905" s="19"/>
-      <c r="B905" s="19"/>
-      <c r="C905" s="19"/>
-      <c r="D905" s="22"/>
+    <row r="904" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A904" s="19"/>
+      <c r="B904" s="19"/>
+      <c r="C904" s="19"/>
+      <c r="D904" s="22"/>
+    </row>
+    <row r="906" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A906" s="19"/>
+      <c r="B906" s="19"/>
+      <c r="C906" s="19"/>
+      <c r="D906" s="22"/>
     </row>
     <row r="907" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A907" s="19"/>
@@ -15793,11 +16822,11 @@
       <c r="C907" s="19"/>
       <c r="D907" s="22"/>
     </row>
-    <row r="908" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A908" s="19"/>
-      <c r="B908" s="19"/>
-      <c r="C908" s="19"/>
-      <c r="D908" s="22"/>
+    <row r="909" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A909" s="19"/>
+      <c r="B909" s="19"/>
+      <c r="C909" s="19"/>
+      <c r="D909" s="22"/>
     </row>
     <row r="910" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A910" s="19"/>
@@ -15811,11 +16840,11 @@
       <c r="C911" s="19"/>
       <c r="D911" s="22"/>
     </row>
-    <row r="912" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A912" s="19"/>
-      <c r="B912" s="19"/>
-      <c r="C912" s="19"/>
-      <c r="D912" s="22"/>
+    <row r="916" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A916" s="19"/>
+      <c r="B916" s="19"/>
+      <c r="C916" s="19"/>
+      <c r="D916" s="22"/>
     </row>
     <row r="917" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A917" s="19"/>
@@ -15829,13 +16858,13 @@
       <c r="C918" s="19"/>
       <c r="D918" s="22"/>
     </row>
-    <row r="919" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A919" s="19"/>
-      <c r="B919" s="19"/>
-      <c r="C919" s="19"/>
-      <c r="D919" s="22"/>
-    </row>
-    <row r="922" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A921" s="19"/>
+      <c r="B921" s="19"/>
+      <c r="C921" s="19"/>
+      <c r="D921" s="22"/>
+    </row>
+    <row r="922" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A922" s="19"/>
       <c r="B922" s="19"/>
       <c r="C922" s="19"/>
@@ -15865,7 +16894,7 @@
       <c r="C926" s="19"/>
       <c r="D926" s="22"/>
     </row>
-    <row r="927" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="927" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A927" s="19"/>
       <c r="B927" s="19"/>
       <c r="C927" s="19"/>
@@ -15883,23 +16912,23 @@
       <c r="C929" s="19"/>
       <c r="D929" s="22"/>
     </row>
-    <row r="930" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="930" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A930" s="19"/>
       <c r="B930" s="19"/>
       <c r="C930" s="19"/>
       <c r="D930" s="22"/>
     </row>
-    <row r="931" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A931" s="19"/>
-      <c r="B931" s="19"/>
-      <c r="C931" s="19"/>
-      <c r="D931" s="22"/>
-    </row>
-    <row r="945" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A945" s="19"/>
-      <c r="B945" s="19"/>
-      <c r="C945" s="19"/>
-      <c r="D945" s="22"/>
+    <row r="944" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A944" s="19"/>
+      <c r="B944" s="19"/>
+      <c r="C944" s="19"/>
+      <c r="D944" s="22"/>
+    </row>
+    <row r="951" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A951" s="19"/>
+      <c r="B951" s="19"/>
+      <c r="C951" s="19"/>
+      <c r="D951" s="22"/>
     </row>
     <row r="952" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A952" s="19"/>
@@ -15907,17 +16936,17 @@
       <c r="C952" s="19"/>
       <c r="D952" s="22"/>
     </row>
-    <row r="953" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A953" s="19"/>
-      <c r="B953" s="19"/>
-      <c r="C953" s="19"/>
-      <c r="D953" s="22"/>
-    </row>
-    <row r="955" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A955" s="19"/>
-      <c r="B955" s="19"/>
-      <c r="C955" s="19"/>
-      <c r="D955" s="22"/>
+    <row r="954" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A954" s="19"/>
+      <c r="B954" s="19"/>
+      <c r="C954" s="19"/>
+      <c r="D954" s="22"/>
+    </row>
+    <row r="960" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A960" s="19"/>
+      <c r="B960" s="19"/>
+      <c r="C960" s="19"/>
+      <c r="D960" s="22"/>
     </row>
     <row r="961" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A961" s="19"/>
@@ -15925,11 +16954,11 @@
       <c r="C961" s="19"/>
       <c r="D961" s="22"/>
     </row>
-    <row r="962" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A962" s="19"/>
-      <c r="B962" s="19"/>
-      <c r="C962" s="19"/>
-      <c r="D962" s="22"/>
+    <row r="967" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A967" s="19"/>
+      <c r="B967" s="19"/>
+      <c r="C967" s="19"/>
+      <c r="D967" s="22"/>
     </row>
     <row r="968" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A968" s="19"/>
@@ -15937,11 +16966,11 @@
       <c r="C968" s="19"/>
       <c r="D968" s="22"/>
     </row>
-    <row r="969" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A969" s="19"/>
-      <c r="B969" s="19"/>
-      <c r="C969" s="19"/>
-      <c r="D969" s="22"/>
+    <row r="978" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A978" s="19"/>
+      <c r="B978" s="19"/>
+      <c r="C978" s="19"/>
+      <c r="D978" s="22"/>
     </row>
     <row r="979" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A979" s="19"/>
@@ -15949,23 +16978,23 @@
       <c r="C979" s="19"/>
       <c r="D979" s="22"/>
     </row>
-    <row r="980" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A980" s="19"/>
-      <c r="B980" s="19"/>
-      <c r="C980" s="19"/>
-      <c r="D980" s="22"/>
-    </row>
-    <row r="990" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A990" s="19"/>
-      <c r="B990" s="19"/>
-      <c r="C990" s="19"/>
-      <c r="D990" s="22"/>
-    </row>
-    <row r="997" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A997" s="19"/>
-      <c r="B997" s="19"/>
-      <c r="C997" s="19"/>
-      <c r="D997" s="22"/>
+    <row r="989" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A989" s="19"/>
+      <c r="B989" s="19"/>
+      <c r="C989" s="19"/>
+      <c r="D989" s="22"/>
+    </row>
+    <row r="996" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A996" s="19"/>
+      <c r="B996" s="19"/>
+      <c r="C996" s="19"/>
+      <c r="D996" s="22"/>
+    </row>
+    <row r="1015" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1015" s="19"/>
+      <c r="B1015" s="19"/>
+      <c r="C1015" s="19"/>
+      <c r="D1015" s="22"/>
     </row>
     <row r="1016" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1016" s="19"/>
@@ -15985,7 +17014,7 @@
       <c r="C1018" s="19"/>
       <c r="D1018" s="22"/>
     </row>
-    <row r="1019" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1019" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1019" s="19"/>
       <c r="B1019" s="19"/>
       <c r="C1019" s="19"/>
@@ -16003,23 +17032,23 @@
       <c r="C1021" s="19"/>
       <c r="D1021" s="22"/>
     </row>
-    <row r="1022" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1022" s="19"/>
-      <c r="B1022" s="19"/>
-      <c r="C1022" s="19"/>
-      <c r="D1022" s="22"/>
-    </row>
-    <row r="1024" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1024" s="19"/>
-      <c r="B1024" s="19"/>
-      <c r="C1024" s="19"/>
-      <c r="D1024" s="22"/>
-    </row>
-    <row r="1037" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1037" s="19"/>
-      <c r="B1037" s="19"/>
-      <c r="C1037" s="19"/>
-      <c r="D1037" s="22"/>
+    <row r="1023" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1023" s="19"/>
+      <c r="B1023" s="19"/>
+      <c r="C1023" s="19"/>
+      <c r="D1023" s="22"/>
+    </row>
+    <row r="1036" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1036" s="19"/>
+      <c r="B1036" s="19"/>
+      <c r="C1036" s="19"/>
+      <c r="D1036" s="22"/>
+    </row>
+    <row r="1043" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1043" s="19"/>
+      <c r="B1043" s="19"/>
+      <c r="C1043" s="19"/>
+      <c r="D1043" s="22"/>
     </row>
     <row r="1044" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1044" s="19"/>
@@ -16027,7 +17056,7 @@
       <c r="C1044" s="19"/>
       <c r="D1044" s="22"/>
     </row>
-    <row r="1045" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1045" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1045" s="19"/>
       <c r="B1045" s="19"/>
       <c r="C1045" s="19"/>
@@ -16045,35 +17074,35 @@
       <c r="C1047" s="19"/>
       <c r="D1047" s="22"/>
     </row>
-    <row r="1048" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1048" s="19"/>
-      <c r="B1048" s="19"/>
-      <c r="C1048" s="19"/>
-      <c r="D1048" s="22"/>
-    </row>
-    <row r="1050" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1050" s="19"/>
-      <c r="B1050" s="19"/>
-      <c r="C1050" s="19"/>
-      <c r="D1050" s="22"/>
-    </row>
-    <row r="1052" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1052" s="19"/>
-      <c r="B1052" s="19"/>
-      <c r="C1052" s="19"/>
-      <c r="D1052" s="22"/>
-    </row>
-    <row r="1059" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1059" s="19"/>
-      <c r="B1059" s="19"/>
-      <c r="C1059" s="19"/>
-      <c r="D1059" s="22"/>
-    </row>
-    <row r="1064" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1064" s="19"/>
-      <c r="B1064" s="19"/>
-      <c r="C1064" s="19"/>
-      <c r="D1064" s="22"/>
+    <row r="1049" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1049" s="19"/>
+      <c r="B1049" s="19"/>
+      <c r="C1049" s="19"/>
+      <c r="D1049" s="22"/>
+    </row>
+    <row r="1051" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1051" s="19"/>
+      <c r="B1051" s="19"/>
+      <c r="C1051" s="19"/>
+      <c r="D1051" s="22"/>
+    </row>
+    <row r="1058" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1058" s="19"/>
+      <c r="B1058" s="19"/>
+      <c r="C1058" s="19"/>
+      <c r="D1058" s="22"/>
+    </row>
+    <row r="1063" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1063" s="19"/>
+      <c r="B1063" s="19"/>
+      <c r="C1063" s="19"/>
+      <c r="D1063" s="22"/>
+    </row>
+    <row r="1065" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1065" s="19"/>
+      <c r="B1065" s="19"/>
+      <c r="C1065" s="19"/>
+      <c r="D1065" s="22"/>
     </row>
     <row r="1066" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1066" s="19"/>
@@ -16087,11 +17116,11 @@
       <c r="C1067" s="19"/>
       <c r="D1067" s="22"/>
     </row>
-    <row r="1068" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1068" s="19"/>
-      <c r="B1068" s="19"/>
-      <c r="C1068" s="19"/>
-      <c r="D1068" s="22"/>
+    <row r="1070" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1070" s="19"/>
+      <c r="B1070" s="19"/>
+      <c r="C1070" s="19"/>
+      <c r="D1070" s="22"/>
     </row>
     <row r="1071" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1071" s="19"/>
@@ -16099,7 +17128,7 @@
       <c r="C1071" s="19"/>
       <c r="D1071" s="22"/>
     </row>
-    <row r="1072" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1072" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1072" s="19"/>
       <c r="B1072" s="19"/>
       <c r="C1072" s="19"/>
@@ -16135,7 +17164,7 @@
       <c r="C1077" s="19"/>
       <c r="D1077" s="22"/>
     </row>
-    <row r="1078" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1078" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1078" s="19"/>
       <c r="B1078" s="19"/>
       <c r="C1078" s="19"/>
@@ -16303,13 +17332,13 @@
       <c r="C1105" s="19"/>
       <c r="D1105" s="22"/>
     </row>
-    <row r="1106" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1106" s="19"/>
-      <c r="B1106" s="19"/>
-      <c r="C1106" s="19"/>
-      <c r="D1106" s="22"/>
-    </row>
-    <row r="1124" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1123" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1123" s="19"/>
+      <c r="B1123" s="19"/>
+      <c r="C1123" s="19"/>
+      <c r="D1123" s="22"/>
+    </row>
+    <row r="1124" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1124" s="19"/>
       <c r="B1124" s="19"/>
       <c r="C1124" s="19"/>
@@ -16339,37 +17368,37 @@
       <c r="C1128" s="19"/>
       <c r="D1128" s="22"/>
     </row>
-    <row r="1129" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1129" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1129" s="19"/>
       <c r="B1129" s="19"/>
       <c r="C1129" s="19"/>
       <c r="D1129" s="22"/>
     </row>
-    <row r="1130" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1130" s="19"/>
-      <c r="B1130" s="19"/>
-      <c r="C1130" s="19"/>
-      <c r="D1130" s="22"/>
-    </row>
-    <row r="1148" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1148" s="19"/>
-      <c r="B1148" s="19"/>
-      <c r="C1148" s="19"/>
-      <c r="D1148" s="22"/>
-    </row>
-    <row r="1150" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1150" s="19"/>
-      <c r="B1150" s="19"/>
-      <c r="C1150" s="19"/>
-      <c r="D1150" s="22"/>
-    </row>
-    <row r="1154" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1147" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1147" s="19"/>
+      <c r="B1147" s="19"/>
+      <c r="C1147" s="19"/>
+      <c r="D1147" s="22"/>
+    </row>
+    <row r="1149" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1149" s="19"/>
+      <c r="B1149" s="19"/>
+      <c r="C1149" s="19"/>
+      <c r="D1149" s="22"/>
+    </row>
+    <row r="1153" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1153" s="19"/>
+      <c r="B1153" s="19"/>
+      <c r="C1153" s="19"/>
+      <c r="D1153" s="22"/>
+    </row>
+    <row r="1154" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1154" s="19"/>
       <c r="B1154" s="19"/>
       <c r="C1154" s="19"/>
       <c r="D1154" s="22"/>
     </row>
-    <row r="1155" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1155" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1155" s="19"/>
       <c r="B1155" s="19"/>
       <c r="C1155" s="19"/>
@@ -16381,7 +17410,7 @@
       <c r="C1156" s="19"/>
       <c r="D1156" s="22"/>
     </row>
-    <row r="1157" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1157" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1157" s="19"/>
       <c r="B1157" s="19"/>
       <c r="C1157" s="19"/>
@@ -16507,11 +17536,11 @@
       <c r="C1177" s="19"/>
       <c r="D1177" s="22"/>
     </row>
-    <row r="1178" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1178" s="19"/>
-      <c r="B1178" s="19"/>
-      <c r="C1178" s="19"/>
-      <c r="D1178" s="22"/>
+    <row r="1187" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1187" s="19"/>
+      <c r="B1187" s="19"/>
+      <c r="C1187" s="19"/>
+      <c r="D1187" s="22"/>
     </row>
     <row r="1188" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1188" s="19"/>
@@ -16537,29 +17566,29 @@
       <c r="C1191" s="19"/>
       <c r="D1191" s="22"/>
     </row>
-    <row r="1192" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1192" s="19"/>
-      <c r="B1192" s="19"/>
-      <c r="C1192" s="19"/>
-      <c r="D1192" s="22"/>
-    </row>
-    <row r="1228" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1228" s="19"/>
-      <c r="B1228" s="19"/>
-      <c r="C1228" s="19"/>
-      <c r="D1228" s="22"/>
-    </row>
-    <row r="1241" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1241" s="19"/>
-      <c r="B1241" s="19"/>
-      <c r="C1241" s="19"/>
-      <c r="D1241" s="22"/>
-    </row>
-    <row r="1244" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1244" s="19"/>
-      <c r="B1244" s="19"/>
-      <c r="C1244" s="19"/>
-      <c r="D1244" s="22"/>
+    <row r="1227" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1227" s="19"/>
+      <c r="B1227" s="19"/>
+      <c r="C1227" s="19"/>
+      <c r="D1227" s="22"/>
+    </row>
+    <row r="1240" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1240" s="19"/>
+      <c r="B1240" s="19"/>
+      <c r="C1240" s="19"/>
+      <c r="D1240" s="22"/>
+    </row>
+    <row r="1243" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1243" s="19"/>
+      <c r="B1243" s="19"/>
+      <c r="C1243" s="19"/>
+      <c r="D1243" s="22"/>
+    </row>
+    <row r="1264" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1264" s="19"/>
+      <c r="B1264" s="19"/>
+      <c r="C1264" s="19"/>
+      <c r="D1264" s="22"/>
     </row>
     <row r="1265" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1265" s="19"/>
@@ -16585,11 +17614,11 @@
       <c r="C1268" s="19"/>
       <c r="D1268" s="22"/>
     </row>
-    <row r="1269" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1269" s="19"/>
-      <c r="B1269" s="19"/>
-      <c r="C1269" s="19"/>
-      <c r="D1269" s="22"/>
+    <row r="1290" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1290" s="19"/>
+      <c r="B1290" s="19"/>
+      <c r="C1290" s="19"/>
+      <c r="D1290" s="22"/>
     </row>
     <row r="1291" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1291" s="19"/>
@@ -16735,11 +17764,11 @@
       <c r="C1314" s="19"/>
       <c r="D1314" s="22"/>
     </row>
-    <row r="1315" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1315" s="19"/>
-      <c r="B1315" s="19"/>
-      <c r="C1315" s="19"/>
-      <c r="D1315" s="22"/>
+    <row r="1320" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1320" s="19"/>
+      <c r="B1320" s="19"/>
+      <c r="C1320" s="19"/>
+      <c r="D1320" s="22"/>
     </row>
     <row r="1321" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1321" s="19"/>
@@ -16747,11 +17776,11 @@
       <c r="C1321" s="19"/>
       <c r="D1321" s="22"/>
     </row>
-    <row r="1322" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1322" s="19"/>
-      <c r="B1322" s="19"/>
-      <c r="C1322" s="19"/>
-      <c r="D1322" s="22"/>
+    <row r="1336" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1336" s="19"/>
+      <c r="B1336" s="19"/>
+      <c r="C1336" s="19"/>
+      <c r="D1336" s="22"/>
     </row>
     <row r="1337" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1337" s="19"/>
@@ -16759,11 +17788,11 @@
       <c r="C1337" s="19"/>
       <c r="D1337" s="22"/>
     </row>
-    <row r="1338" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1338" s="19"/>
-      <c r="B1338" s="19"/>
-      <c r="C1338" s="19"/>
-      <c r="D1338" s="22"/>
+    <row r="1343" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1343" s="19"/>
+      <c r="B1343" s="19"/>
+      <c r="C1343" s="19"/>
+      <c r="D1343" s="22"/>
     </row>
     <row r="1344" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1344" s="19"/>
@@ -16795,47 +17824,47 @@
       <c r="C1348" s="19"/>
       <c r="D1348" s="22"/>
     </row>
-    <row r="1349" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1349" s="19"/>
-      <c r="B1349" s="19"/>
-      <c r="C1349" s="19"/>
-      <c r="D1349" s="22"/>
-    </row>
-    <row r="1355" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1354" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1354" s="19"/>
+      <c r="B1354" s="19"/>
+      <c r="C1354" s="19"/>
+      <c r="D1354" s="22"/>
+    </row>
+    <row r="1355" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1355" s="19"/>
       <c r="B1355" s="19"/>
       <c r="C1355" s="19"/>
       <c r="D1355" s="22"/>
     </row>
-    <row r="1356" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1356" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1356" s="19"/>
       <c r="B1356" s="19"/>
       <c r="C1356" s="19"/>
       <c r="D1356" s="22"/>
     </row>
-    <row r="1357" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1357" s="19"/>
-      <c r="B1357" s="19"/>
-      <c r="C1357" s="19"/>
-      <c r="D1357" s="22"/>
-    </row>
-    <row r="1361" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1360" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1360" s="19"/>
+      <c r="B1360" s="19"/>
+      <c r="C1360" s="19"/>
+      <c r="D1360" s="22"/>
+    </row>
+    <row r="1361" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1361" s="19"/>
       <c r="B1361" s="19"/>
       <c r="C1361" s="19"/>
       <c r="D1361" s="22"/>
     </row>
-    <row r="1362" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1362" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1362" s="19"/>
       <c r="B1362" s="19"/>
       <c r="C1362" s="19"/>
       <c r="D1362" s="22"/>
     </row>
-    <row r="1363" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1363" s="19"/>
-      <c r="B1363" s="19"/>
-      <c r="C1363" s="19"/>
-      <c r="D1363" s="22"/>
+    <row r="1368" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1368" s="19"/>
+      <c r="B1368" s="19"/>
+      <c r="C1368" s="19"/>
+      <c r="D1368" s="22"/>
     </row>
     <row r="1369" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="19"/>
@@ -16843,23 +17872,23 @@
       <c r="C1369" s="19"/>
       <c r="D1369" s="22"/>
     </row>
-    <row r="1370" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1370" s="19"/>
-      <c r="B1370" s="19"/>
-      <c r="C1370" s="19"/>
-      <c r="D1370" s="22"/>
-    </row>
-    <row r="1381" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1381" s="19"/>
-      <c r="B1381" s="19"/>
-      <c r="C1381" s="19"/>
-      <c r="D1381" s="22"/>
-    </row>
-    <row r="1448" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1448" s="19"/>
-      <c r="B1448" s="19"/>
-      <c r="C1448" s="19"/>
-      <c r="D1448" s="22"/>
+    <row r="1380" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1380" s="19"/>
+      <c r="B1380" s="19"/>
+      <c r="C1380" s="19"/>
+      <c r="D1380" s="22"/>
+    </row>
+    <row r="1447" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1447" s="19"/>
+      <c r="B1447" s="19"/>
+      <c r="C1447" s="19"/>
+      <c r="D1447" s="22"/>
+    </row>
+    <row r="1603" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1603" s="19"/>
+      <c r="B1603" s="19"/>
+      <c r="C1603" s="19"/>
+      <c r="D1603" s="22"/>
     </row>
     <row r="1604" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1604" s="19"/>
@@ -16867,37 +17896,37 @@
       <c r="C1604" s="19"/>
       <c r="D1604" s="22"/>
     </row>
-    <row r="1605" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1605" s="19"/>
-      <c r="B1605" s="19"/>
-      <c r="C1605" s="19"/>
-      <c r="D1605" s="22"/>
-    </row>
-    <row r="1651" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1651" s="19"/>
-      <c r="B1651" s="19"/>
-      <c r="C1651" s="19"/>
-      <c r="D1651" s="22"/>
-    </row>
-    <row r="1654" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1654" s="19"/>
-      <c r="B1654" s="19"/>
-      <c r="C1654" s="19"/>
-      <c r="D1654" s="22"/>
-    </row>
-    <row r="1660" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1660" s="19"/>
-      <c r="B1660" s="19"/>
-      <c r="C1660" s="19"/>
-      <c r="D1660" s="22"/>
-    </row>
-    <row r="1662" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1650" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1650" s="19"/>
+      <c r="B1650" s="19"/>
+      <c r="C1650" s="19"/>
+      <c r="D1650" s="22"/>
+    </row>
+    <row r="1653" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1653" s="19"/>
+      <c r="B1653" s="19"/>
+      <c r="C1653" s="19"/>
+      <c r="D1653" s="22"/>
+    </row>
+    <row r="1659" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1659" s="19"/>
+      <c r="B1659" s="19"/>
+      <c r="C1659" s="19"/>
+      <c r="D1659" s="22"/>
+    </row>
+    <row r="1661" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1661" s="19"/>
+      <c r="B1661" s="19"/>
+      <c r="C1661" s="19"/>
+      <c r="D1661" s="22"/>
+    </row>
+    <row r="1662" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1662" s="19"/>
       <c r="B1662" s="19"/>
       <c r="C1662" s="19"/>
       <c r="D1662" s="22"/>
     </row>
-    <row r="1663" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1663" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1663" s="19"/>
       <c r="B1663" s="19"/>
       <c r="C1663" s="19"/>
@@ -16909,23 +17938,23 @@
       <c r="C1664" s="19"/>
       <c r="D1664" s="22"/>
     </row>
-    <row r="1665" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1665" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1665" s="19"/>
       <c r="B1665" s="19"/>
       <c r="C1665" s="19"/>
       <c r="D1665" s="22"/>
     </row>
-    <row r="1666" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1666" s="19"/>
-      <c r="B1666" s="19"/>
-      <c r="C1666" s="19"/>
-      <c r="D1666" s="22"/>
-    </row>
-    <row r="1677" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1677" s="19"/>
-      <c r="B1677" s="19"/>
-      <c r="C1677" s="19"/>
-      <c r="D1677" s="22"/>
+    <row r="1676" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1676" s="19"/>
+      <c r="B1676" s="19"/>
+      <c r="C1676" s="19"/>
+      <c r="D1676" s="22"/>
+    </row>
+    <row r="1678" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1678" s="19"/>
+      <c r="B1678" s="19"/>
+      <c r="C1678" s="19"/>
+      <c r="D1678" s="22"/>
     </row>
     <row r="1679" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1679" s="19"/>
@@ -17077,11 +18106,11 @@
       <c r="C1703" s="19"/>
       <c r="D1703" s="22"/>
     </row>
-    <row r="1704" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1704" s="19"/>
-      <c r="B1704" s="19"/>
-      <c r="C1704" s="19"/>
-      <c r="D1704" s="22"/>
+    <row r="1762" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1762" s="19"/>
+      <c r="B1762" s="19"/>
+      <c r="C1762" s="19"/>
+      <c r="D1762" s="22"/>
     </row>
     <row r="1763" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1763" s="19"/>
@@ -17089,17 +18118,17 @@
       <c r="C1763" s="19"/>
       <c r="D1763" s="22"/>
     </row>
-    <row r="1764" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1764" s="19"/>
-      <c r="B1764" s="19"/>
-      <c r="C1764" s="19"/>
-      <c r="D1764" s="22"/>
-    </row>
-    <row r="2092" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2092" s="19"/>
-      <c r="B2092" s="19"/>
-      <c r="C2092" s="19"/>
-      <c r="D2092" s="22"/>
+    <row r="2091" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2091" s="19"/>
+      <c r="B2091" s="19"/>
+      <c r="C2091" s="19"/>
+      <c r="D2091" s="22"/>
+    </row>
+    <row r="2235" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2235" s="19"/>
+      <c r="B2235" s="19"/>
+      <c r="C2235" s="19"/>
+      <c r="D2235" s="22"/>
     </row>
     <row r="2236" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2236" s="19"/>
@@ -17197,47 +18226,47 @@
       <c r="C2251" s="19"/>
       <c r="D2251" s="22"/>
     </row>
-    <row r="2252" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2252" s="19"/>
-      <c r="B2252" s="19"/>
-      <c r="C2252" s="19"/>
-      <c r="D2252" s="22"/>
-    </row>
-    <row r="2259" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2259" s="19"/>
-      <c r="B2259" s="19"/>
-      <c r="C2259" s="19"/>
-      <c r="D2259" s="22"/>
-    </row>
-    <row r="2420" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2258" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2258" s="19"/>
+      <c r="B2258" s="19"/>
+      <c r="C2258" s="19"/>
+      <c r="D2258" s="22"/>
+    </row>
+    <row r="2419" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2419" s="19"/>
+      <c r="B2419" s="19"/>
+      <c r="C2419" s="19"/>
+      <c r="D2419" s="22"/>
+    </row>
+    <row r="2420" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2420" s="19"/>
       <c r="B2420" s="19"/>
       <c r="C2420" s="19"/>
       <c r="D2420" s="22"/>
     </row>
-    <row r="2421" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2421" s="19"/>
-      <c r="B2421" s="19"/>
-      <c r="C2421" s="19"/>
-      <c r="D2421" s="22"/>
-    </row>
-    <row r="2426" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2426" s="19"/>
-      <c r="B2426" s="19"/>
-      <c r="C2426" s="19"/>
-      <c r="D2426" s="22"/>
-    </row>
-    <row r="2520" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2520" s="19"/>
-      <c r="B2520" s="19"/>
-      <c r="C2520" s="19"/>
-      <c r="D2520" s="22"/>
-    </row>
-    <row r="2545" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2545" s="19"/>
-      <c r="B2545" s="19"/>
-      <c r="C2545" s="19"/>
-      <c r="D2545" s="22"/>
+    <row r="2425" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2425" s="19"/>
+      <c r="B2425" s="19"/>
+      <c r="C2425" s="19"/>
+      <c r="D2425" s="22"/>
+    </row>
+    <row r="2519" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2519" s="19"/>
+      <c r="B2519" s="19"/>
+      <c r="C2519" s="19"/>
+      <c r="D2519" s="22"/>
+    </row>
+    <row r="2544" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2544" s="19"/>
+      <c r="B2544" s="19"/>
+      <c r="C2544" s="19"/>
+      <c r="D2544" s="22"/>
+    </row>
+    <row r="2546" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2546" s="19"/>
+      <c r="B2546" s="19"/>
+      <c r="C2546" s="19"/>
+      <c r="D2546" s="22"/>
     </row>
     <row r="2547" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2547" s="19"/>
@@ -17245,11 +18274,11 @@
       <c r="C2547" s="19"/>
       <c r="D2547" s="22"/>
     </row>
-    <row r="2548" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2548" s="19"/>
-      <c r="B2548" s="19"/>
-      <c r="C2548" s="19"/>
-      <c r="D2548" s="22"/>
+    <row r="2549" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2549" s="19"/>
+      <c r="B2549" s="19"/>
+      <c r="C2549" s="19"/>
+      <c r="D2549" s="22"/>
     </row>
     <row r="2550" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2550" s="19"/>
@@ -17257,11 +18286,11 @@
       <c r="C2550" s="19"/>
       <c r="D2550" s="22"/>
     </row>
-    <row r="2551" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2551" s="19"/>
-      <c r="B2551" s="19"/>
-      <c r="C2551" s="19"/>
-      <c r="D2551" s="22"/>
+    <row r="2556" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2556" s="19"/>
+      <c r="B2556" s="19"/>
+      <c r="C2556" s="19"/>
+      <c r="D2556" s="22"/>
     </row>
     <row r="2557" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2557" s="19"/>
@@ -17287,17 +18316,17 @@
       <c r="C2560" s="19"/>
       <c r="D2560" s="22"/>
     </row>
-    <row r="2561" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2561" s="19"/>
-      <c r="B2561" s="19"/>
-      <c r="C2561" s="19"/>
-      <c r="D2561" s="22"/>
-    </row>
-    <row r="2570" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2570" s="19"/>
-      <c r="B2570" s="19"/>
-      <c r="C2570" s="19"/>
-      <c r="D2570" s="22"/>
+    <row r="2569" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2569" s="19"/>
+      <c r="B2569" s="19"/>
+      <c r="C2569" s="19"/>
+      <c r="D2569" s="22"/>
+    </row>
+    <row r="2571" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2571" s="19"/>
+      <c r="B2571" s="19"/>
+      <c r="C2571" s="19"/>
+      <c r="D2571" s="22"/>
     </row>
     <row r="2572" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2572" s="19"/>
@@ -17305,11 +18334,11 @@
       <c r="C2572" s="19"/>
       <c r="D2572" s="22"/>
     </row>
-    <row r="2573" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2573" s="19"/>
-      <c r="B2573" s="19"/>
-      <c r="C2573" s="19"/>
-      <c r="D2573" s="22"/>
+    <row r="2574" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2574" s="19"/>
+      <c r="B2574" s="19"/>
+      <c r="C2574" s="19"/>
+      <c r="D2574" s="22"/>
     </row>
     <row r="2575" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2575" s="19"/>
@@ -17317,11 +18346,11 @@
       <c r="C2575" s="19"/>
       <c r="D2575" s="22"/>
     </row>
-    <row r="2576" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2576" s="19"/>
-      <c r="B2576" s="19"/>
-      <c r="C2576" s="19"/>
-      <c r="D2576" s="22"/>
+    <row r="2581" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2581" s="19"/>
+      <c r="B2581" s="19"/>
+      <c r="C2581" s="19"/>
+      <c r="D2581" s="22"/>
     </row>
     <row r="2582" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2582" s="19"/>
@@ -17347,11 +18376,11 @@
       <c r="C2585" s="19"/>
       <c r="D2585" s="22"/>
     </row>
-    <row r="2586" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2586" s="19"/>
-      <c r="B2586" s="19"/>
-      <c r="C2586" s="19"/>
-      <c r="D2586" s="22"/>
+    <row r="2587" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2587" s="19"/>
+      <c r="B2587" s="19"/>
+      <c r="C2587" s="19"/>
+      <c r="D2587" s="22"/>
     </row>
     <row r="2588" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2588" s="19"/>
@@ -17365,11 +18394,11 @@
       <c r="C2589" s="19"/>
       <c r="D2589" s="22"/>
     </row>
-    <row r="2590" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2590" s="19"/>
-      <c r="B2590" s="19"/>
-      <c r="C2590" s="19"/>
-      <c r="D2590" s="22"/>
+    <row r="2604" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2604" s="19"/>
+      <c r="B2604" s="19"/>
+      <c r="C2604" s="19"/>
+      <c r="D2604" s="22"/>
     </row>
     <row r="2605" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2605" s="19"/>
@@ -17641,17 +18670,17 @@
       <c r="C2649" s="19"/>
       <c r="D2649" s="22"/>
     </row>
-    <row r="2650" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2650" s="19"/>
-      <c r="B2650" s="19"/>
-      <c r="C2650" s="19"/>
-      <c r="D2650" s="22"/>
-    </row>
-    <row r="2673" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2673" s="19"/>
-      <c r="B2673" s="19"/>
-      <c r="C2673" s="19"/>
-      <c r="D2673" s="22"/>
+    <row r="2672" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2672" s="19"/>
+      <c r="B2672" s="19"/>
+      <c r="C2672" s="19"/>
+      <c r="D2672" s="22"/>
+    </row>
+    <row r="2682" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2682" s="19"/>
+      <c r="B2682" s="19"/>
+      <c r="C2682" s="19"/>
+      <c r="D2682" s="22"/>
     </row>
     <row r="2683" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2683" s="19"/>
@@ -17659,17 +18688,17 @@
       <c r="C2683" s="19"/>
       <c r="D2683" s="22"/>
     </row>
-    <row r="2684" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2684" s="19"/>
-      <c r="B2684" s="19"/>
-      <c r="C2684" s="19"/>
-      <c r="D2684" s="22"/>
-    </row>
-    <row r="2689" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2689" s="19"/>
-      <c r="B2689" s="19"/>
-      <c r="C2689" s="19"/>
-      <c r="D2689" s="22"/>
+    <row r="2688" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2688" s="19"/>
+      <c r="B2688" s="19"/>
+      <c r="C2688" s="19"/>
+      <c r="D2688" s="22"/>
+    </row>
+    <row r="2698" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2698" s="19"/>
+      <c r="B2698" s="19"/>
+      <c r="C2698" s="19"/>
+      <c r="D2698" s="22"/>
     </row>
     <row r="2699" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2699" s="19"/>
@@ -17677,17 +18706,17 @@
       <c r="C2699" s="19"/>
       <c r="D2699" s="22"/>
     </row>
-    <row r="2700" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2700" s="19"/>
-      <c r="B2700" s="19"/>
-      <c r="C2700" s="19"/>
-      <c r="D2700" s="22"/>
-    </row>
-    <row r="2705" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2705" s="19"/>
-      <c r="B2705" s="19"/>
-      <c r="C2705" s="19"/>
-      <c r="D2705" s="22"/>
+    <row r="2704" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2704" s="19"/>
+      <c r="B2704" s="19"/>
+      <c r="C2704" s="19"/>
+      <c r="D2704" s="22"/>
+    </row>
+    <row r="2714" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2714" s="19"/>
+      <c r="B2714" s="19"/>
+      <c r="C2714" s="19"/>
+      <c r="D2714" s="22"/>
     </row>
     <row r="2715" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2715" s="19"/>
@@ -17695,35 +18724,29 @@
       <c r="C2715" s="19"/>
       <c r="D2715" s="22"/>
     </row>
-    <row r="2716" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2716" s="19"/>
-      <c r="B2716" s="19"/>
-      <c r="C2716" s="19"/>
-      <c r="D2716" s="22"/>
-    </row>
-    <row r="2735" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2735" s="19"/>
-      <c r="B2735" s="19"/>
-      <c r="C2735" s="19"/>
-      <c r="D2735" s="22"/>
-    </row>
-    <row r="2752" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2752" s="19"/>
-      <c r="B2752" s="19"/>
-      <c r="C2752" s="19"/>
-      <c r="D2752" s="22"/>
-    </row>
-    <row r="2777" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2777" s="19"/>
-      <c r="B2777" s="19"/>
-      <c r="C2777" s="19"/>
-      <c r="D2777" s="22"/>
-    </row>
-    <row r="2803" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2803" s="19"/>
-      <c r="B2803" s="19"/>
-      <c r="C2803" s="19"/>
-      <c r="D2803" s="22"/>
+    <row r="2734" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2734" s="19"/>
+      <c r="B2734" s="19"/>
+      <c r="C2734" s="19"/>
+      <c r="D2734" s="22"/>
+    </row>
+    <row r="2751" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2751" s="19"/>
+      <c r="B2751" s="19"/>
+      <c r="C2751" s="19"/>
+      <c r="D2751" s="22"/>
+    </row>
+    <row r="2776" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2776" s="19"/>
+      <c r="B2776" s="19"/>
+      <c r="C2776" s="19"/>
+      <c r="D2776" s="22"/>
+    </row>
+    <row r="2802" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2802" s="19"/>
+      <c r="B2802" s="19"/>
+      <c r="C2802" s="19"/>
+      <c r="D2802" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17852,10 +18875,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1238"/>
+  <dimension ref="A1:C1301"/>
   <sheetViews>
-    <sheetView topLeftCell="A1197" workbookViewId="0">
-      <selection activeCell="A1196" sqref="A1196:B1238"/>
+    <sheetView topLeftCell="A1263" workbookViewId="0">
+      <selection activeCell="A1246" sqref="A1246:B1301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31570,6 +32593,678 @@
       <c r="C1238" s="18" t="str">
         <f t="shared" si="24"/>
         <v xml:space="preserve">ccd_cruise_leg_v.PLAT_TYPE_DESC, </v>
+      </c>
+    </row>
+    <row r="1246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1246" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1246" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1246" s="18" t="str">
+        <f t="shared" ref="C1246:C1301" si="25">CONCATENATE(A1246, ".", B1246, ", ")</f>
+        <v xml:space="preserve">CCD_DATA_SETS_V.DATA_SET_ID, </v>
+      </c>
+    </row>
+    <row r="1247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1247" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1247" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1247" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">CCD_DATA_SETS_V.DATA_SET_NAME, </v>
+      </c>
+    </row>
+    <row r="1248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1248" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1248" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1248" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">CCD_DATA_SETS_V.DATA_SET_DESC, </v>
+      </c>
+    </row>
+    <row r="1249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1249" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1249" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1249" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">CCD_DATA_SETS_V.DATA_SET_INPORT_CAT_ID, </v>
+      </c>
+    </row>
+    <row r="1250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1250" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1250" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1250" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">CCD_DATA_SETS_V.DATA_SET_INPORT_URL, </v>
+      </c>
+    </row>
+    <row r="1251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1251" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1251" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1251" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">CCD_DATA_SETS_V.DATA_SET_TYPE_ID, </v>
+      </c>
+    </row>
+    <row r="1252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1252" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1252" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1252" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">CCD_DATA_SETS_V.DATA_SET_TYPE_NAME, </v>
+      </c>
+    </row>
+    <row r="1253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1253" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1253" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1253" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">CCD_DATA_SETS_V.DATA_SET_TYPE_DESC, </v>
+      </c>
+    </row>
+    <row r="1254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1254" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1254" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1254" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">CCD_DATA_SETS_V.DATA_SET_TYPE_DOC_URL, </v>
+      </c>
+    </row>
+    <row r="1255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1255" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1255" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1255" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">CCD_DATA_SETS_V.DATA_SET_STATUS_ID, </v>
+      </c>
+    </row>
+    <row r="1256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1256" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1256" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1256" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">CCD_DATA_SETS_V.STATUS_CODE, </v>
+      </c>
+    </row>
+    <row r="1257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1257" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1257" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1257" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">CCD_DATA_SETS_V.STATUS_NAME, </v>
+      </c>
+    </row>
+    <row r="1258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1258" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1258" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1258" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">CCD_DATA_SETS_V.STATUS_DESC, </v>
+      </c>
+    </row>
+    <row r="1259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1259" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1259" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1259" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">CCD_DATA_SETS_V.STATUS_COLOR, </v>
+      </c>
+    </row>
+    <row r="1260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1260" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1260" t="s">
+        <v>569</v>
+      </c>
+      <c r="C1260" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.METADATA_FOLDER, </v>
+      </c>
+    </row>
+    <row r="1261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1261" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1261" t="s">
+        <v>570</v>
+      </c>
+      <c r="C1261" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.ORG_ALIAS_ABBREV, </v>
+      </c>
+    </row>
+    <row r="1262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1262" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1262" t="s">
+        <v>571</v>
+      </c>
+      <c r="C1262" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.LIBRARY_ORG, </v>
+      </c>
+    </row>
+    <row r="1263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1263" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1263" t="s">
+        <v>572</v>
+      </c>
+      <c r="C1263" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.CAT_ID, </v>
+      </c>
+    </row>
+    <row r="1264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1264" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1264" t="s">
+        <v>573</v>
+      </c>
+      <c r="C1264" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.TITLE, </v>
+      </c>
+    </row>
+    <row r="1265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1265" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1265" t="s">
+        <v>574</v>
+      </c>
+      <c r="C1265" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.PARR_KEYWORDS, </v>
+      </c>
+    </row>
+    <row r="1266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1266" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1266" t="s">
+        <v>575</v>
+      </c>
+      <c r="C1266" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.COMPLETION_SCORE, </v>
+      </c>
+    </row>
+    <row r="1267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1267" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1267" t="s">
+        <v>576</v>
+      </c>
+      <c r="C1267" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.COMPLETION_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1268" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1268" t="s">
+        <v>577</v>
+      </c>
+      <c r="C1268" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.FORMAT_COMPLETION_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1269" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1269" t="s">
+        <v>578</v>
+      </c>
+      <c r="C1269" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.IDENTIFICATION_SCORE, </v>
+      </c>
+    </row>
+    <row r="1270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1270" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1270" t="s">
+        <v>579</v>
+      </c>
+      <c r="C1270" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.IDENTIFICATION_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1271" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1271" t="s">
+        <v>580</v>
+      </c>
+      <c r="C1271" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.FORMAT_IDENTIFICATION_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1272" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1272" t="s">
+        <v>581</v>
+      </c>
+      <c r="C1272" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.ACCESS_SCORE, </v>
+      </c>
+    </row>
+    <row r="1273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1273" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1273" t="s">
+        <v>582</v>
+      </c>
+      <c r="C1273" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.ACCESS_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1274" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1274" t="s">
+        <v>583</v>
+      </c>
+      <c r="C1274" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.FORMAT_ACCESS_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1275" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1275" t="s">
+        <v>584</v>
+      </c>
+      <c r="C1275" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.COVERAGE_SCORE, </v>
+      </c>
+    </row>
+    <row r="1276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1276" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1276" t="s">
+        <v>585</v>
+      </c>
+      <c r="C1276" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.COVERAGE_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1277" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1277" t="s">
+        <v>586</v>
+      </c>
+      <c r="C1277" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.FORMAT_COVERAGE_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1278" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1278" t="s">
+        <v>587</v>
+      </c>
+      <c r="C1278" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.CONTENT_SCORE, </v>
+      </c>
+    </row>
+    <row r="1279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1279" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1279" t="s">
+        <v>588</v>
+      </c>
+      <c r="C1279" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.CONTENT_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1280" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1280" t="s">
+        <v>589</v>
+      </c>
+      <c r="C1280" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.FORMAT_CONTENT_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1281" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1281" t="s">
+        <v>590</v>
+      </c>
+      <c r="C1281" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.HISTORY_SCORE, </v>
+      </c>
+    </row>
+    <row r="1282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1282" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1282" t="s">
+        <v>591</v>
+      </c>
+      <c r="C1282" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.HISTORY_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1283" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1283" t="s">
+        <v>592</v>
+      </c>
+      <c r="C1283" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.FORMAT_HISTORY_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1284" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1284" t="s">
+        <v>593</v>
+      </c>
+      <c r="C1284" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.QUALITY_SCORE, </v>
+      </c>
+    </row>
+    <row r="1285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1285" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1285" t="s">
+        <v>594</v>
+      </c>
+      <c r="C1285" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.QUALITY_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1286" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1286" t="s">
+        <v>595</v>
+      </c>
+      <c r="C1286" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.FORMAT_QUALITY_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1287" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1287" t="s">
+        <v>596</v>
+      </c>
+      <c r="C1287" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.CONNECTION_SCORE, </v>
+      </c>
+    </row>
+    <row r="1288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1288" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1288" t="s">
+        <v>597</v>
+      </c>
+      <c r="C1288" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.CONNECTION_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1289" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1289" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1289" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.FORMAT_CONNECTION_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1290" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1290" t="s">
+        <v>599</v>
+      </c>
+      <c r="C1290" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.METADATA_SCORE, </v>
+      </c>
+    </row>
+    <row r="1291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1291" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1291" t="s">
+        <v>600</v>
+      </c>
+      <c r="C1291" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.METADATA_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1292" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1292" t="s">
+        <v>601</v>
+      </c>
+      <c r="C1292" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.FORMAT_METADATA_SCORE_PCT, </v>
+      </c>
+    </row>
+    <row r="1293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1293" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1293" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1293" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.METADATA_CONTACT, </v>
+      </c>
+    </row>
+    <row r="1294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1294" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1294" t="s">
+        <v>603</v>
+      </c>
+      <c r="C1294" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.ACCESS_WAIVER_YN, </v>
+      </c>
+    </row>
+    <row r="1295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1295" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1295" t="s">
+        <v>604</v>
+      </c>
+      <c r="C1295" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.GEO_DATA_PRES_FORM, </v>
+      </c>
+    </row>
+    <row r="1296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1296" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1296" t="s">
+        <v>605</v>
+      </c>
+      <c r="C1296" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.PUBLISHED_STATUS, </v>
+      </c>
+    </row>
+    <row r="1297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1297" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1297" t="s">
+        <v>606</v>
+      </c>
+      <c r="C1297" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.CREATE_DTM, </v>
+      </c>
+    </row>
+    <row r="1298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1298" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1298" t="s">
+        <v>607</v>
+      </c>
+      <c r="C1298" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.LAST_MOD_DTM, </v>
+      </c>
+    </row>
+    <row r="1299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1299" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1299" t="s">
+        <v>608</v>
+      </c>
+      <c r="C1299" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.INPORT_LINK_URL, </v>
+      </c>
+    </row>
+    <row r="1300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1300" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1300" t="s">
+        <v>609</v>
+      </c>
+      <c r="C1300" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.REFRESH_DTM, </v>
+      </c>
+    </row>
+    <row r="1301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1301" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1301" t="s">
+        <v>610</v>
+      </c>
+      <c r="C1301" s="18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">DS_PIR_SCOR_V.FORMAT_REFRESH_DTM, </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data model upgrade description and implemented consistent abbreviations in object names.  Updated DB and PL/SQL naming conventions
</commit_message>
<xml_diff>
--- a/docs/DB_DDL_helper_template.xlsx
+++ b/docs/DB_DDL_helper_template.xlsx
@@ -737,7 +737,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3987" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3987" uniqueCount="654">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -2697,6 +2697,9 @@
   </si>
   <si>
     <t>The Formatted Date/Time the PIR data set record was refreshed from ODS (in MM/DD/YYYY HH24:MI:SS format)</t>
+  </si>
+  <si>
+    <t>CCD_DATA_SETS_INPORT_V</t>
   </si>
 </sst>
 </file>
@@ -8584,8 +8587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2802"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A477" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D496" sqref="D496:D550"/>
+    <sheetView tabSelected="1" topLeftCell="A271" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B290" sqref="B290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15285,7 +15288,7 @@
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A496" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B496" s="18" t="s">
         <v>126</v>
@@ -15295,12 +15298,12 @@
       </c>
       <c r="D496" s="22" t="str">
         <f t="shared" ref="D496:D550" si="11">CONCATENATE("COMMENT ON COLUMN ",A496, ".", B496, " IS '", SUBSTITUTE(C496, "'", "''"), "';")</f>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_ID IS 'Primary key for the CCD_DATA_SETS table';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.DATA_SET_ID IS 'Primary key for the CCD_DATA_SETS table';</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A497" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B497" s="18" t="s">
         <v>135</v>
@@ -15310,12 +15313,12 @@
       </c>
       <c r="D497" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_NAME IS 'The Name of the data set';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.DATA_SET_NAME IS 'The Name of the data set';</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A498" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B498" s="18" t="s">
         <v>136</v>
@@ -15325,12 +15328,12 @@
       </c>
       <c r="D498" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_DESC IS 'Description for the data set';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.DATA_SET_DESC IS 'Description for the data set';</v>
       </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A499" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B499" s="18" t="s">
         <v>137</v>
@@ -15340,12 +15343,12 @@
       </c>
       <c r="D499" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_INPORT_CAT_ID IS 'InPort Catalog ID for the data set';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.DATA_SET_INPORT_CAT_ID IS 'InPort Catalog ID for the data set';</v>
       </c>
     </row>
     <row r="500" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A500" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B500" s="18" t="s">
         <v>138</v>
@@ -15355,12 +15358,12 @@
       </c>
       <c r="D500" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_INPORT_URL IS 'InPort metadata URL for the data set';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.DATA_SET_INPORT_URL IS 'InPort metadata URL for the data set';</v>
       </c>
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A501" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B501" s="18" t="s">
         <v>139</v>
@@ -15370,12 +15373,12 @@
       </c>
       <c r="D501" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_TYPE_ID IS 'Primary key for the CCD_DATA_SET_TYPES table';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.DATA_SET_TYPE_ID IS 'Primary key for the CCD_DATA_SET_TYPES table';</v>
       </c>
     </row>
     <row r="502" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A502" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B502" s="18" t="s">
         <v>140</v>
@@ -15385,12 +15388,12 @@
       </c>
       <c r="D502" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_TYPE_NAME IS 'Name for the data set type';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.DATA_SET_TYPE_NAME IS 'Name for the data set type';</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A503" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B503" s="18" t="s">
         <v>141</v>
@@ -15400,12 +15403,12 @@
       </c>
       <c r="D503" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_TYPE_DESC IS 'Description for the data set type';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.DATA_SET_TYPE_DESC IS 'Description for the data set type';</v>
       </c>
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A504" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B504" s="18" t="s">
         <v>142</v>
@@ -15415,12 +15418,12 @@
       </c>
       <c r="D504" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_TYPE_DOC_URL IS 'Documentation URL for the data type, this can be an InPort URL for the parent Project record of the individual data sets or a documentation package that provides information about this data set type';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.DATA_SET_TYPE_DOC_URL IS 'Documentation URL for the data type, this can be an InPort URL for the parent Project record of the individual data sets or a documentation package that provides information about this data set type';</v>
       </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A505" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B505" s="18" t="s">
         <v>143</v>
@@ -15430,12 +15433,12 @@
       </c>
       <c r="D505" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.DATA_SET_STATUS_ID IS 'Primary key for the CCD_DATA_SET_STATUS table';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.DATA_SET_STATUS_ID IS 'Primary key for the CCD_DATA_SET_STATUS table';</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A506" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B506" s="18" t="s">
         <v>144</v>
@@ -15445,12 +15448,12 @@
       </c>
       <c r="D506" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.STATUS_CODE IS 'The alpha-numeric code for the data status';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.STATUS_CODE IS 'The alpha-numeric code for the data status';</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A507" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B507" s="18" t="s">
         <v>145</v>
@@ -15460,12 +15463,12 @@
       </c>
       <c r="D507" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.STATUS_NAME IS 'The name of the data status';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.STATUS_NAME IS 'The name of the data status';</v>
       </c>
     </row>
     <row r="508" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A508" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B508" s="18" t="s">
         <v>146</v>
@@ -15475,12 +15478,12 @@
       </c>
       <c r="D508" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.STATUS_DESC IS 'The description for the data status';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.STATUS_DESC IS 'The description for the data status';</v>
       </c>
     </row>
     <row r="509" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A509" s="18" t="s">
-        <v>148</v>
+        <v>653</v>
       </c>
       <c r="B509" s="18" t="s">
         <v>147</v>
@@ -15490,12 +15493,12 @@
       </c>
       <c r="D509" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN CCD_DATA_SETS_V.STATUS_COLOR IS 'The hex value for the color that the data set status has in the application interface';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.STATUS_COLOR IS 'The hex value for the color that the data set status has in the application interface';</v>
       </c>
     </row>
     <row r="510" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A510" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B510" s="18" t="s">
         <v>569</v>
@@ -15505,12 +15508,12 @@
       </c>
       <c r="D510" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.METADATA_FOLDER IS 'The maximum parent InPort folder''s Title (division/program level) for the given Pacific Island Region''s data set';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.METADATA_FOLDER IS 'The maximum parent InPort folder''s Title (division/program level) for the given Pacific Island Region''s data set';</v>
       </c>
     </row>
     <row r="511" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A511" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B511" s="18" t="s">
         <v>570</v>
@@ -15520,12 +15523,12 @@
       </c>
       <c r="D511" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.ORG_ALIAS_ABBREV IS 'The organization division/program alias abbreviation defined for the given InPort Metadata Folder name';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.ORG_ALIAS_ABBREV IS 'The organization division/program alias abbreviation defined for the given InPort Metadata Folder name';</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A512" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B512" s="18" t="s">
         <v>571</v>
@@ -15535,12 +15538,12 @@
       </c>
       <c r="D512" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.LIBRARY_ORG IS 'The InPort Library Organization';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.LIBRARY_ORG IS 'The InPort Library Organization';</v>
       </c>
     </row>
     <row r="513" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A513" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B513" s="18" t="s">
         <v>573</v>
@@ -15550,12 +15553,12 @@
       </c>
       <c r="D513" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.TITLE IS 'InPort Title (NMFS_INP_CATALOG_ITEMS.TITLE)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.TITLE IS 'InPort Title (NMFS_INP_CATALOG_ITEMS.TITLE)';</v>
       </c>
     </row>
     <row r="514" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A514" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B514" s="18" t="s">
         <v>574</v>
@@ -15565,12 +15568,12 @@
       </c>
       <c r="D514" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.PARR_KEYWORDS IS 'InPort  PARR Keywords (NMFS_INP_CC_KEYWORDS.KEYWORD)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.PARR_KEYWORDS IS 'InPort  PARR Keywords (NMFS_INP_CC_KEYWORDS.KEYWORD)';</v>
       </c>
     </row>
     <row r="515" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A515" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B515" s="18" t="s">
         <v>575</v>
@@ -15580,12 +15583,12 @@
       </c>
       <c r="D515" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.COMPLETION_SCORE IS 'InPort Completion Score (NMFS_INP_RBR_DS_SCORES.COMPLETION_SCORE)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.COMPLETION_SCORE IS 'InPort Completion Score (NMFS_INP_RBR_DS_SCORES.COMPLETION_SCORE)';</v>
       </c>
     </row>
     <row r="516" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A516" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B516" s="18" t="s">
         <v>576</v>
@@ -15595,12 +15598,12 @@
       </c>
       <c r="D516" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.COMPLETION_SCORE_PCT IS 'InPort Completion Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.COMPLETION_SCORE_PCT IS 'InPort Completion Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="517" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A517" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B517" s="18" t="s">
         <v>577</v>
@@ -15610,12 +15613,12 @@
       </c>
       <c r="D517" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_COMPLETION_SCORE_PCT IS 'Formatted InPort Completion Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.FORMAT_COMPLETION_SCORE_PCT IS 'Formatted InPort Completion Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A518" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B518" s="18" t="s">
         <v>578</v>
@@ -15625,12 +15628,12 @@
       </c>
       <c r="D518" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.IDENTIFICATION_SCORE IS 'InPort Identification Score (NMFS_INP_RBR_DS_SCORES.IDENTIFICATION_SCORE)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.IDENTIFICATION_SCORE IS 'InPort Identification Score (NMFS_INP_RBR_DS_SCORES.IDENTIFICATION_SCORE)';</v>
       </c>
     </row>
     <row r="519" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A519" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B519" s="18" t="s">
         <v>579</v>
@@ -15640,12 +15643,12 @@
       </c>
       <c r="D519" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.IDENTIFICATION_SCORE_PCT IS 'InPort Identification Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.IDENTIFICATION_SCORE_PCT IS 'InPort Identification Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="520" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A520" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B520" s="18" t="s">
         <v>580</v>
@@ -15655,12 +15658,12 @@
       </c>
       <c r="D520" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_IDENTIFICATION_SCORE_PCT IS 'Formatted InPort Identification Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.FORMAT_IDENTIFICATION_SCORE_PCT IS 'Formatted InPort Identification Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="521" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A521" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B521" s="18" t="s">
         <v>581</v>
@@ -15670,12 +15673,12 @@
       </c>
       <c r="D521" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.ACCESS_SCORE IS 'InPort Access Score (NMFS_INP_RBR_DS_SCORES.ACCESS_SCORE)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.ACCESS_SCORE IS 'InPort Access Score (NMFS_INP_RBR_DS_SCORES.ACCESS_SCORE)';</v>
       </c>
     </row>
     <row r="522" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A522" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B522" s="18" t="s">
         <v>582</v>
@@ -15685,12 +15688,12 @@
       </c>
       <c r="D522" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.ACCESS_SCORE_PCT IS 'InPort Access Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.ACCESS_SCORE_PCT IS 'InPort Access Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="523" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A523" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B523" s="18" t="s">
         <v>583</v>
@@ -15700,12 +15703,12 @@
       </c>
       <c r="D523" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_ACCESS_SCORE_PCT IS 'Formatted InPort Access Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.FORMAT_ACCESS_SCORE_PCT IS 'Formatted InPort Access Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="524" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A524" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B524" s="18" t="s">
         <v>584</v>
@@ -15715,12 +15718,12 @@
       </c>
       <c r="D524" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.COVERAGE_SCORE IS 'InPort Coverage Score (NMFS_INP_RBR_DS_SCORES.COVERAGE_SCORE)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.COVERAGE_SCORE IS 'InPort Coverage Score (NMFS_INP_RBR_DS_SCORES.COVERAGE_SCORE)';</v>
       </c>
     </row>
     <row r="525" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A525" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B525" s="18" t="s">
         <v>585</v>
@@ -15730,12 +15733,12 @@
       </c>
       <c r="D525" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.COVERAGE_SCORE_PCT IS 'InPort Coverage Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.COVERAGE_SCORE_PCT IS 'InPort Coverage Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A526" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B526" s="18" t="s">
         <v>586</v>
@@ -15745,12 +15748,12 @@
       </c>
       <c r="D526" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_COVERAGE_SCORE_PCT IS 'Formatted InPort Coverage Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.FORMAT_COVERAGE_SCORE_PCT IS 'Formatted InPort Coverage Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="527" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A527" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B527" s="18" t="s">
         <v>587</v>
@@ -15760,12 +15763,12 @@
       </c>
       <c r="D527" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.CONTENT_SCORE IS 'InPort Content Score (NMFS_INP_RBR_DS_SCORES.CONTENT_SCORE)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.CONTENT_SCORE IS 'InPort Content Score (NMFS_INP_RBR_DS_SCORES.CONTENT_SCORE)';</v>
       </c>
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A528" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B528" s="18" t="s">
         <v>588</v>
@@ -15775,12 +15778,12 @@
       </c>
       <c r="D528" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.CONTENT_SCORE_PCT IS 'InPort Content Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.CONTENT_SCORE_PCT IS 'InPort Content Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A529" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B529" s="18" t="s">
         <v>589</v>
@@ -15790,12 +15793,12 @@
       </c>
       <c r="D529" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_CONTENT_SCORE_PCT IS 'Formatted InPort Content Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.FORMAT_CONTENT_SCORE_PCT IS 'Formatted InPort Content Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A530" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B530" s="18" t="s">
         <v>590</v>
@@ -15805,12 +15808,12 @@
       </c>
       <c r="D530" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.HISTORY_SCORE IS 'InPort History Score (NMFS_INP_RBR_DS_SCORES.HISTORY_SCORE)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.HISTORY_SCORE IS 'InPort History Score (NMFS_INP_RBR_DS_SCORES.HISTORY_SCORE)';</v>
       </c>
     </row>
     <row r="531" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A531" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B531" s="18" t="s">
         <v>591</v>
@@ -15820,12 +15823,12 @@
       </c>
       <c r="D531" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.HISTORY_SCORE_PCT IS 'InPort History Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.HISTORY_SCORE_PCT IS 'InPort History Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A532" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B532" s="18" t="s">
         <v>592</v>
@@ -15835,12 +15838,12 @@
       </c>
       <c r="D532" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_HISTORY_SCORE_PCT IS 'Formatted InPort History Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.FORMAT_HISTORY_SCORE_PCT IS 'Formatted InPort History Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A533" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B533" s="18" t="s">
         <v>593</v>
@@ -15850,12 +15853,12 @@
       </c>
       <c r="D533" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.QUALITY_SCORE IS 'InPort Quality Score (NMFS_INP_RBR_DS_SCORES.QUALITY_SCORE)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.QUALITY_SCORE IS 'InPort Quality Score (NMFS_INP_RBR_DS_SCORES.QUALITY_SCORE)';</v>
       </c>
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A534" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B534" s="18" t="s">
         <v>594</v>
@@ -15865,12 +15868,12 @@
       </c>
       <c r="D534" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.QUALITY_SCORE_PCT IS 'InPort Quality Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.QUALITY_SCORE_PCT IS 'InPort Quality Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A535" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B535" s="18" t="s">
         <v>595</v>
@@ -15880,12 +15883,12 @@
       </c>
       <c r="D535" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_QUALITY_SCORE_PCT IS 'Formatted InPort Quality Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.FORMAT_QUALITY_SCORE_PCT IS 'Formatted InPort Quality Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A536" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B536" s="18" t="s">
         <v>596</v>
@@ -15895,12 +15898,12 @@
       </c>
       <c r="D536" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.CONNECTION_SCORE IS 'InPort Connection Score (NMFS_INP_RBR_DS_SCORES.CONNECTION_SCORE)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.CONNECTION_SCORE IS 'InPort Connection Score (NMFS_INP_RBR_DS_SCORES.CONNECTION_SCORE)';</v>
       </c>
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A537" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B537" s="18" t="s">
         <v>597</v>
@@ -15910,12 +15913,12 @@
       </c>
       <c r="D537" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.CONNECTION_SCORE_PCT IS 'InPort Connection Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.CONNECTION_SCORE_PCT IS 'InPort Connection Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A538" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B538" s="18" t="s">
         <v>598</v>
@@ -15925,12 +15928,12 @@
       </c>
       <c r="D538" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_CONNECTION_SCORE_PCT IS 'Formatted InPort Connection Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.FORMAT_CONNECTION_SCORE_PCT IS 'Formatted InPort Connection Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A539" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B539" s="18" t="s">
         <v>599</v>
@@ -15940,12 +15943,12 @@
       </c>
       <c r="D539" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.METADATA_SCORE IS 'InPort Metadata Score (NMFS_INP_RBR_DS_SCORES.METADATA_SCORE)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.METADATA_SCORE IS 'InPort Metadata Score (NMFS_INP_RBR_DS_SCORES.METADATA_SCORE)';</v>
       </c>
     </row>
     <row r="540" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A540" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B540" s="18" t="s">
         <v>600</v>
@@ -15955,12 +15958,12 @@
       </c>
       <c r="D540" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.METADATA_SCORE_PCT IS 'InPort Metadata Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.METADATA_SCORE_PCT IS 'InPort Metadata Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="541" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A541" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B541" s="18" t="s">
         <v>601</v>
@@ -15970,12 +15973,12 @@
       </c>
       <c r="D541" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_METADATA_SCORE_PCT IS 'Formatted InPort Metadata Score Percentage (to 2 significant digits)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.FORMAT_METADATA_SCORE_PCT IS 'Formatted InPort Metadata Score Percentage (to 2 significant digits)';</v>
       </c>
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A542" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B542" s="18" t="s">
         <v>602</v>
@@ -15985,12 +15988,12 @@
       </c>
       <c r="D542" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.METADATA_CONTACT IS 'Comma-delimited list of metadata contacts for the corresponding data set';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.METADATA_CONTACT IS 'Comma-delimited list of metadata contacts for the corresponding data set';</v>
       </c>
     </row>
     <row r="543" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A543" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B543" s="18" t="s">
         <v>603</v>
@@ -16000,12 +16003,12 @@
       </c>
       <c r="D543" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.ACCESS_WAIVER_YN IS 'Access Waiver? (NMFS_INP_CC_DATA_MANAGEMENT.ACCESS_WAIVER_YN)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.ACCESS_WAIVER_YN IS 'Access Waiver? (NMFS_INP_CC_DATA_MANAGEMENT.ACCESS_WAIVER_YN)';</v>
       </c>
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A544" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B544" s="18" t="s">
         <v>604</v>
@@ -16015,12 +16018,12 @@
       </c>
       <c r="D544" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.GEO_DATA_PRES_FORM IS 'Geo Data Presentation Format (NMFS_INP_CATALOG_ITEMS.DS_GEO_DATA_PRES_FORM)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.GEO_DATA_PRES_FORM IS 'Geo Data Presentation Format (NMFS_INP_CATALOG_ITEMS.DS_GEO_DATA_PRES_FORM)';</v>
       </c>
     </row>
     <row r="545" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A545" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B545" s="18" t="s">
         <v>605</v>
@@ -16030,12 +16033,12 @@
       </c>
       <c r="D545" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.PUBLISHED_STATUS IS 'Published Status (NMFS_INP_CATALOG_ITEMS.PUBLISHED_STATUS)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.PUBLISHED_STATUS IS 'Published Status (NMFS_INP_CATALOG_ITEMS.PUBLISHED_STATUS)';</v>
       </c>
     </row>
     <row r="546" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A546" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B546" s="18" t="s">
         <v>606</v>
@@ -16045,12 +16048,12 @@
       </c>
       <c r="D546" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.CREATE_DTM IS 'Create Date/Time (NMFS_INP_CATALOG_ITEMS.CREATE_DTM)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.CREATE_DTM IS 'Create Date/Time (NMFS_INP_CATALOG_ITEMS.CREATE_DTM)';</v>
       </c>
     </row>
     <row r="547" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A547" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B547" s="18" t="s">
         <v>607</v>
@@ -16060,12 +16063,12 @@
       </c>
       <c r="D547" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.LAST_MOD_DTM IS 'Modified Date/Time (NMFS_INP_CATALOG_ITEMS.LAST_MOD_DTM)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.LAST_MOD_DTM IS 'Modified Date/Time (NMFS_INP_CATALOG_ITEMS.LAST_MOD_DTM)';</v>
       </c>
     </row>
     <row r="548" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A548" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B548" s="18" t="s">
         <v>608</v>
@@ -16075,12 +16078,12 @@
       </c>
       <c r="D548" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.INPORT_LINK_URL IS 'Generated standard InPort data set URL based on the corresponding CAT_ID';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.INPORT_LINK_URL IS 'Generated standard InPort data set URL based on the corresponding CAT_ID';</v>
       </c>
     </row>
     <row r="549" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A549" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B549" s="18" t="s">
         <v>609</v>
@@ -16090,12 +16093,12 @@
       </c>
       <c r="D549" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.REFRESH_DTM IS 'The Date/Time the PIR data set record was refreshed from ODS';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.REFRESH_DTM IS 'The Date/Time the PIR data set record was refreshed from ODS';</v>
       </c>
     </row>
     <row r="550" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A550" s="18" t="s">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="B550" s="18" t="s">
         <v>610</v>
@@ -16105,7 +16108,7 @@
       </c>
       <c r="D550" s="22" t="str">
         <f t="shared" si="11"/>
-        <v>COMMENT ON COLUMN DS_PIR_SCOR_V.FORMAT_REFRESH_DTM IS 'The Formatted Date/Time the PIR data set record was refreshed from ODS (in MM/DD/YYYY HH24:MI:SS format)';</v>
+        <v>COMMENT ON COLUMN CCD_DATA_SETS_INPORT_V.FORMAT_REFRESH_DTM IS 'The Formatted Date/Time the PIR data set record was refreshed from ODS (in MM/DD/YYYY HH24:MI:SS format)';</v>
       </c>
     </row>
     <row r="551" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -18878,7 +18881,7 @@
   <dimension ref="A1:C1301"/>
   <sheetViews>
     <sheetView topLeftCell="A1263" workbookViewId="0">
-      <selection activeCell="A1246" sqref="A1246:B1301"/>
+      <selection activeCell="C1260" sqref="C1260:C1301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>